<commit_message>
creation of test cases for administrative functions
</commit_message>
<xml_diff>
--- a/testing/Team eXi Test Cases.xlsx
+++ b/testing/Team eXi Test Cases.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>S/N</t>
   </si>
@@ -178,6 +178,56 @@
   </si>
   <si>
     <t>Information to be displayed exactly the same as what was entered</t>
+  </si>
+  <si>
+    <t>Management of User Accounts</t>
+  </si>
+  <si>
+    <t>Verify that if the user is logged in as an admin user, the user would be able to create new accounts for access into system for tutors</t>
+  </si>
+  <si>
+    <t>Tutor Name: Amy Tan
+Academic Level: P6
+Subject: Maths
+Class: G1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login as an admin user and navigate to the Tutor Account Creation Page. Input the details into the corresponding field </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login as an admin user and navigate to the Tutor Account Creation Page. Input the details into the corresponding field and click Create Tutor </t>
+  </si>
+  <si>
+    <t>Tutor Creation Successful</t>
+  </si>
+  <si>
+    <t>Verify that the user would not be able to create tutor accounts if the mandatory fields are missing</t>
+  </si>
+  <si>
+    <t>Tutor Name: Amy Tan
+Academic Level: P6
+Subject: Maths
+Class: G1
+ID: amytan86</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tutor Name: Amy Tan
+Academic Level: P6
+Subject: Maths
+Class: G1
+ID: </t>
+  </si>
+  <si>
+    <t>Error Message prompting user to key in all mandatory fields would be displayed</t>
+  </si>
+  <si>
+    <t>Verify that if the user is logged in as an admin user, the user would be able to remove tutor accounts when the need arises</t>
+  </si>
+  <si>
+    <t>Login as an admin user and navigate to the List of Tutor Pages. Input the details into the corresponding field and click Create Tutor Select the tutor Amy Tan and press Delete</t>
+  </si>
+  <si>
+    <t>The tutor should be removed from the database</t>
   </si>
 </sst>
 </file>
@@ -384,161 +434,193 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799980"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599990"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399980"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799980"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599990"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399980"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799980"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599990"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399980"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799980"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599990"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399980"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799980"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599990"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399980"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799980"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599990"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399980"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -548,9 +630,7 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -565,9 +645,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -582,9 +660,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -597,9 +673,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -614,33 +688,25 @@
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <bottom style="thick">
         <color theme="4"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <bottom style="thick">
         <color rgb="FFACCCEA"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <bottom style="medium">
         <color theme="4" tint="0.399980"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -655,9 +721,7 @@
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -672,9 +736,7 @@
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <left style="double">
@@ -689,17 +751,13 @@
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <top style="thin">
@@ -708,9 +766,7 @@
       <bottom style="double">
         <color theme="4"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -725,9 +781,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -738,9 +792,7 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -753,9 +805,7 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
@@ -809,7 +859,7 @@
     <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -926,6 +976,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1304,8 +1360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView topLeftCell="A19" tabSelected="1" zoomScale="180" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.500000"/>
@@ -1372,7 +1428,7 @@
       <c r="C2" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="43" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="25" t="s">
@@ -1394,7 +1450,7 @@
       <c r="C3" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="43" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="25" t="s">
@@ -1416,7 +1472,7 @@
       <c r="C4" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="43" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="25" t="s">
@@ -1438,7 +1494,7 @@
       <c r="C5" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="43" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="25" t="s">
@@ -1460,7 +1516,7 @@
       <c r="C6" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="43" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="25" t="s">
@@ -1482,7 +1538,7 @@
       <c r="C7" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="43" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="25" t="s">
@@ -1504,7 +1560,7 @@
       <c r="C8" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="D8" s="44" t="s">
         <v>13</v>
       </c>
       <c r="E8" s="38" t="s">
@@ -1548,7 +1604,7 @@
       <c r="C10" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="38" t="s">
+      <c r="D10" s="44" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="34" t="s">
@@ -1570,7 +1626,7 @@
       <c r="C11" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="39" t="s">
+      <c r="D11" s="34" t="s">
         <v>13</v>
       </c>
       <c r="E11" s="34" t="s">
@@ -1592,7 +1648,7 @@
       <c r="C12" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="39" t="s">
+      <c r="D12" s="34" t="s">
         <v>13</v>
       </c>
       <c r="E12" s="34" t="s">
@@ -1614,7 +1670,7 @@
       <c r="C13" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="39" t="s">
+      <c r="D13" s="34" t="s">
         <v>39</v>
       </c>
       <c r="E13" s="34" t="s">
@@ -1636,7 +1692,7 @@
       <c r="C14" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="39" t="s">
+      <c r="D14" s="34" t="s">
         <v>43</v>
       </c>
       <c r="E14" s="34" t="s">
@@ -1658,7 +1714,7 @@
       <c r="C15" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="39" t="s">
+      <c r="D15" s="34" t="s">
         <v>46</v>
       </c>
       <c r="E15" s="34" t="s">
@@ -1692,39 +1748,69 @@
       <c r="G16" s="34"/>
       <c r="H16" s="34"/>
     </row>
-    <row r="17" spans="1:8" ht="16.500000">
+    <row r="17" spans="1:8" ht="115.000000">
       <c r="A17" s="34">
         <v>16</v>
       </c>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
+      <c r="B17" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="34" t="s">
+        <v>57</v>
+      </c>
       <c r="G17" s="34"/>
       <c r="H17" s="34"/>
     </row>
-    <row r="18" spans="1:8" ht="16.500000">
+    <row r="18" spans="1:8" ht="115.000000">
       <c r="A18" s="34">
         <v>17</v>
       </c>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
+      <c r="B18" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18" s="34" t="s">
+        <v>61</v>
+      </c>
       <c r="G18" s="34"/>
       <c r="H18" s="34"/>
     </row>
-    <row r="19" spans="1:8" ht="16.500000">
+    <row r="19" spans="1:8" ht="131.350000">
       <c r="A19" s="34">
         <v>18</v>
       </c>
-      <c r="B19" s="42"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
+      <c r="B19" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" s="34" t="s">
+        <v>64</v>
+      </c>
       <c r="G19" s="40"/>
       <c r="H19" s="40"/>
     </row>
@@ -1968,7 +2054,6 @@
       <c r="G39" s="40"/>
       <c r="H39" s="40"/>
     </row>
-    <row r="40" spans="1:8"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="H1">

</xml_diff>

<commit_message>
creation of test cases for Student Management
</commit_message>
<xml_diff>
--- a/testing/Team eXi Test Cases.xlsx
+++ b/testing/Team eXi Test Cases.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
     <t>S/N</t>
   </si>
@@ -228,6 +228,145 @@
   </si>
   <si>
     <t>The tutor should be removed from the database</t>
+  </si>
+  <si>
+    <t>Sign Ups</t>
+  </si>
+  <si>
+    <t>Verify that when all the neccessary information are filled in, the admin user would be able to successfully create the Student record in the database</t>
+  </si>
+  <si>
+    <t>Name: Jenny Kim
+Age: 14
+Gender: F
+Phone: 91978630
+Address: Bukit Panjang Ring Rd
+Subjects: Maths, Science</t>
+  </si>
+  <si>
+    <t>Name: Jenny Kim
+Age: 14
+Gender: F
+Phone: 91978630
+Address: Bukit Panjang Ring Rd
+Subjects: Maths, Science
+Required Amt: $320</t>
+  </si>
+  <si>
+    <t>Name: Jenny Kim
+Age: 14
+Gender: F
+Phone: 91978630
+Address: Bukit Panjang Ring Rd
+Subjects: Maths, Science
+Required Amt: $320
+Outstanding Amt: $0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login as an admin user and navigate to the Sign Ups Page. Input the </t>
+  </si>
+  <si>
+    <t>Login as an admin user and navigate to the List of Tutor Page. Input the details into the corresponding field and click Create Tutor Select the tutor Amy Tan and press Delete</t>
+  </si>
+  <si>
+    <t>Login as an admin user and navigate to the Sign Ups Page. Input the information as specified into the corresponding fields and click Sign Up</t>
+  </si>
+  <si>
+    <t>Student Creation Successful</t>
+  </si>
+  <si>
+    <t>Name: Jenny Kim
+ID: T0018765H
+Age: 14
+Gender: F
+Phone: 91978630
+Address: Bukit Panjang Ring Rd
+Subjects: Maths, Science
+Required Amt: $320
+Outstanding Amt: $0</t>
+  </si>
+  <si>
+    <t>Verify that when mandatory fields are empty, the admin user would not be able to successfully create the Student record in the database</t>
+  </si>
+  <si>
+    <t>Name: Jenny Kim
+ID: 
+Age: 14
+Gender: F
+Phone: 91978630
+Address: Bukit Panjang Ring Rd
+Subjects: Maths, Science
+Required Amt: $320
+Outstanding Amt: $0</t>
+  </si>
+  <si>
+    <t>Error Message regarding Student Creation Failure to be displayed</t>
+  </si>
+  <si>
+    <t>Verify that when there is a duplicate of student, the admin user would not be able to overwrite the existing record in the database</t>
+  </si>
+  <si>
+    <t>Error Message prompting that there was already a record of the specified student</t>
+  </si>
+  <si>
+    <t>Updating of Student Details</t>
+  </si>
+  <si>
+    <t>Verify that if the user is logged in as an admin user, he would be able to modify the records of a specified tutor</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Login as an admin user and navigate to the Students Records Page. Select the student Jenny Kim and edit her phone number before clicking Update</t>
+  </si>
+  <si>
+    <t>Update Successful</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that if the user is logged in as an admin user, he would be able to modify the records of a specified tutornew </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that if the new phone number entered does not satisfy the requirements of 8 digits, the update would not be successful </t>
+  </si>
+  <si>
+    <t>Phone No. : 8333999</t>
+  </si>
+  <si>
+    <t>Login as an admin user and navigate to the Students Records Page. Select the student Jenny Kim and edit her phone number as specified before clicking Update</t>
+  </si>
+  <si>
+    <t>Update Unsuccessful</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that if the new  phone number entered does not satisfy the requirements of 8 digits, the update would not be successful </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that if the new  ID entered does not satisfy the requirements of 8 digits, the update would not be successful </t>
+  </si>
+  <si>
+    <t>ID : T833399</t>
+  </si>
+  <si>
+    <t>Login as an admin user and navigate to the Students Records Page. Select the student Jenny Kim and edit her ID as specified before clicking Update</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that if the new  subjects entered does not satisfy the requirements of 8 digits, the update would not be successful </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that if the new  ID entered does not satisfy the format requirements, the update would not be successful </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that if the new  subjects entered is not being offered by the tuition centre, the update would not be successful </t>
+  </si>
+  <si>
+    <t>Subjects : Chinese</t>
+  </si>
+  <si>
+    <t>Login as an admin user and navigate to the Students Records Page. Select the student Jenny Kim and edit her subjects taken as specified before clicking Update</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that if the new  outstanding amount entered is not postive, the update would not be successful </t>
   </si>
 </sst>
 </file>
@@ -859,7 +998,7 @@
     <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -982,6 +1121,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1360,15 +1505,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z40"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" tabSelected="1" zoomScale="180" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView topLeftCell="A24" tabSelected="1" zoomScale="180" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27:F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.500000"/>
   <cols>
     <col min="2" max="2" width="26.62999916" customWidth="1" outlineLevel="0"/>
     <col min="3" max="3" width="30.00499916" customWidth="1" outlineLevel="0"/>
-    <col min="4" max="4" width="21.50499916" customWidth="1" outlineLevel="0"/>
+    <col min="4" max="4" width="29.12999916" customWidth="1" outlineLevel="0"/>
     <col min="5" max="5" width="19.50499916" customWidth="1" outlineLevel="0"/>
     <col min="6" max="6" width="16.38000011" customWidth="1" outlineLevel="0"/>
     <col min="7" max="7" width="13.25500011" customWidth="1" outlineLevel="0"/>
@@ -1806,7 +1951,7 @@
         <v>25</v>
       </c>
       <c r="E19" s="34" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="F19" s="34" t="s">
         <v>64</v>
@@ -1814,245 +1959,315 @@
       <c r="G19" s="40"/>
       <c r="H19" s="40"/>
     </row>
-    <row r="20" spans="1:8" ht="16.500000">
+    <row r="20" spans="1:8" ht="147.700000">
       <c r="A20" s="34">
         <v>19</v>
       </c>
-      <c r="B20" s="42"/>
-      <c r="C20" s="42"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="42"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="40"/>
-    </row>
-    <row r="21" spans="1:8" ht="16.500000">
+      <c r="B20" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="F20" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+    </row>
+    <row r="21" spans="1:8" ht="147.700000">
       <c r="A21" s="34">
         <v>20</v>
       </c>
-      <c r="B21" s="42"/>
-      <c r="C21" s="42"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="40"/>
-      <c r="H21" s="40"/>
-    </row>
-    <row r="22" spans="1:8" ht="16.500000">
+      <c r="B21" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+    </row>
+    <row r="22" spans="1:8" ht="147.700000">
       <c r="A22" s="34">
         <v>21</v>
       </c>
-      <c r="B22" s="42"/>
-      <c r="C22" s="42"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="40"/>
-    </row>
-    <row r="23" spans="1:8" ht="16.500000">
+      <c r="B22" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="D22" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="F22" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
+    </row>
+    <row r="23" spans="1:8" ht="115.000000">
       <c r="A23" s="34">
         <v>22</v>
       </c>
-      <c r="B23" s="42"/>
-      <c r="C23" s="42"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="42"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="40"/>
-    </row>
-    <row r="24" spans="1:8" ht="16.500000">
+      <c r="B23" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="E23" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="F23" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="G23" s="34"/>
+      <c r="H23" s="34"/>
+    </row>
+    <row r="24" spans="1:8" ht="115.000000">
       <c r="A24" s="34">
         <v>23</v>
       </c>
-      <c r="B24" s="42"/>
-      <c r="C24" s="42"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-    </row>
-    <row r="25" spans="1:8" ht="16.500000">
+      <c r="B24" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="E24" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="F24" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+    </row>
+    <row r="25" spans="1:8" ht="115.000000">
       <c r="A25" s="34">
         <v>24</v>
       </c>
-      <c r="B25" s="42"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
-      <c r="F25" s="42"/>
-      <c r="G25" s="40"/>
-      <c r="H25" s="40"/>
-    </row>
-    <row r="26" spans="1:8" ht="16.500000">
+      <c r="B25" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="D25" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="E25" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="F25" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
+    </row>
+    <row r="26" spans="1:8" ht="115.000000">
       <c r="A26" s="34">
         <v>25</v>
       </c>
-      <c r="B26" s="42"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="40"/>
-      <c r="H26" s="40"/>
+      <c r="B26" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="E26" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="F26" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="G26" s="34"/>
+      <c r="H26" s="34"/>
     </row>
     <row r="27" spans="1:8" ht="16.500000">
       <c r="A27" s="34">
         <v>26</v>
       </c>
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="40"/>
-      <c r="H27" s="40"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="34"/>
     </row>
     <row r="28" spans="1:8" ht="16.500000">
       <c r="A28" s="34">
         <v>27</v>
       </c>
-      <c r="B28" s="42"/>
-      <c r="C28" s="42"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="42"/>
-      <c r="G28" s="40"/>
-      <c r="H28" s="40"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="34"/>
     </row>
     <row r="29" spans="1:8" ht="16.500000">
       <c r="A29" s="34">
         <v>28</v>
       </c>
-      <c r="B29" s="42"/>
-      <c r="C29" s="42"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="42"/>
-      <c r="F29" s="42"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="34"/>
     </row>
     <row r="30" spans="1:8" ht="16.500000">
       <c r="A30" s="34">
         <v>29</v>
       </c>
-      <c r="B30" s="42"/>
-      <c r="C30" s="42"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="34"/>
+      <c r="H30" s="34"/>
     </row>
     <row r="31" spans="1:8" ht="16.500000">
       <c r="A31" s="34">
         <v>30</v>
       </c>
-      <c r="B31" s="42"/>
-      <c r="C31" s="42"/>
-      <c r="D31" s="42"/>
-      <c r="E31" s="42"/>
-      <c r="F31" s="42"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="34"/>
+      <c r="H31" s="34"/>
     </row>
     <row r="32" spans="1:8" ht="16.500000">
       <c r="A32" s="34">
         <v>31</v>
       </c>
-      <c r="B32" s="42"/>
-      <c r="C32" s="42"/>
-      <c r="D32" s="42"/>
-      <c r="E32" s="42"/>
-      <c r="F32" s="42"/>
-      <c r="G32" s="40"/>
-      <c r="H32" s="40"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="34"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="34"/>
+      <c r="G32" s="34"/>
+      <c r="H32" s="34"/>
     </row>
     <row r="33" spans="1:8" ht="16.500000">
       <c r="A33" s="34">
         <v>32</v>
       </c>
-      <c r="B33" s="42"/>
-      <c r="C33" s="42"/>
-      <c r="D33" s="42"/>
-      <c r="E33" s="42"/>
-      <c r="F33" s="42"/>
-      <c r="G33" s="40"/>
-      <c r="H33" s="40"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="34"/>
     </row>
     <row r="34" spans="1:8" ht="16.500000">
       <c r="A34" s="34">
         <v>33</v>
       </c>
-      <c r="B34" s="42"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="42"/>
-      <c r="E34" s="42"/>
-      <c r="F34" s="42"/>
-      <c r="G34" s="40"/>
-      <c r="H34" s="40"/>
+      <c r="B34" s="34"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="34"/>
+      <c r="H34" s="34"/>
     </row>
     <row r="35" spans="1:8" ht="16.500000">
       <c r="A35" s="34">
         <v>34</v>
       </c>
-      <c r="B35" s="42"/>
-      <c r="C35" s="42"/>
-      <c r="D35" s="42"/>
-      <c r="E35" s="42"/>
-      <c r="F35" s="42"/>
-      <c r="G35" s="40"/>
-      <c r="H35" s="40"/>
+      <c r="B35" s="34"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="34"/>
+      <c r="G35" s="34"/>
+      <c r="H35" s="34"/>
     </row>
     <row r="36" spans="1:8" ht="16.500000">
       <c r="A36" s="34">
         <v>35</v>
       </c>
-      <c r="B36" s="42"/>
-      <c r="C36" s="42"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="42"/>
-      <c r="F36" s="42"/>
-      <c r="G36" s="40"/>
-      <c r="H36" s="40"/>
+      <c r="B36" s="34"/>
+      <c r="C36" s="34"/>
+      <c r="D36" s="34"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
+      <c r="G36" s="34"/>
+      <c r="H36" s="34"/>
     </row>
     <row r="37" spans="1:8" ht="16.500000">
       <c r="A37" s="34">
         <v>36</v>
       </c>
-      <c r="B37" s="42"/>
-      <c r="C37" s="42"/>
-      <c r="D37" s="42"/>
-      <c r="E37" s="42"/>
-      <c r="F37" s="42"/>
-      <c r="G37" s="40"/>
-      <c r="H37" s="40"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="34"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
+      <c r="G37" s="34"/>
+      <c r="H37" s="34"/>
     </row>
     <row r="38" spans="1:8" ht="16.500000">
       <c r="A38" s="34">
         <v>37</v>
       </c>
-      <c r="B38" s="42"/>
-      <c r="C38" s="42"/>
-      <c r="D38" s="42"/>
-      <c r="E38" s="42"/>
-      <c r="F38" s="42"/>
-      <c r="G38" s="40"/>
-      <c r="H38" s="40"/>
+      <c r="B38" s="34"/>
+      <c r="C38" s="34"/>
+      <c r="D38" s="34"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="34"/>
+      <c r="G38" s="34"/>
+      <c r="H38" s="34"/>
     </row>
     <row r="39" spans="1:8" ht="16.500000">
       <c r="A39" s="34">
         <v>38</v>
       </c>
-      <c r="B39" s="42"/>
-      <c r="C39" s="42"/>
-      <c r="D39" s="42"/>
-      <c r="E39" s="42"/>
-      <c r="F39" s="42"/>
-      <c r="G39" s="40"/>
-      <c r="H39" s="40"/>
+      <c r="B39" s="34"/>
+      <c r="C39" s="34"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="34"/>
+      <c r="G39" s="34"/>
+      <c r="H39" s="34"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
testing for login functionality on app
</commit_message>
<xml_diff>
--- a/testing/Team eXi Test Cases.xlsx
+++ b/testing/Team eXi Test Cases.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
   <si>
     <t>S/N</t>
   </si>
@@ -368,13 +368,71 @@
   <si>
     <t xml:space="preserve">Verify that if the new  outstanding amount entered is not postive, the update would not be successful </t>
   </si>
+  <si>
+    <t>Login (App)</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Email: admin
+Pwd: adminadmin</t>
+  </si>
+  <si>
+    <t>Input username into email field and password into password field before clicking login</t>
+  </si>
+  <si>
+    <t>Email: jerald@steppingstones.com.sg</t>
+  </si>
+  <si>
+    <t>Email: jerald@steppingstones.com.sg
+Pwd: jerald86</t>
+  </si>
+  <si>
+    <t>Input email into email field and password into password field before clicking login</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Error Message Username does not exist</t>
+  </si>
+  <si>
+    <t>Email: admin
+Pwd: adminadmin!</t>
+  </si>
+  <si>
+    <t>Login Error (Wrong Password)</t>
+  </si>
+  <si>
+    <t>Email: jerald@steppingstones.com.sg
+Pwd: jerald</t>
+  </si>
+  <si>
+    <t>Verify that upon successful login of the account, the user would be brought to the dashboard view</t>
+  </si>
+  <si>
+    <t>Dashboard to be shown</t>
+  </si>
+  <si>
+    <t>Dashboard Controller is shown</t>
+  </si>
+  <si>
+    <t>Error Login (Username does not exist)</t>
+  </si>
+  <si>
+    <t>Pass/Fail (Before Debugging)</t>
+  </si>
+  <si>
+    <t>Pass/Fail after debugging</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="30">
+  <fonts count="33">
     <font>
       <sz val="11.0"/>
       <name val="Calibri"/>
@@ -560,6 +618,25 @@
       <name val="Arial"/>
       <color theme="0"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color theme="10"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10.0"/>
+      <name val="Arial"/>
+      <color rgb="FFFFFFFF"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <name val="Arial"/>
+      <color theme="0"/>
+    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -763,13 +840,15 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <left style="thin">
@@ -784,7 +863,9 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <left style="medium">
@@ -799,7 +880,9 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <left style="thin">
@@ -812,7 +895,9 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <left style="thin">
@@ -827,25 +912,33 @@
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <bottom style="thick">
         <color theme="4"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <bottom style="thick">
         <color rgb="FFACCCEA"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <bottom style="medium">
         <color theme="4" tint="0.399980"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <left style="thin">
@@ -860,7 +953,9 @@
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <left style="thin">
@@ -875,7 +970,9 @@
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <left style="double">
@@ -890,13 +987,17 @@
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <top style="thin">
@@ -905,7 +1006,9 @@
       <bottom style="double">
         <color theme="4"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <left style="thin">
@@ -920,7 +1023,9 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <left style="thin">
@@ -931,7 +1036,9 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <left style="thin">
@@ -944,7 +1051,24 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
   </borders>
   <cellStyleXfs count="49">
@@ -998,7 +1122,7 @@
     <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1127,6 +1251,50 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="33" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="33" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="33" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1503,10 +1671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z40"/>
+  <dimension ref="A1:Z39"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" tabSelected="1" zoomScale="180" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:F27"/>
+    <sheetView topLeftCell="A28" tabSelected="1" zoomScale="180" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.500000"/>
@@ -1518,6 +1686,7 @@
     <col min="6" max="6" width="16.38000011" customWidth="1" outlineLevel="0"/>
     <col min="7" max="7" width="13.25500011" customWidth="1" outlineLevel="0"/>
     <col min="8" max="8" width="10.00500011" customWidth="1" outlineLevel="0"/>
+    <col min="9" max="9" width="23.62999916" customWidth="1" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="15" customFormat="1" ht="21.000000" customHeight="1">
@@ -1544,6 +1713,9 @@
       </c>
       <c r="H1" s="22" t="s">
         <v>6</v>
+      </c>
+      <c r="I1" s="62" t="s">
+        <v>117</v>
       </c>
       <c r="J1" s="19"/>
       <c r="K1" s="19"/>
@@ -1584,6 +1756,7 @@
       </c>
       <c r="G2" s="25"/>
       <c r="H2" s="25"/>
+      <c r="I2" s="60"/>
     </row>
     <row r="3" spans="1:26" ht="65.950000">
       <c r="A3" s="24">
@@ -1605,7 +1778,8 @@
         <v>12</v>
       </c>
       <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="40"/>
     </row>
     <row r="4" spans="1:26" ht="65.950000">
       <c r="A4" s="24">
@@ -1627,7 +1801,8 @@
         <v>15</v>
       </c>
       <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
+      <c r="H4" s="57"/>
+      <c r="I4" s="40"/>
     </row>
     <row r="5" spans="1:26" ht="65.950000">
       <c r="A5" s="24">
@@ -1649,7 +1824,8 @@
         <v>15</v>
       </c>
       <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="40"/>
     </row>
     <row r="6" spans="1:26" ht="65.950000">
       <c r="A6" s="24">
@@ -1671,7 +1847,8 @@
         <v>15</v>
       </c>
       <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="40"/>
     </row>
     <row r="7" spans="1:26" ht="65.950000">
       <c r="A7" s="24">
@@ -1693,7 +1870,8 @@
         <v>20</v>
       </c>
       <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="40"/>
     </row>
     <row r="8" spans="1:26" ht="65.950000">
       <c r="A8" s="35">
@@ -1716,6 +1894,7 @@
       </c>
       <c r="G8" s="36"/>
       <c r="H8" s="36"/>
+      <c r="I8" s="40"/>
     </row>
     <row r="9" spans="1:26" ht="49.600000">
       <c r="A9" s="34">
@@ -1738,6 +1917,7 @@
       </c>
       <c r="G9" s="34"/>
       <c r="H9" s="34"/>
+      <c r="I9" s="40"/>
     </row>
     <row r="10" spans="1:26" ht="147.700000">
       <c r="A10" s="34">
@@ -1760,6 +1940,7 @@
       </c>
       <c r="G10" s="34"/>
       <c r="H10" s="34"/>
+      <c r="I10" s="40"/>
     </row>
     <row r="11" spans="1:26" ht="131.350000">
       <c r="A11" s="34">
@@ -1782,6 +1963,7 @@
       </c>
       <c r="G11" s="34"/>
       <c r="H11" s="34"/>
+      <c r="I11" s="40"/>
     </row>
     <row r="12" spans="1:26" ht="131.350000">
       <c r="A12" s="34">
@@ -1804,6 +1986,7 @@
       </c>
       <c r="G12" s="34"/>
       <c r="H12" s="34"/>
+      <c r="I12" s="40"/>
     </row>
     <row r="13" spans="1:26" ht="65.950000">
       <c r="A13" s="34">
@@ -1826,6 +2009,7 @@
       </c>
       <c r="G13" s="34"/>
       <c r="H13" s="34"/>
+      <c r="I13" s="40"/>
     </row>
     <row r="14" spans="1:26" ht="65.950000">
       <c r="A14" s="34">
@@ -1848,6 +2032,7 @@
       </c>
       <c r="G14" s="34"/>
       <c r="H14" s="34"/>
+      <c r="I14" s="40"/>
     </row>
     <row r="15" spans="1:26" ht="65.950000">
       <c r="A15" s="34">
@@ -1870,6 +2055,7 @@
       </c>
       <c r="G15" s="34"/>
       <c r="H15" s="34"/>
+      <c r="I15" s="40"/>
     </row>
     <row r="16" spans="1:26" ht="65.950000">
       <c r="A16" s="34">
@@ -1892,8 +2078,9 @@
       </c>
       <c r="G16" s="34"/>
       <c r="H16" s="34"/>
-    </row>
-    <row r="17" spans="1:8" ht="115.000000">
+      <c r="I16" s="40"/>
+    </row>
+    <row r="17" spans="1:9" ht="115.000000">
       <c r="A17" s="34">
         <v>16</v>
       </c>
@@ -1914,8 +2101,9 @@
       </c>
       <c r="G17" s="34"/>
       <c r="H17" s="34"/>
-    </row>
-    <row r="18" spans="1:8" ht="115.000000">
+      <c r="I17" s="40"/>
+    </row>
+    <row r="18" spans="1:9" ht="115.000000">
       <c r="A18" s="34">
         <v>17</v>
       </c>
@@ -1936,8 +2124,9 @@
       </c>
       <c r="G18" s="34"/>
       <c r="H18" s="34"/>
-    </row>
-    <row r="19" spans="1:8" ht="131.350000">
+      <c r="I18" s="40"/>
+    </row>
+    <row r="19" spans="1:9" ht="131.350000">
       <c r="A19" s="34">
         <v>18</v>
       </c>
@@ -1958,8 +2147,9 @@
       </c>
       <c r="G19" s="40"/>
       <c r="H19" s="40"/>
-    </row>
-    <row r="20" spans="1:8" ht="147.700000">
+      <c r="I19" s="40"/>
+    </row>
+    <row r="20" spans="1:9" ht="147.700000">
       <c r="A20" s="34">
         <v>19</v>
       </c>
@@ -1980,8 +2170,9 @@
       </c>
       <c r="G20" s="34"/>
       <c r="H20" s="34"/>
-    </row>
-    <row r="21" spans="1:8" ht="147.700000">
+      <c r="I20" s="40"/>
+    </row>
+    <row r="21" spans="1:9" ht="147.700000">
       <c r="A21" s="34">
         <v>20</v>
       </c>
@@ -2002,8 +2193,9 @@
       </c>
       <c r="G21" s="34"/>
       <c r="H21" s="34"/>
-    </row>
-    <row r="22" spans="1:8" ht="147.700000">
+      <c r="I21" s="40"/>
+    </row>
+    <row r="22" spans="1:9" ht="147.700000">
       <c r="A22" s="34">
         <v>21</v>
       </c>
@@ -2024,8 +2216,9 @@
       </c>
       <c r="G22" s="34"/>
       <c r="H22" s="34"/>
-    </row>
-    <row r="23" spans="1:8" ht="115.000000">
+      <c r="I22" s="40"/>
+    </row>
+    <row r="23" spans="1:9" ht="115.000000">
       <c r="A23" s="34">
         <v>22</v>
       </c>
@@ -2046,8 +2239,9 @@
       </c>
       <c r="G23" s="34"/>
       <c r="H23" s="34"/>
-    </row>
-    <row r="24" spans="1:8" ht="115.000000">
+      <c r="I23" s="40"/>
+    </row>
+    <row r="24" spans="1:9" ht="115.000000">
       <c r="A24" s="34">
         <v>23</v>
       </c>
@@ -2068,8 +2262,9 @@
       </c>
       <c r="G24" s="34"/>
       <c r="H24" s="34"/>
-    </row>
-    <row r="25" spans="1:8" ht="115.000000">
+      <c r="I24" s="40"/>
+    </row>
+    <row r="25" spans="1:9" ht="115.000000">
       <c r="A25" s="34">
         <v>24</v>
       </c>
@@ -2090,8 +2285,9 @@
       </c>
       <c r="G25" s="34"/>
       <c r="H25" s="34"/>
-    </row>
-    <row r="26" spans="1:8" ht="115.000000">
+      <c r="I25" s="40"/>
+    </row>
+    <row r="26" spans="1:9" ht="115.000000">
       <c r="A26" s="34">
         <v>25</v>
       </c>
@@ -2112,92 +2308,170 @@
       </c>
       <c r="G26" s="34"/>
       <c r="H26" s="34"/>
-    </row>
-    <row r="27" spans="1:8" ht="16.500000">
+      <c r="I26" s="40"/>
+    </row>
+    <row r="27" spans="1:9" ht="65.950000">
       <c r="A27" s="34">
         <v>26</v>
       </c>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
-    </row>
-    <row r="28" spans="1:8" ht="16.500000">
+      <c r="B27" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="C27" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="43" t="s">
+        <v>102</v>
+      </c>
+      <c r="E27" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="F27" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="I27" s="40"/>
+    </row>
+    <row r="28" spans="1:9" ht="65.950000">
       <c r="A28" s="34">
         <v>27</v>
       </c>
-      <c r="B28" s="34"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
-    </row>
-    <row r="29" spans="1:8" ht="16.500000">
+      <c r="B28" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="C28" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="53" t="s">
+        <v>105</v>
+      </c>
+      <c r="E28" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="F28" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="H28" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="I28" s="40"/>
+    </row>
+    <row r="29" spans="1:9" ht="65.950000">
       <c r="A29" s="34">
         <v>28</v>
       </c>
-      <c r="B29" s="34"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="34"/>
-      <c r="G29" s="34"/>
-      <c r="H29" s="34"/>
-    </row>
-    <row r="30" spans="1:8" ht="16.500000">
+      <c r="B29" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="C29" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="E29" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="F29" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="G29" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="H29" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="I29" s="40"/>
+    </row>
+    <row r="30" spans="1:9" ht="65.950000">
       <c r="A30" s="34">
         <v>29</v>
       </c>
-      <c r="B30" s="34"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="34"/>
-      <c r="H30" s="34"/>
-    </row>
-    <row r="31" spans="1:8" ht="16.500000">
+      <c r="B30" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="C30" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="56" t="s">
+        <v>111</v>
+      </c>
+      <c r="E30" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="F30" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="G30" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="H30" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="I30" s="40"/>
+    </row>
+    <row r="31" spans="1:9" ht="65.950000">
       <c r="A31" s="34">
         <v>30</v>
       </c>
-      <c r="B31" s="34"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="34"/>
-      <c r="E31" s="34"/>
-      <c r="F31" s="34"/>
-      <c r="G31" s="34"/>
-      <c r="H31" s="34"/>
-    </row>
-    <row r="32" spans="1:8" ht="16.500000">
+      <c r="B31" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="C31" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="D31" s="53" t="s">
+        <v>105</v>
+      </c>
+      <c r="E31" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="F31" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="G31" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="H31" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="I31" s="40"/>
+    </row>
+    <row r="32" spans="1:9" ht="16.500000">
       <c r="A32" s="34">
         <v>31</v>
       </c>
-      <c r="B32" s="34"/>
-      <c r="C32" s="34"/>
+      <c r="B32" s="57"/>
+      <c r="C32" s="39"/>
       <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34"/>
+      <c r="E32" s="39"/>
+      <c r="F32" s="39"/>
       <c r="G32" s="34"/>
       <c r="H32" s="34"/>
-    </row>
-    <row r="33" spans="1:8" ht="16.500000">
+      <c r="I32" s="40"/>
+    </row>
+    <row r="33" spans="1:9" ht="16.500000">
       <c r="A33" s="34">
         <v>32</v>
       </c>
-      <c r="B33" s="34"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34"/>
+      <c r="B33" s="40"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="40"/>
+      <c r="F33" s="40"/>
       <c r="G33" s="34"/>
       <c r="H33" s="34"/>
-    </row>
-    <row r="34" spans="1:8" ht="16.500000">
+      <c r="I33" s="40"/>
+    </row>
+    <row r="34" spans="1:9" ht="16.500000">
       <c r="A34" s="34">
         <v>33</v>
       </c>
@@ -2208,8 +2482,9 @@
       <c r="F34" s="34"/>
       <c r="G34" s="34"/>
       <c r="H34" s="34"/>
-    </row>
-    <row r="35" spans="1:8" ht="16.500000">
+      <c r="I34" s="40"/>
+    </row>
+    <row r="35" spans="1:9" ht="16.500000">
       <c r="A35" s="34">
         <v>34</v>
       </c>
@@ -2220,8 +2495,9 @@
       <c r="F35" s="34"/>
       <c r="G35" s="34"/>
       <c r="H35" s="34"/>
-    </row>
-    <row r="36" spans="1:8" ht="16.500000">
+      <c r="I35" s="40"/>
+    </row>
+    <row r="36" spans="1:9" ht="16.500000">
       <c r="A36" s="34">
         <v>35</v>
       </c>
@@ -2232,8 +2508,9 @@
       <c r="F36" s="34"/>
       <c r="G36" s="34"/>
       <c r="H36" s="34"/>
-    </row>
-    <row r="37" spans="1:8" ht="16.500000">
+      <c r="I36" s="40"/>
+    </row>
+    <row r="37" spans="1:9" ht="16.500000">
       <c r="A37" s="34">
         <v>36</v>
       </c>
@@ -2244,8 +2521,9 @@
       <c r="F37" s="34"/>
       <c r="G37" s="34"/>
       <c r="H37" s="34"/>
-    </row>
-    <row r="38" spans="1:8" ht="16.500000">
+      <c r="I37" s="40"/>
+    </row>
+    <row r="38" spans="1:9" ht="16.500000">
       <c r="A38" s="34">
         <v>37</v>
       </c>
@@ -2256,8 +2534,9 @@
       <c r="F38" s="34"/>
       <c r="G38" s="34"/>
       <c r="H38" s="34"/>
-    </row>
-    <row r="39" spans="1:8" ht="16.500000">
+      <c r="I38" s="40"/>
+    </row>
+    <row r="39" spans="1:9" ht="16.500000">
       <c r="A39" s="34">
         <v>38</v>
       </c>
@@ -2268,7 +2547,9 @@
       <c r="F39" s="34"/>
       <c r="G39" s="34"/>
       <c r="H39" s="34"/>
-    </row>
+      <c r="I39" s="40"/>
+    </row>
+    <row r="40" spans="1:9"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="H1">

</xml_diff>

<commit_message>
debugging for login functionality on app
</commit_message>
<xml_diff>
--- a/testing/Team eXi Test Cases.xlsx
+++ b/testing/Team eXi Test Cases.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
   <si>
     <t>S/N</t>
   </si>
@@ -425,6 +425,24 @@
   </si>
   <si>
     <t>Pass/Fail after debugging</t>
+  </si>
+  <si>
+    <t>Error Message Wrong Password</t>
+  </si>
+  <si>
+    <t>Error Message Account does not exist</t>
+  </si>
+  <si>
+    <t>Error Message Username does not exist</t>
+  </si>
+  <si>
+    <t>Psas</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Login Error (Invalid Email / Password)</t>
   </si>
 </sst>
 </file>
@@ -1673,8 +1691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z39"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" tabSelected="1" zoomScale="180" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView topLeftCell="A27" tabSelected="1" zoomScale="180" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.500000"/>
@@ -2335,7 +2353,9 @@
       <c r="H27" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="I27" s="40"/>
+      <c r="I27" s="45" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="28" spans="1:9" ht="65.950000">
       <c r="A28" s="34">
@@ -2362,7 +2382,9 @@
       <c r="H28" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="I28" s="40"/>
+      <c r="I28" s="45" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="29" spans="1:9" ht="65.950000">
       <c r="A29" s="34">
@@ -2384,12 +2406,14 @@
         <v>110</v>
       </c>
       <c r="G29" s="34" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="H29" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="I29" s="40"/>
+      <c r="I29" s="45" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="30" spans="1:9" ht="65.950000">
       <c r="A30" s="34">
@@ -2408,15 +2432,17 @@
         <v>106</v>
       </c>
       <c r="F30" s="25" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="G30" s="34" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="H30" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="I30" s="40"/>
+      <c r="I30" s="45" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="31" spans="1:9" ht="65.950000">
       <c r="A31" s="34">
@@ -2443,7 +2469,9 @@
       <c r="H31" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="I31" s="40"/>
+      <c r="I31" s="45" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="32" spans="1:9" ht="16.500000">
       <c r="A32" s="34">

</xml_diff>

<commit_message>
adding reset password functionality for app
</commit_message>
<xml_diff>
--- a/testing/Team eXi Test Cases.xlsx
+++ b/testing/Team eXi Test Cases.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="129">
   <si>
     <t>S/N</t>
   </si>
@@ -443,6 +443,25 @@
   </si>
   <si>
     <t>Login Error (Invalid Email / Password)</t>
+  </si>
+  <si>
+    <t>Account Management (App)</t>
+  </si>
+  <si>
+    <t>Old Pwd: jerald86
+New Pwd: amytan97</t>
+  </si>
+  <si>
+    <t>Old Pwd: jerald86
+New Pwd: jerald97</t>
+  </si>
+  <si>
+    <t>Old Pwd: jerald86
+New Pwd: jerald</t>
+  </si>
+  <si>
+    <t>Old Pwd: jerald8
+New Pwd: jerald97</t>
   </si>
 </sst>
 </file>
@@ -1691,8 +1710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z39"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" tabSelected="1" zoomScale="180" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView topLeftCell="A28" tabSelected="1" zoomScale="180" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.500000"/>
@@ -1892,7 +1911,7 @@
       <c r="I7" s="40"/>
     </row>
     <row r="8" spans="1:26" ht="65.950000">
-      <c r="A8" s="35">
+      <c r="A8" s="24">
         <v>7</v>
       </c>
       <c r="B8" s="36" t="s">
@@ -1915,7 +1934,7 @@
       <c r="I8" s="40"/>
     </row>
     <row r="9" spans="1:26" ht="49.600000">
-      <c r="A9" s="34">
+      <c r="A9" s="24">
         <v>8</v>
       </c>
       <c r="B9" s="34" t="s">
@@ -1938,7 +1957,7 @@
       <c r="I9" s="40"/>
     </row>
     <row r="10" spans="1:26" ht="147.700000">
-      <c r="A10" s="34">
+      <c r="A10" s="24">
         <v>9</v>
       </c>
       <c r="B10" s="34" t="s">
@@ -1961,7 +1980,7 @@
       <c r="I10" s="40"/>
     </row>
     <row r="11" spans="1:26" ht="131.350000">
-      <c r="A11" s="34">
+      <c r="A11" s="24">
         <v>10</v>
       </c>
       <c r="B11" s="34" t="s">
@@ -1984,7 +2003,7 @@
       <c r="I11" s="40"/>
     </row>
     <row r="12" spans="1:26" ht="131.350000">
-      <c r="A12" s="34">
+      <c r="A12" s="24">
         <v>11</v>
       </c>
       <c r="B12" s="34" t="s">
@@ -2007,7 +2026,7 @@
       <c r="I12" s="40"/>
     </row>
     <row r="13" spans="1:26" ht="65.950000">
-      <c r="A13" s="34">
+      <c r="A13" s="24">
         <v>12</v>
       </c>
       <c r="B13" s="34" t="s">
@@ -2030,7 +2049,7 @@
       <c r="I13" s="40"/>
     </row>
     <row r="14" spans="1:26" ht="65.950000">
-      <c r="A14" s="34">
+      <c r="A14" s="24">
         <v>13</v>
       </c>
       <c r="B14" s="34" t="s">
@@ -2053,7 +2072,7 @@
       <c r="I14" s="40"/>
     </row>
     <row r="15" spans="1:26" ht="65.950000">
-      <c r="A15" s="34">
+      <c r="A15" s="24">
         <v>14</v>
       </c>
       <c r="B15" s="34" t="s">
@@ -2075,205 +2094,205 @@
       <c r="H15" s="34"/>
       <c r="I15" s="40"/>
     </row>
-    <row r="16" spans="1:26" ht="65.950000">
-      <c r="A16" s="34">
+    <row r="16" spans="1:26" ht="115.000000">
+      <c r="A16" s="24">
         <v>15</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="D16" s="34" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="E16" s="34" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="F16" s="34" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="G16" s="34"/>
       <c r="H16" s="34"/>
       <c r="I16" s="40"/>
     </row>
     <row r="17" spans="1:9" ht="115.000000">
-      <c r="A17" s="34">
+      <c r="A17" s="24">
         <v>16</v>
       </c>
       <c r="B17" s="34" t="s">
         <v>52</v>
       </c>
       <c r="C17" s="34" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D17" s="34" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E17" s="34" t="s">
         <v>56</v>
       </c>
       <c r="F17" s="34" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G17" s="34"/>
       <c r="H17" s="34"/>
       <c r="I17" s="40"/>
     </row>
-    <row r="18" spans="1:9" ht="115.000000">
-      <c r="A18" s="34">
+    <row r="18" spans="1:9" ht="131.350000">
+      <c r="A18" s="24">
         <v>17</v>
       </c>
       <c r="B18" s="34" t="s">
         <v>52</v>
       </c>
       <c r="C18" s="34" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D18" s="34" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="E18" s="34" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="F18" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
+        <v>64</v>
+      </c>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
       <c r="I18" s="40"/>
     </row>
-    <row r="19" spans="1:9" ht="131.350000">
-      <c r="A19" s="34">
+    <row r="19" spans="1:9" ht="147.700000">
+      <c r="A19" s="24">
         <v>18</v>
       </c>
       <c r="B19" s="34" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="C19" s="34" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D19" s="34" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="E19" s="34" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F19" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
+        <v>73</v>
+      </c>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
       <c r="I19" s="40"/>
     </row>
     <row r="20" spans="1:9" ht="147.700000">
-      <c r="A20" s="34">
+      <c r="A20" s="24">
         <v>19</v>
       </c>
       <c r="B20" s="34" t="s">
         <v>65</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="D20" s="34" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E20" s="34" t="s">
         <v>72</v>
       </c>
       <c r="F20" s="34" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="G20" s="34"/>
       <c r="H20" s="34"/>
       <c r="I20" s="40"/>
     </row>
     <row r="21" spans="1:9" ht="147.700000">
-      <c r="A21" s="34">
+      <c r="A21" s="24">
         <v>20</v>
       </c>
       <c r="B21" s="34" t="s">
         <v>65</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D21" s="34" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E21" s="34" t="s">
         <v>72</v>
       </c>
       <c r="F21" s="34" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G21" s="34"/>
       <c r="H21" s="34"/>
       <c r="I21" s="40"/>
     </row>
-    <row r="22" spans="1:9" ht="147.700000">
-      <c r="A22" s="34">
+    <row r="22" spans="1:9" ht="115.000000">
+      <c r="A22" s="24">
         <v>21</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="C22" s="34" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D22" s="34" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E22" s="34" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="F22" s="34" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="G22" s="34"/>
       <c r="H22" s="34"/>
       <c r="I22" s="40"/>
     </row>
     <row r="23" spans="1:9" ht="115.000000">
-      <c r="A23" s="34">
+      <c r="A23" s="24">
         <v>22</v>
       </c>
       <c r="B23" s="34" t="s">
         <v>80</v>
       </c>
       <c r="C23" s="34" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D23" s="34" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="E23" s="34" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="F23" s="34" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="G23" s="34"/>
       <c r="H23" s="34"/>
       <c r="I23" s="40"/>
     </row>
     <row r="24" spans="1:9" ht="115.000000">
-      <c r="A24" s="34">
+      <c r="A24" s="24">
         <v>23</v>
       </c>
       <c r="B24" s="34" t="s">
         <v>80</v>
       </c>
       <c r="C24" s="34" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="D24" s="34" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="E24" s="34" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="F24" s="34" t="s">
         <v>89</v>
@@ -2283,20 +2302,20 @@
       <c r="I24" s="40"/>
     </row>
     <row r="25" spans="1:9" ht="115.000000">
-      <c r="A25" s="34">
+      <c r="A25" s="24">
         <v>24</v>
       </c>
       <c r="B25" s="34" t="s">
         <v>80</v>
       </c>
       <c r="C25" s="34" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D25" s="34" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="E25" s="34" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="F25" s="34" t="s">
         <v>89</v>
@@ -2305,79 +2324,85 @@
       <c r="H25" s="34"/>
       <c r="I25" s="40"/>
     </row>
-    <row r="26" spans="1:9" ht="115.000000">
-      <c r="A26" s="34">
+    <row r="26" spans="1:9" ht="65.950000">
+      <c r="A26" s="24">
         <v>25</v>
       </c>
-      <c r="B26" s="34" t="s">
-        <v>80</v>
-      </c>
-      <c r="C26" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="D26" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="E26" s="34" t="s">
-        <v>98</v>
-      </c>
-      <c r="F26" s="34" t="s">
-        <v>89</v>
-      </c>
-      <c r="G26" s="34"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="40"/>
+      <c r="B26" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="43" t="s">
+        <v>102</v>
+      </c>
+      <c r="E26" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="F26" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="H26" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="I26" s="45" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="27" spans="1:9" ht="65.950000">
-      <c r="A27" s="34">
+      <c r="A27" s="24">
         <v>26</v>
       </c>
       <c r="B27" s="24" t="s">
         <v>100</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="D27" s="43" t="s">
-        <v>102</v>
+        <v>17</v>
+      </c>
+      <c r="D27" s="53" t="s">
+        <v>105</v>
       </c>
       <c r="E27" s="25" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="F27" s="25" t="s">
         <v>12</v>
       </c>
       <c r="G27" s="34" t="s">
-        <v>12</v>
+        <v>108</v>
       </c>
       <c r="H27" s="34" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="I27" s="45" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="65.950000">
-      <c r="A28" s="34">
+      <c r="A28" s="24">
         <v>27</v>
       </c>
       <c r="B28" s="24" t="s">
         <v>100</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="D28" s="53" t="s">
-        <v>105</v>
+        <v>18</v>
+      </c>
+      <c r="D28" s="43" t="s">
+        <v>109</v>
       </c>
       <c r="E28" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F28" s="25" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="G28" s="34" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="H28" s="34" t="s">
         <v>107</v>
@@ -2387,7 +2412,7 @@
       </c>
     </row>
     <row r="29" spans="1:9" ht="65.950000">
-      <c r="A29" s="34">
+      <c r="A29" s="24">
         <v>28</v>
       </c>
       <c r="B29" s="24" t="s">
@@ -2396,14 +2421,14 @@
       <c r="C29" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D29" s="43" t="s">
-        <v>109</v>
+      <c r="D29" s="56" t="s">
+        <v>111</v>
       </c>
       <c r="E29" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F29" s="25" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="G29" s="34" t="s">
         <v>120</v>
@@ -2416,91 +2441,105 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="65.950000">
-      <c r="A30" s="34">
+      <c r="A30" s="24">
         <v>29</v>
       </c>
       <c r="B30" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="C30" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="D30" s="56" t="s">
-        <v>111</v>
+      <c r="C30" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="D30" s="53" t="s">
+        <v>105</v>
       </c>
       <c r="E30" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F30" s="25" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="G30" s="34" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="H30" s="34" t="s">
         <v>107</v>
       </c>
       <c r="I30" s="45" t="s">
-        <v>101</v>
+        <v>122</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="65.950000">
-      <c r="A31" s="34">
+      <c r="A31" s="24">
         <v>30</v>
       </c>
-      <c r="B31" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="C31" s="39" t="s">
-        <v>112</v>
-      </c>
-      <c r="D31" s="53" t="s">
-        <v>105</v>
-      </c>
-      <c r="E31" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="F31" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="G31" s="34" t="s">
-        <v>115</v>
-      </c>
-      <c r="H31" s="34" t="s">
-        <v>107</v>
-      </c>
-      <c r="I31" s="45" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="16.500000">
-      <c r="A32" s="34">
+      <c r="B31" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="C31" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="E31" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="F31" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="G31" s="34"/>
+      <c r="H31" s="34"/>
+      <c r="I31" s="40"/>
+    </row>
+    <row r="32" spans="1:9" ht="65.950000">
+      <c r="A32" s="24">
         <v>31</v>
       </c>
-      <c r="B32" s="57"/>
-      <c r="C32" s="39"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="39"/>
-      <c r="F32" s="39"/>
+      <c r="B32" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="C32" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="34" t="s">
+        <v>127</v>
+      </c>
+      <c r="E32" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="F32" s="34" t="s">
+        <v>44</v>
+      </c>
       <c r="G32" s="34"/>
       <c r="H32" s="34"/>
       <c r="I32" s="40"/>
     </row>
-    <row r="33" spans="1:9" ht="16.500000">
-      <c r="A33" s="34">
+    <row r="33" spans="1:9" ht="65.950000">
+      <c r="A33" s="24">
         <v>32</v>
       </c>
-      <c r="B33" s="40"/>
-      <c r="C33" s="40"/>
-      <c r="D33" s="40"/>
-      <c r="E33" s="40"/>
-      <c r="F33" s="40"/>
+      <c r="B33" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="C33" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="D33" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="E33" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="F33" s="34" t="s">
+        <v>44</v>
+      </c>
       <c r="G33" s="34"/>
       <c r="H33" s="34"/>
       <c r="I33" s="40"/>
     </row>
     <row r="34" spans="1:9" ht="16.500000">
-      <c r="A34" s="34">
+      <c r="A34" s="24">
         <v>33</v>
       </c>
       <c r="B34" s="34"/>
@@ -2513,7 +2552,7 @@
       <c r="I34" s="40"/>
     </row>
     <row r="35" spans="1:9" ht="16.500000">
-      <c r="A35" s="34">
+      <c r="A35" s="24">
         <v>34</v>
       </c>
       <c r="B35" s="34"/>
@@ -2526,7 +2565,7 @@
       <c r="I35" s="40"/>
     </row>
     <row r="36" spans="1:9" ht="16.500000">
-      <c r="A36" s="34">
+      <c r="A36" s="24">
         <v>35</v>
       </c>
       <c r="B36" s="34"/>
@@ -2539,7 +2578,7 @@
       <c r="I36" s="40"/>
     </row>
     <row r="37" spans="1:9" ht="16.500000">
-      <c r="A37" s="34">
+      <c r="A37" s="24">
         <v>36</v>
       </c>
       <c r="B37" s="34"/>
@@ -2552,7 +2591,7 @@
       <c r="I37" s="40"/>
     </row>
     <row r="38" spans="1:9" ht="16.500000">
-      <c r="A38" s="34">
+      <c r="A38" s="24">
         <v>37</v>
       </c>
       <c r="B38" s="34"/>
@@ -2564,20 +2603,7 @@
       <c r="H38" s="34"/>
       <c r="I38" s="40"/>
     </row>
-    <row r="39" spans="1:9" ht="16.500000">
-      <c r="A39" s="34">
-        <v>38</v>
-      </c>
-      <c r="B39" s="34"/>
-      <c r="C39" s="34"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="34"/>
-      <c r="F39" s="34"/>
-      <c r="G39" s="34"/>
-      <c r="H39" s="34"/>
-      <c r="I39" s="40"/>
-    </row>
-    <row r="40" spans="1:9"/>
+    <row r="39" spans="1:9"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="H1">

</xml_diff>

<commit_message>
testing for reset pwd functionality on app
</commit_message>
<xml_diff>
--- a/testing/Team eXi Test Cases.xlsx
+++ b/testing/Team eXi Test Cases.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="140">
   <si>
     <t>S/N</t>
   </si>
@@ -462,6 +462,39 @@
   <si>
     <t>Old Pwd: jerald8
 New Pwd: jerald97</t>
+  </si>
+  <si>
+    <t>Verify that the user is able to reset his password if they entered the registered email address</t>
+  </si>
+  <si>
+    <t>Email: jerald@steppingstones.com.sg</t>
+  </si>
+  <si>
+    <t>Verify that the user is able to receive his password reset email if they entered the registered email address</t>
+  </si>
+  <si>
+    <t>Input email in the email field</t>
+  </si>
+  <si>
+    <t>Password Reset Success Alert</t>
+  </si>
+  <si>
+    <t>Verify that the user is unable to receive his reset password email if he did not enter the registered email address</t>
+  </si>
+  <si>
+    <t>Email: huixin@gmail.com</t>
+  </si>
+  <si>
+    <t>Invalid Emai Alert</t>
+  </si>
+  <si>
+    <t>Invalid Email Alert</t>
+  </si>
+  <si>
+    <t>Verify that the user is unable to receive his reset password email if he left the email field blank</t>
+  </si>
+  <si>
+    <t>Email:</t>
   </si>
 </sst>
 </file>
@@ -1159,7 +1192,7 @@
     <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1331,6 +1364,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="33" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1710,8 +1746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z39"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" tabSelected="1" zoomScale="180" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView topLeftCell="A27" tabSelected="1" zoomScale="180" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.500000"/>
@@ -2469,7 +2505,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="65.950000">
+    <row r="31" spans="1:9" ht="49.600000">
       <c r="A31" s="24">
         <v>30</v>
       </c>
@@ -2477,22 +2513,26 @@
         <v>124</v>
       </c>
       <c r="C31" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="D31" s="34" t="s">
-        <v>126</v>
+        <v>131</v>
+      </c>
+      <c r="D31" s="63" t="s">
+        <v>130</v>
       </c>
       <c r="E31" s="34" t="s">
-        <v>40</v>
+        <v>132</v>
       </c>
       <c r="F31" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="G31" s="34"/>
-      <c r="H31" s="34"/>
+        <v>133</v>
+      </c>
+      <c r="G31" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="H31" s="34" t="s">
+        <v>122</v>
+      </c>
       <c r="I31" s="40"/>
     </row>
-    <row r="32" spans="1:9" ht="65.950000">
+    <row r="32" spans="1:9" ht="49.600000">
       <c r="A32" s="24">
         <v>31</v>
       </c>
@@ -2500,22 +2540,26 @@
         <v>124</v>
       </c>
       <c r="C32" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="D32" s="34" t="s">
-        <v>127</v>
+        <v>134</v>
+      </c>
+      <c r="D32" s="47" t="s">
+        <v>135</v>
       </c>
       <c r="E32" s="34" t="s">
-        <v>40</v>
+        <v>132</v>
       </c>
       <c r="F32" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="G32" s="34"/>
-      <c r="H32" s="34"/>
+        <v>137</v>
+      </c>
+      <c r="G32" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="H32" s="34" t="s">
+        <v>122</v>
+      </c>
       <c r="I32" s="40"/>
     </row>
-    <row r="33" spans="1:9" ht="65.950000">
+    <row r="33" spans="1:9" ht="49.600000">
       <c r="A33" s="24">
         <v>32</v>
       </c>
@@ -2523,19 +2567,23 @@
         <v>124</v>
       </c>
       <c r="C33" s="34" t="s">
-        <v>45</v>
+        <v>138</v>
       </c>
       <c r="D33" s="34" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="E33" s="34" t="s">
-        <v>40</v>
+        <v>132</v>
       </c>
       <c r="F33" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="G33" s="34"/>
-      <c r="H33" s="34"/>
+        <v>137</v>
+      </c>
+      <c r="G33" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="H33" s="34" t="s">
+        <v>122</v>
+      </c>
       <c r="I33" s="40"/>
     </row>
     <row r="34" spans="1:9" ht="16.500000">
@@ -2619,6 +2667,10 @@
       <formula1>"Pass,Fail"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink r:id="rId0" ref="D31"/>
+    <hyperlink r:id="rId1" ref="D32"/>
+  </hyperlinks>
   <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>

</xml_diff>

<commit_message>
Debug for login and update test case
</commit_message>
<xml_diff>
--- a/testing/Team eXi Test Cases.xlsx
+++ b/testing/Team eXi Test Cases.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DEYU\Documents\YR3 Term1\Thriving-Stones-Project\testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Riana\Desktop\FYP\Thriving-Stones-Project\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47E4F50-4164-40FF-822E-4C1683BF7991}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="36" windowWidth="25752" windowHeight="11592"/>
+    <workbookView xWindow="360" yWindow="40" windowWidth="25750" windowHeight="11590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 2" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="110">
   <si>
     <t>S/N</t>
   </si>
@@ -70,10 +71,6 @@
   </si>
   <si>
     <t>Login Error</t>
-  </si>
-  <si>
-    <t>Username: amytan
-Pwd: adminadmin!</t>
   </si>
   <si>
     <t>Verify that tutors are able to login with the designated accounts</t>
@@ -372,12 +369,32 @@
   <si>
     <t>Error Message, redundant subjects selected</t>
   </si>
+  <si>
+    <t>Username: jerald@steppingstones.com.sg
+Pwd: J4BuWZ6i0rFmfUTL</t>
+  </si>
+  <si>
+    <t>invalid password alert</t>
+  </si>
+  <si>
+    <t>Username: jerald@steppingstones.com.sg
+Pwd: adminadmin!</t>
+  </si>
+  <si>
+    <t>Show Admin Homepage</t>
+  </si>
+  <si>
+    <t>Show Tutor Homepage</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -385,32 +402,51 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="0"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="0"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -522,16 +558,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -571,7 +607,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -580,15 +616,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -924,23 +980,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="26.6640625" customWidth="1"/>
+    <col min="2" max="2" width="26.6328125" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="29.109375" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" customWidth="1"/>
-    <col min="7" max="7" width="13.21875" customWidth="1"/>
+    <col min="4" max="4" width="29.08984375" customWidth="1"/>
+    <col min="5" max="5" width="19.54296875" customWidth="1"/>
+    <col min="6" max="6" width="16.36328125" customWidth="1"/>
+    <col min="7" max="7" width="13.1796875" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="23.6640625" customWidth="1"/>
+    <col min="9" max="9" width="23.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -968,8 +1024,8 @@
       <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="23" t="s">
-        <v>75</v>
+      <c r="I1" s="21" t="s">
+        <v>74</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -989,7 +1045,7 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1008,11 +1064,17 @@
       <c r="F2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="22"/>
-    </row>
-    <row r="3" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+      <c r="G2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="I2" s="30" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1020,10 +1082,10 @@
         <v>8</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>104</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>11</v>
@@ -1031,11 +1093,17 @@
       <c r="F3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="14"/>
-    </row>
-    <row r="4" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+      <c r="G3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="I3" s="29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1043,7 +1111,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>14</v>
@@ -1054,11 +1122,17 @@
       <c r="F4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="14"/>
-    </row>
-    <row r="5" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+      <c r="G4" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="H4" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="I4" s="29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1066,10 +1140,10 @@
         <v>8</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>106</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>11</v>
@@ -1077,11 +1151,17 @@
       <c r="F5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="14"/>
-    </row>
-    <row r="6" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+      <c r="G5" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="H5" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="I5" s="29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1089,7 +1169,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>14</v>
@@ -1100,11 +1180,17 @@
       <c r="F6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="14"/>
-    </row>
-    <row r="7" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+      <c r="G6" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="H6" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="I6" s="29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1112,7 +1198,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>10</v>
@@ -1121,13 +1207,19 @@
         <v>11</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="7"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="14"/>
-    </row>
-    <row r="8" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="G7" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="H7" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="I7" s="29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -1135,469 +1227,475 @@
         <v>8</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>13</v>
+        <v>20</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>104</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>11</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="14"/>
-    </row>
-    <row r="9" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="G8" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="H8" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="I8" s="29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>8</v>
       </c>
       <c r="B9" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="D9" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="E9" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="F9" s="9" t="s">
         <v>26</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>27</v>
       </c>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
       <c r="I9" s="14"/>
     </row>
-    <row r="10" spans="1:26" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>9</v>
       </c>
       <c r="B10" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>28</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>29</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
       <c r="I10" s="14"/>
     </row>
-    <row r="11" spans="1:26" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>10</v>
       </c>
       <c r="B11" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>28</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>29</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
       <c r="I11" s="14"/>
     </row>
-    <row r="12" spans="1:26" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>11</v>
       </c>
       <c r="B12" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>28</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>29</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
       <c r="I12" s="14"/>
     </row>
-    <row r="13" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" ht="58" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>12</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="E13" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="F13" s="9" t="s">
         <v>35</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>36</v>
       </c>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
       <c r="I13" s="14"/>
     </row>
-    <row r="14" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" ht="58" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>13</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C14" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="E14" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="9" t="s">
         <v>38</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>39</v>
       </c>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
       <c r="I14" s="14"/>
     </row>
-    <row r="15" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" ht="58" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>14</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="9" t="s">
-        <v>41</v>
-      </c>
       <c r="E15" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
       <c r="I15" s="14"/>
     </row>
-    <row r="16" spans="1:26" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>15</v>
       </c>
       <c r="B16" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="D16" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" s="9" t="s">
+      <c r="F16" s="9" t="s">
         <v>44</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>45</v>
       </c>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
       <c r="I16" s="14"/>
     </row>
-    <row r="17" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>16</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D17" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="9" t="s">
         <v>48</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>49</v>
       </c>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
       <c r="I17" s="14"/>
     </row>
-    <row r="18" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>17</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C18" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="9" t="s">
         <v>50</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>51</v>
       </c>
       <c r="G18" s="14"/>
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
     </row>
-    <row r="19" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>18</v>
       </c>
       <c r="B19" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>53</v>
-      </c>
       <c r="D19" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="E19" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>90</v>
-      </c>
       <c r="H19" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I19" s="17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>19</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C20" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D20" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="E20" s="9" t="s">
+      <c r="G20" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="F20" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>56</v>
-      </c>
       <c r="H20" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I20" s="17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>20</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C21" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="G21" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="E21" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>93</v>
-      </c>
       <c r="H21" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I21" s="17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>21</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C22" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D22" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="E22" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F22" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="G22" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="F22" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>56</v>
-      </c>
       <c r="H22" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I22" s="17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>22</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C23" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="E23" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F23" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="G23" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="F23" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>56</v>
-      </c>
       <c r="H23" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I23" s="17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>23</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C24" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="D24" s="9" t="s">
-        <v>101</v>
-      </c>
       <c r="E24" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="G24" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="F24" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>56</v>
-      </c>
       <c r="H24" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I24" s="17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>24</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C25" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D25" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="E25" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F25" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="G25" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="F25" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>56</v>
-      </c>
       <c r="H25" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I25" s="17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>25</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D26" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>64</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>12</v>
@@ -1606,210 +1704,210 @@
         <v>12</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I26" s="17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>26</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D27" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E27" s="6" t="s">
         <v>65</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>66</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>12</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I27" s="17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>27</v>
       </c>
       <c r="B28" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="I28" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="C28" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G28" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="H28" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="I28" s="17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="I29" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D29" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="G29" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="H29" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="I29" s="17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>29</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C30" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F30" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D30" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="E30" s="6" t="s">
+      <c r="G30" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="H30" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="F30" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="G30" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="H30" s="9" t="s">
-        <v>67</v>
-      </c>
       <c r="I30" s="17" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>30</v>
       </c>
       <c r="B31" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D31" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="E31" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="D31" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="E31" s="9" t="s">
+      <c r="F31" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="F31" s="9" t="s">
-        <v>83</v>
-      </c>
       <c r="G31" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I31" s="14"/>
     </row>
-    <row r="32" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>31</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C32" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D32" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="D32" s="18" t="s">
+      <c r="E32" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F32" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="E32" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="F32" s="9" t="s">
-        <v>86</v>
-      </c>
       <c r="G32" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H32" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I32" s="14"/>
     </row>
-    <row r="33" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>32</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C33" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D33" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D33" s="9" t="s">
-        <v>88</v>
-      </c>
       <c r="E33" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H33" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I33" s="14"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -1822,7 +1920,7 @@
       <c r="H34" s="9"/>
       <c r="I34" s="14"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -1835,7 +1933,7 @@
       <c r="H35" s="9"/>
       <c r="I35" s="14"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -1848,7 +1946,7 @@
       <c r="H36" s="9"/>
       <c r="I36" s="14"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -1861,7 +1959,7 @@
       <c r="H37" s="9"/>
       <c r="I37" s="14"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -1875,7 +1973,7 @@
       <c r="I38" s="14"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H1">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"fail"</formula>
@@ -1885,13 +1983,13 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Pass,Fail"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D31" r:id="rId1"/>
-    <hyperlink ref="D32" r:id="rId2"/>
+    <hyperlink ref="D31" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D32" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Updated Student Delete Testcase
</commit_message>
<xml_diff>
--- a/testing/Team eXi Test Cases.xlsx
+++ b/testing/Team eXi Test Cases.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SCHOOL\y3s1\IS480 FYP\Thriving-Stones-Project\testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DEYU\Documents\YR3 Term1\IS Application Project\Thriving-Stones-Project\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{871B098A-0F05-4698-9EB3-056CE6086646}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="36" windowWidth="25752" windowHeight="11592"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 2" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="174">
   <si>
     <t>S/N</t>
   </si>
@@ -703,11 +702,26 @@
 Tutor Email: shawn@steppingstones.com.sg
 Tutor Age: </t>
   </si>
+  <si>
+    <t>Delete Student (Web)</t>
+  </si>
+  <si>
+    <t>Verify that all the data related to student will be deleted from database</t>
+  </si>
+  <si>
+    <t>Click Rubbish Bin Icon on selected student</t>
+  </si>
+  <si>
+    <t>No inputs</t>
+  </si>
+  <si>
+    <t>Student Deleted successfully and display message "Deleted Student record successfully"</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -771,7 +785,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -876,22 +890,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -937,9 +940,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1279,27 +1279,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z105"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z106"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L29" sqref="L29"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="29.140625" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="29.109375" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="23.7109375" customWidth="1"/>
+    <col min="9" max="9" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1345,7 +1345,7 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1368,7 +1368,7 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="1:26" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1391,7 +1391,7 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:26" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1414,7 +1414,7 @@
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:26" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1437,7 +1437,7 @@
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:26" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1460,7 +1460,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:26" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1483,7 +1483,7 @@
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:26" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -1506,7 +1506,7 @@
       <c r="H8" s="16"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:26" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -1529,7 +1529,7 @@
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="1:26" ht="150" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1552,7 +1552,7 @@
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" spans="1:26" ht="150" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1575,7 +1575,7 @@
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
     </row>
-    <row r="12" spans="1:26" ht="150" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -1598,7 +1598,7 @@
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" spans="1:26" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1621,7 +1621,7 @@
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:26" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1644,7 +1644,7 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:26" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1667,7 +1667,7 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:26" ht="120" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1690,7 +1690,7 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1713,7 +1713,7 @@
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1736,7 +1736,7 @@
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
     </row>
-    <row r="19" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -1765,7 +1765,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -1794,7 +1794,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -1823,7 +1823,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -1852,7 +1852,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -1910,7 +1910,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -1939,27 +1939,27 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>25</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>61</v>
+        <v>169</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>9</v>
+        <v>170</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>63</v>
+        <v>172</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>64</v>
+        <v>171</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>12</v>
+        <v>173</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>173</v>
       </c>
       <c r="H26" s="4" t="s">
         <v>62</v>
@@ -1968,7 +1968,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -1976,28 +1976,28 @@
         <v>61</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>65</v>
+        <v>9</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>12</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I27" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -2005,19 +2005,19 @@
         <v>61</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>69</v>
+        <v>17</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>66</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="H28" s="4" t="s">
         <v>67</v>
@@ -2026,7 +2026,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -2036,14 +2036,14 @@
       <c r="C29" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D29" s="8" t="s">
-        <v>71</v>
+      <c r="D29" s="5" t="s">
+        <v>69</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>66</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>76</v>
@@ -2055,63 +2055,65 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>29</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>65</v>
+      <c r="C30" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>66</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H30" s="4" t="s">
         <v>67</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
         <v>30</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>79</v>
+      <c r="B31" s="5" t="s">
+        <v>61</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>83</v>
+        <v>72</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>73</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="H31" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I31" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="I31" s="4"/>
-    </row>
-    <row r="32" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -2119,26 +2121,26 @@
         <v>79</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>85</v>
+        <v>81</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>80</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>82</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H32" s="4" t="s">
         <v>77</v>
       </c>
       <c r="I32" s="4"/>
     </row>
-    <row r="33" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -2146,10 +2148,10 @@
         <v>79</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>85</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>82</v>
@@ -2165,36 +2167,34 @@
       </c>
       <c r="I33" s="4"/>
     </row>
-    <row r="34" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
         <v>33</v>
       </c>
-      <c r="B34" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="E34" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="F34" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="G34" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="H34" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="I34" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="B34" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I34" s="4"/>
+    </row>
+    <row r="35" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -2202,26 +2202,28 @@
         <v>105</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="G35" s="11" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="H35" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="I35" s="4"/>
-    </row>
-    <row r="36" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="I35" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -2232,7 +2234,7 @@
         <v>111</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E36" s="11" t="s">
         <v>112</v>
@@ -2248,7 +2250,7 @@
       </c>
       <c r="I36" s="4"/>
     </row>
-    <row r="37" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -2256,13 +2258,13 @@
         <v>105</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F37" s="11" t="s">
         <v>114</v>
@@ -2275,7 +2277,7 @@
       </c>
       <c r="I37" s="4"/>
     </row>
-    <row r="38" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -2286,10 +2288,10 @@
         <v>118</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F38" s="11" t="s">
         <v>114</v>
@@ -2302,7 +2304,7 @@
       </c>
       <c r="I38" s="4"/>
     </row>
-    <row r="39" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -2310,13 +2312,13 @@
         <v>105</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F39" s="11" t="s">
         <v>114</v>
@@ -2329,7 +2331,7 @@
       </c>
       <c r="I39" s="4"/>
     </row>
-    <row r="40" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -2337,13 +2339,13 @@
         <v>105</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>114</v>
@@ -2356,7 +2358,7 @@
       </c>
       <c r="I40" s="4"/>
     </row>
-    <row r="41" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -2364,13 +2366,13 @@
         <v>105</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>123</v>
+        <v>138</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>124</v>
+        <v>139</v>
       </c>
       <c r="F41" s="11" t="s">
         <v>114</v>
@@ -2383,7 +2385,7 @@
       </c>
       <c r="I41" s="4"/>
     </row>
-    <row r="42" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -2391,13 +2393,13 @@
         <v>105</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F42" s="11" t="s">
         <v>114</v>
@@ -2410,7 +2412,7 @@
       </c>
       <c r="I42" s="4"/>
     </row>
-    <row r="43" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -2421,10 +2423,10 @@
         <v>126</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E43" s="11" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F43" s="11" t="s">
         <v>114</v>
@@ -2437,7 +2439,7 @@
       </c>
       <c r="I43" s="4"/>
     </row>
-    <row r="44" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -2448,10 +2450,10 @@
         <v>126</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F44" s="11" t="s">
         <v>114</v>
@@ -2464,7 +2466,7 @@
       </c>
       <c r="I44" s="4"/>
     </row>
-    <row r="45" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -2475,10 +2477,10 @@
         <v>126</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F45" s="11" t="s">
         <v>114</v>
@@ -2491,7 +2493,7 @@
       </c>
       <c r="I45" s="4"/>
     </row>
-    <row r="46" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -2502,10 +2504,10 @@
         <v>126</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F46" s="11" t="s">
         <v>114</v>
@@ -2518,7 +2520,7 @@
       </c>
       <c r="I46" s="4"/>
     </row>
-    <row r="47" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -2529,10 +2531,10 @@
         <v>126</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F47" s="11" t="s">
         <v>114</v>
@@ -2545,62 +2547,62 @@
       </c>
       <c r="I47" s="4"/>
     </row>
-    <row r="48" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A48" s="5">
         <v>47</v>
       </c>
-      <c r="B48" s="13" t="s">
+      <c r="B48" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="C48" s="13" t="s">
+      <c r="C48" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="D48" s="13" t="s">
+      <c r="D48" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="E48" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="F48" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="G48" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="H48" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="I48" s="4"/>
+    </row>
+    <row r="49" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A49" s="5">
+        <v>48</v>
+      </c>
+      <c r="B49" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D49" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="E48" s="13" t="s">
+      <c r="E49" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="F48" s="13" t="s">
+      <c r="F49" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="G48" s="13" t="s">
+      <c r="G49" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="H48" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="I48" s="16"/>
-    </row>
-    <row r="49" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="17">
-        <v>48</v>
-      </c>
-      <c r="B49" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="C49" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="D49" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="E49" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F49" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="G49" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="H49" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="I49" s="18"/>
-    </row>
-    <row r="50" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="17">
+      <c r="H49" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="I49" s="16"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" s="5">
         <v>49</v>
       </c>
       <c r="B50" s="14" t="s">
@@ -2610,24 +2612,24 @@
         <v>145</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E50" s="14" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F50" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G50" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H50" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="I50" s="18"/>
-    </row>
-    <row r="51" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="17">
+      <c r="I50" s="17"/>
+    </row>
+    <row r="51" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A51" s="5">
         <v>50</v>
       </c>
       <c r="B51" s="14" t="s">
@@ -2637,7 +2639,7 @@
         <v>145</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E51" s="14" t="s">
         <v>151</v>
@@ -2651,74 +2653,74 @@
       <c r="H51" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="I51" s="18"/>
-    </row>
-    <row r="52" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A52" s="17">
+      <c r="I51" s="17"/>
+    </row>
+    <row r="52" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A52" s="5">
         <v>51</v>
       </c>
-      <c r="B52" s="18" t="s">
+      <c r="B52" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="C52" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="D52" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="E52" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="F52" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="G52" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="H52" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="I52" s="17"/>
+    </row>
+    <row r="53" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A53" s="5">
+        <v>52</v>
+      </c>
+      <c r="B53" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="C52" s="11" t="s">
+      <c r="C53" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="D52" s="11" t="s">
+      <c r="D53" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="E52" s="11" t="s">
+      <c r="E53" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="F52" s="11" t="s">
+      <c r="F53" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="G52" s="11" t="s">
+      <c r="G53" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="H52" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="I52" s="18"/>
-    </row>
-    <row r="53" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A53" s="17">
-        <v>52</v>
-      </c>
-      <c r="B53" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="C53" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="D53" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="E53" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="F53" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="G53" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="H53" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="I53" s="18"/>
-    </row>
-    <row r="54" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A54" s="17">
+      <c r="H53" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="I53" s="17"/>
+    </row>
+    <row r="54" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A54" s="5">
         <v>53</v>
       </c>
-      <c r="B54" s="18" t="s">
+      <c r="B54" s="17" t="s">
         <v>153</v>
       </c>
       <c r="C54" s="11" t="s">
         <v>111</v>
       </c>
       <c r="D54" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E54" s="11" t="s">
         <v>112</v>
@@ -2732,23 +2734,23 @@
       <c r="H54" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="I54" s="18"/>
-    </row>
-    <row r="55" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A55" s="17">
+      <c r="I54" s="17"/>
+    </row>
+    <row r="55" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A55" s="5">
         <v>54</v>
       </c>
-      <c r="B55" s="18" t="s">
+      <c r="B55" s="17" t="s">
         <v>153</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D55" s="11" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="E55" s="11" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F55" s="11" t="s">
         <v>156</v>
@@ -2759,23 +2761,23 @@
       <c r="H55" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="I55" s="18"/>
-    </row>
-    <row r="56" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A56" s="17">
+      <c r="I55" s="17"/>
+    </row>
+    <row r="56" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A56" s="5">
         <v>55</v>
       </c>
-      <c r="B56" s="18" t="s">
+      <c r="B56" s="17" t="s">
         <v>153</v>
       </c>
       <c r="C56" s="11" t="s">
         <v>118</v>
       </c>
       <c r="D56" s="11" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E56" s="11" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F56" s="11" t="s">
         <v>156</v>
@@ -2786,23 +2788,23 @@
       <c r="H56" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="I56" s="18"/>
-    </row>
-    <row r="57" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A57" s="17">
+      <c r="I56" s="17"/>
+    </row>
+    <row r="57" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A57" s="5">
         <v>56</v>
       </c>
-      <c r="B57" s="18" t="s">
+      <c r="B57" s="17" t="s">
         <v>153</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F57" s="11" t="s">
         <v>156</v>
@@ -2813,23 +2815,23 @@
       <c r="H57" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="I57" s="18"/>
-    </row>
-    <row r="58" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A58" s="17">
+      <c r="I57" s="17"/>
+    </row>
+    <row r="58" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A58" s="5">
         <v>57</v>
       </c>
-      <c r="B58" s="18" t="s">
+      <c r="B58" s="17" t="s">
         <v>153</v>
       </c>
       <c r="C58" s="11" t="s">
         <v>122</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F58" s="11" t="s">
         <v>156</v>
@@ -2840,23 +2842,23 @@
       <c r="H58" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="I58" s="18"/>
-    </row>
-    <row r="59" spans="1:9" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="17">
+      <c r="I58" s="17"/>
+    </row>
+    <row r="59" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A59" s="5">
         <v>58</v>
       </c>
-      <c r="B59" s="18" t="s">
+      <c r="B59" s="17" t="s">
         <v>153</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D59" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E59" s="11" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F59" s="11" t="s">
         <v>156</v>
@@ -2867,23 +2869,23 @@
       <c r="H59" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="I59" s="18"/>
-    </row>
-    <row r="60" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A60" s="17">
+      <c r="I59" s="17"/>
+    </row>
+    <row r="60" spans="1:9" ht="150.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="5">
         <v>59</v>
       </c>
-      <c r="B60" s="18" t="s">
+      <c r="B60" s="17" t="s">
         <v>153</v>
       </c>
       <c r="C60" s="11" t="s">
         <v>126</v>
       </c>
       <c r="D60" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E60" s="11" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F60" s="11" t="s">
         <v>156</v>
@@ -2894,23 +2896,23 @@
       <c r="H60" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="I60" s="18"/>
-    </row>
-    <row r="61" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A61" s="17">
+      <c r="I60" s="17"/>
+    </row>
+    <row r="61" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A61" s="5">
         <v>60</v>
       </c>
-      <c r="B61" s="18" t="s">
+      <c r="B61" s="17" t="s">
         <v>153</v>
       </c>
       <c r="C61" s="11" t="s">
         <v>126</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E61" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F61" s="11" t="s">
         <v>156</v>
@@ -2921,23 +2923,23 @@
       <c r="H61" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="I61" s="18"/>
-    </row>
-    <row r="62" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A62" s="17">
+      <c r="I61" s="17"/>
+    </row>
+    <row r="62" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A62" s="5">
         <v>61</v>
       </c>
-      <c r="B62" s="18" t="s">
+      <c r="B62" s="17" t="s">
         <v>153</v>
       </c>
       <c r="C62" s="11" t="s">
         <v>126</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E62" s="11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F62" s="11" t="s">
         <v>156</v>
@@ -2948,23 +2950,23 @@
       <c r="H62" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="I62" s="18"/>
-    </row>
-    <row r="63" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A63" s="17">
-        <v>62</v>
-      </c>
-      <c r="B63" s="18" t="s">
+      <c r="I62" s="17"/>
+    </row>
+    <row r="63" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A63" s="5">
+        <v>62</v>
+      </c>
+      <c r="B63" s="17" t="s">
         <v>153</v>
       </c>
       <c r="C63" s="11" t="s">
         <v>126</v>
       </c>
       <c r="D63" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E63" s="11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F63" s="11" t="s">
         <v>156</v>
@@ -2975,553 +2977,580 @@
       <c r="H63" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="I63" s="18"/>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="17">
+      <c r="I63" s="17"/>
+    </row>
+    <row r="64" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A64" s="5">
         <v>63</v>
       </c>
-      <c r="B64" s="18"/>
-      <c r="C64" s="11"/>
-      <c r="D64" s="11"/>
-      <c r="E64" s="11"/>
-      <c r="F64" s="11"/>
-      <c r="G64" s="11"/>
-      <c r="H64" s="11"/>
-      <c r="I64" s="18"/>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="17">
+      <c r="B64" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="C64" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="D64" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="E64" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="F64" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="G64" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H64" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="I64" s="17"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A65" s="5">
         <v>64</v>
       </c>
-      <c r="B65" s="18"/>
-      <c r="C65" s="13"/>
-      <c r="D65" s="13"/>
-      <c r="E65" s="13"/>
+      <c r="B65" s="17"/>
+      <c r="C65" s="11"/>
+      <c r="D65" s="11"/>
+      <c r="E65" s="11"/>
       <c r="F65" s="11"/>
       <c r="G65" s="11"/>
-      <c r="H65" s="13"/>
-      <c r="I65" s="18"/>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="17">
+      <c r="H65" s="11"/>
+      <c r="I65" s="17"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A66" s="5">
         <v>65</v>
       </c>
-      <c r="B66" s="18"/>
-      <c r="C66" s="18"/>
-      <c r="D66" s="18"/>
-      <c r="E66" s="18"/>
-      <c r="F66" s="18"/>
-      <c r="G66" s="18"/>
-      <c r="H66" s="18"/>
-      <c r="I66" s="18"/>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="17">
+      <c r="B66" s="17"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="13"/>
+      <c r="E66" s="13"/>
+      <c r="F66" s="11"/>
+      <c r="G66" s="11"/>
+      <c r="H66" s="13"/>
+      <c r="I66" s="17"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A67" s="5">
         <v>66</v>
       </c>
-      <c r="B67" s="18"/>
-      <c r="C67" s="18"/>
-      <c r="D67" s="18"/>
-      <c r="E67" s="18"/>
-      <c r="F67" s="18"/>
-      <c r="G67" s="18"/>
-      <c r="H67" s="18"/>
-      <c r="I67" s="18"/>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="17">
+      <c r="B67" s="17"/>
+      <c r="C67" s="17"/>
+      <c r="D67" s="17"/>
+      <c r="E67" s="17"/>
+      <c r="F67" s="17"/>
+      <c r="G67" s="17"/>
+      <c r="H67" s="17"/>
+      <c r="I67" s="17"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A68" s="5">
         <v>67</v>
       </c>
-      <c r="B68" s="18"/>
-      <c r="C68" s="18"/>
-      <c r="D68" s="18"/>
-      <c r="E68" s="18"/>
-      <c r="F68" s="18"/>
-      <c r="G68" s="18"/>
-      <c r="H68" s="18"/>
-      <c r="I68" s="18"/>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="17">
+      <c r="B68" s="17"/>
+      <c r="C68" s="17"/>
+      <c r="D68" s="17"/>
+      <c r="E68" s="17"/>
+      <c r="F68" s="17"/>
+      <c r="G68" s="17"/>
+      <c r="H68" s="17"/>
+      <c r="I68" s="17"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A69" s="5">
         <v>68</v>
       </c>
-      <c r="B69" s="18"/>
-      <c r="C69" s="18"/>
-      <c r="D69" s="18"/>
-      <c r="E69" s="18"/>
-      <c r="F69" s="18"/>
-      <c r="G69" s="18"/>
-      <c r="H69" s="18"/>
-      <c r="I69" s="18"/>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="17">
+      <c r="B69" s="17"/>
+      <c r="C69" s="17"/>
+      <c r="D69" s="17"/>
+      <c r="E69" s="17"/>
+      <c r="F69" s="17"/>
+      <c r="G69" s="17"/>
+      <c r="H69" s="17"/>
+      <c r="I69" s="17"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A70" s="5">
         <v>69</v>
       </c>
-      <c r="B70" s="18"/>
-      <c r="C70" s="18"/>
-      <c r="D70" s="18"/>
-      <c r="E70" s="18"/>
-      <c r="F70" s="18"/>
-      <c r="G70" s="18"/>
-      <c r="H70" s="18"/>
-      <c r="I70" s="18"/>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="17">
+      <c r="B70" s="17"/>
+      <c r="C70" s="17"/>
+      <c r="D70" s="17"/>
+      <c r="E70" s="17"/>
+      <c r="F70" s="17"/>
+      <c r="G70" s="17"/>
+      <c r="H70" s="17"/>
+      <c r="I70" s="17"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A71" s="5">
         <v>70</v>
       </c>
-      <c r="B71" s="18"/>
-      <c r="C71" s="18"/>
-      <c r="D71" s="18"/>
-      <c r="E71" s="18"/>
-      <c r="F71" s="18"/>
-      <c r="G71" s="18"/>
-      <c r="H71" s="18"/>
-      <c r="I71" s="18"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="17">
+      <c r="B71" s="17"/>
+      <c r="C71" s="17"/>
+      <c r="D71" s="17"/>
+      <c r="E71" s="17"/>
+      <c r="F71" s="17"/>
+      <c r="G71" s="17"/>
+      <c r="H71" s="17"/>
+      <c r="I71" s="17"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A72" s="5">
         <v>71</v>
       </c>
-      <c r="B72" s="18"/>
-      <c r="C72" s="18"/>
-      <c r="D72" s="18"/>
-      <c r="E72" s="18"/>
-      <c r="F72" s="18"/>
-      <c r="G72" s="18"/>
-      <c r="H72" s="18"/>
-      <c r="I72" s="18"/>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" s="17">
+      <c r="B72" s="17"/>
+      <c r="C72" s="17"/>
+      <c r="D72" s="17"/>
+      <c r="E72" s="17"/>
+      <c r="F72" s="17"/>
+      <c r="G72" s="17"/>
+      <c r="H72" s="17"/>
+      <c r="I72" s="17"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A73" s="5">
         <v>72</v>
       </c>
-      <c r="B73" s="18"/>
-      <c r="C73" s="18"/>
-      <c r="D73" s="18"/>
-      <c r="E73" s="18"/>
-      <c r="F73" s="18"/>
-      <c r="G73" s="18"/>
-      <c r="H73" s="18"/>
-      <c r="I73" s="18"/>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="17">
+      <c r="B73" s="17"/>
+      <c r="C73" s="17"/>
+      <c r="D73" s="17"/>
+      <c r="E73" s="17"/>
+      <c r="F73" s="17"/>
+      <c r="G73" s="17"/>
+      <c r="H73" s="17"/>
+      <c r="I73" s="17"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A74" s="5">
         <v>73</v>
       </c>
-      <c r="B74" s="18"/>
-      <c r="C74" s="18"/>
-      <c r="D74" s="18"/>
-      <c r="E74" s="18"/>
-      <c r="F74" s="18"/>
-      <c r="G74" s="18"/>
-      <c r="H74" s="18"/>
-      <c r="I74" s="18"/>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" s="17">
+      <c r="B74" s="17"/>
+      <c r="C74" s="17"/>
+      <c r="D74" s="17"/>
+      <c r="E74" s="17"/>
+      <c r="F74" s="17"/>
+      <c r="G74" s="17"/>
+      <c r="H74" s="17"/>
+      <c r="I74" s="17"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A75" s="5">
         <v>74</v>
       </c>
-      <c r="B75" s="18"/>
-      <c r="C75" s="18"/>
-      <c r="D75" s="18"/>
-      <c r="E75" s="18"/>
-      <c r="F75" s="18"/>
-      <c r="G75" s="18"/>
-      <c r="H75" s="18"/>
-      <c r="I75" s="18"/>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="17">
+      <c r="B75" s="17"/>
+      <c r="C75" s="17"/>
+      <c r="D75" s="17"/>
+      <c r="E75" s="17"/>
+      <c r="F75" s="17"/>
+      <c r="G75" s="17"/>
+      <c r="H75" s="17"/>
+      <c r="I75" s="17"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A76" s="5">
         <v>75</v>
       </c>
-      <c r="B76" s="18"/>
-      <c r="C76" s="18"/>
-      <c r="D76" s="18"/>
-      <c r="E76" s="18"/>
-      <c r="F76" s="18"/>
-      <c r="G76" s="18"/>
-      <c r="H76" s="18"/>
-      <c r="I76" s="18"/>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" s="17">
+      <c r="B76" s="17"/>
+      <c r="C76" s="17"/>
+      <c r="D76" s="17"/>
+      <c r="E76" s="17"/>
+      <c r="F76" s="17"/>
+      <c r="G76" s="17"/>
+      <c r="H76" s="17"/>
+      <c r="I76" s="17"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A77" s="5">
         <v>76</v>
       </c>
-      <c r="B77" s="18"/>
-      <c r="C77" s="18"/>
-      <c r="D77" s="18"/>
-      <c r="E77" s="18"/>
-      <c r="F77" s="18"/>
-      <c r="G77" s="18"/>
-      <c r="H77" s="18"/>
-      <c r="I77" s="18"/>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" s="17">
+      <c r="B77" s="17"/>
+      <c r="C77" s="17"/>
+      <c r="D77" s="17"/>
+      <c r="E77" s="17"/>
+      <c r="F77" s="17"/>
+      <c r="G77" s="17"/>
+      <c r="H77" s="17"/>
+      <c r="I77" s="17"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A78" s="5">
         <v>77</v>
       </c>
-      <c r="B78" s="18"/>
-      <c r="C78" s="18"/>
-      <c r="D78" s="18"/>
-      <c r="E78" s="18"/>
-      <c r="F78" s="18"/>
-      <c r="G78" s="18"/>
-      <c r="H78" s="18"/>
-      <c r="I78" s="18"/>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" s="17">
+      <c r="B78" s="17"/>
+      <c r="C78" s="17"/>
+      <c r="D78" s="17"/>
+      <c r="E78" s="17"/>
+      <c r="F78" s="17"/>
+      <c r="G78" s="17"/>
+      <c r="H78" s="17"/>
+      <c r="I78" s="17"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A79" s="5">
         <v>78</v>
       </c>
-      <c r="B79" s="18"/>
-      <c r="C79" s="18"/>
-      <c r="D79" s="18"/>
-      <c r="E79" s="18"/>
-      <c r="F79" s="18"/>
-      <c r="G79" s="18"/>
-      <c r="H79" s="18"/>
-      <c r="I79" s="18"/>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" s="17">
+      <c r="B79" s="17"/>
+      <c r="C79" s="17"/>
+      <c r="D79" s="17"/>
+      <c r="E79" s="17"/>
+      <c r="F79" s="17"/>
+      <c r="G79" s="17"/>
+      <c r="H79" s="17"/>
+      <c r="I79" s="17"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A80" s="5">
         <v>79</v>
       </c>
-      <c r="B80" s="18"/>
-      <c r="C80" s="18"/>
-      <c r="D80" s="18"/>
-      <c r="E80" s="18"/>
-      <c r="F80" s="18"/>
-      <c r="G80" s="18"/>
-      <c r="H80" s="18"/>
-      <c r="I80" s="18"/>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A81" s="17">
+      <c r="B80" s="17"/>
+      <c r="C80" s="17"/>
+      <c r="D80" s="17"/>
+      <c r="E80" s="17"/>
+      <c r="F80" s="17"/>
+      <c r="G80" s="17"/>
+      <c r="H80" s="17"/>
+      <c r="I80" s="17"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A81" s="5">
         <v>80</v>
       </c>
-      <c r="B81" s="18"/>
-      <c r="C81" s="18"/>
-      <c r="D81" s="18"/>
-      <c r="E81" s="18"/>
-      <c r="F81" s="18"/>
-      <c r="G81" s="18"/>
-      <c r="H81" s="18"/>
-      <c r="I81" s="18"/>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A82" s="17">
+      <c r="B81" s="17"/>
+      <c r="C81" s="17"/>
+      <c r="D81" s="17"/>
+      <c r="E81" s="17"/>
+      <c r="F81" s="17"/>
+      <c r="G81" s="17"/>
+      <c r="H81" s="17"/>
+      <c r="I81" s="17"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A82" s="5">
         <v>81</v>
       </c>
-      <c r="B82" s="18"/>
-      <c r="C82" s="18"/>
-      <c r="D82" s="18"/>
-      <c r="E82" s="18"/>
-      <c r="F82" s="18"/>
-      <c r="G82" s="18"/>
-      <c r="H82" s="18"/>
-      <c r="I82" s="18"/>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A83" s="17">
+      <c r="B82" s="17"/>
+      <c r="C82" s="17"/>
+      <c r="D82" s="17"/>
+      <c r="E82" s="17"/>
+      <c r="F82" s="17"/>
+      <c r="G82" s="17"/>
+      <c r="H82" s="17"/>
+      <c r="I82" s="17"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A83" s="5">
         <v>82</v>
       </c>
-      <c r="B83" s="18"/>
-      <c r="C83" s="18"/>
-      <c r="D83" s="18"/>
-      <c r="E83" s="18"/>
-      <c r="F83" s="18"/>
-      <c r="G83" s="18"/>
-      <c r="H83" s="18"/>
-      <c r="I83" s="18"/>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A84" s="17">
+      <c r="B83" s="17"/>
+      <c r="C83" s="17"/>
+      <c r="D83" s="17"/>
+      <c r="E83" s="17"/>
+      <c r="F83" s="17"/>
+      <c r="G83" s="17"/>
+      <c r="H83" s="17"/>
+      <c r="I83" s="17"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A84" s="5">
         <v>83</v>
       </c>
-      <c r="B84" s="18"/>
-      <c r="C84" s="18"/>
-      <c r="D84" s="18"/>
-      <c r="E84" s="18"/>
-      <c r="F84" s="18"/>
-      <c r="G84" s="18"/>
-      <c r="H84" s="18"/>
-      <c r="I84" s="18"/>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A85" s="17">
+      <c r="B84" s="17"/>
+      <c r="C84" s="17"/>
+      <c r="D84" s="17"/>
+      <c r="E84" s="17"/>
+      <c r="F84" s="17"/>
+      <c r="G84" s="17"/>
+      <c r="H84" s="17"/>
+      <c r="I84" s="17"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A85" s="5">
         <v>84</v>
       </c>
-      <c r="B85" s="18"/>
-      <c r="C85" s="18"/>
-      <c r="D85" s="18"/>
-      <c r="E85" s="18"/>
-      <c r="F85" s="18"/>
-      <c r="G85" s="18"/>
-      <c r="H85" s="18"/>
-      <c r="I85" s="18"/>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A86" s="17">
+      <c r="B85" s="17"/>
+      <c r="C85" s="17"/>
+      <c r="D85" s="17"/>
+      <c r="E85" s="17"/>
+      <c r="F85" s="17"/>
+      <c r="G85" s="17"/>
+      <c r="H85" s="17"/>
+      <c r="I85" s="17"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A86" s="5">
         <v>85</v>
       </c>
-      <c r="B86" s="18"/>
-      <c r="C86" s="18"/>
-      <c r="D86" s="18"/>
-      <c r="E86" s="18"/>
-      <c r="F86" s="18"/>
-      <c r="G86" s="18"/>
-      <c r="H86" s="18"/>
-      <c r="I86" s="18"/>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A87" s="17">
+      <c r="B86" s="17"/>
+      <c r="C86" s="17"/>
+      <c r="D86" s="17"/>
+      <c r="E86" s="17"/>
+      <c r="F86" s="17"/>
+      <c r="G86" s="17"/>
+      <c r="H86" s="17"/>
+      <c r="I86" s="17"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A87" s="5">
         <v>86</v>
       </c>
-      <c r="B87" s="18"/>
-      <c r="C87" s="18"/>
-      <c r="D87" s="18"/>
-      <c r="E87" s="18"/>
-      <c r="F87" s="18"/>
-      <c r="G87" s="18"/>
-      <c r="H87" s="18"/>
-      <c r="I87" s="18"/>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A88" s="17">
+      <c r="B87" s="17"/>
+      <c r="C87" s="17"/>
+      <c r="D87" s="17"/>
+      <c r="E87" s="17"/>
+      <c r="F87" s="17"/>
+      <c r="G87" s="17"/>
+      <c r="H87" s="17"/>
+      <c r="I87" s="17"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A88" s="5">
         <v>87</v>
       </c>
-      <c r="B88" s="18"/>
-      <c r="C88" s="18"/>
-      <c r="D88" s="18"/>
-      <c r="E88" s="18"/>
-      <c r="F88" s="18"/>
-      <c r="G88" s="18"/>
-      <c r="H88" s="18"/>
-      <c r="I88" s="18"/>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A89" s="17">
+      <c r="B88" s="17"/>
+      <c r="C88" s="17"/>
+      <c r="D88" s="17"/>
+      <c r="E88" s="17"/>
+      <c r="F88" s="17"/>
+      <c r="G88" s="17"/>
+      <c r="H88" s="17"/>
+      <c r="I88" s="17"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A89" s="5">
         <v>88</v>
       </c>
-      <c r="B89" s="18"/>
-      <c r="C89" s="18"/>
-      <c r="D89" s="18"/>
-      <c r="E89" s="18"/>
-      <c r="F89" s="18"/>
-      <c r="G89" s="18"/>
-      <c r="H89" s="18"/>
-      <c r="I89" s="18"/>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A90" s="17">
+      <c r="B89" s="17"/>
+      <c r="C89" s="17"/>
+      <c r="D89" s="17"/>
+      <c r="E89" s="17"/>
+      <c r="F89" s="17"/>
+      <c r="G89" s="17"/>
+      <c r="H89" s="17"/>
+      <c r="I89" s="17"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A90" s="5">
         <v>89</v>
       </c>
-      <c r="B90" s="18"/>
-      <c r="C90" s="18"/>
-      <c r="D90" s="18"/>
-      <c r="E90" s="18"/>
-      <c r="F90" s="18"/>
-      <c r="G90" s="18"/>
-      <c r="H90" s="18"/>
-      <c r="I90" s="18"/>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A91" s="17">
+      <c r="B90" s="17"/>
+      <c r="C90" s="17"/>
+      <c r="D90" s="17"/>
+      <c r="E90" s="17"/>
+      <c r="F90" s="17"/>
+      <c r="G90" s="17"/>
+      <c r="H90" s="17"/>
+      <c r="I90" s="17"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A91" s="5">
         <v>90</v>
       </c>
-      <c r="B91" s="18"/>
-      <c r="C91" s="18"/>
-      <c r="D91" s="18"/>
-      <c r="E91" s="18"/>
-      <c r="F91" s="18"/>
-      <c r="G91" s="18"/>
-      <c r="H91" s="18"/>
-      <c r="I91" s="18"/>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A92" s="17">
+      <c r="B91" s="17"/>
+      <c r="C91" s="17"/>
+      <c r="D91" s="17"/>
+      <c r="E91" s="17"/>
+      <c r="F91" s="17"/>
+      <c r="G91" s="17"/>
+      <c r="H91" s="17"/>
+      <c r="I91" s="17"/>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A92" s="5">
         <v>91</v>
       </c>
-      <c r="B92" s="18"/>
-      <c r="C92" s="18"/>
-      <c r="D92" s="18"/>
-      <c r="E92" s="18"/>
-      <c r="F92" s="18"/>
-      <c r="G92" s="18"/>
-      <c r="H92" s="18"/>
-      <c r="I92" s="18"/>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A93" s="17">
+      <c r="B92" s="17"/>
+      <c r="C92" s="17"/>
+      <c r="D92" s="17"/>
+      <c r="E92" s="17"/>
+      <c r="F92" s="17"/>
+      <c r="G92" s="17"/>
+      <c r="H92" s="17"/>
+      <c r="I92" s="17"/>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A93" s="5">
         <v>92</v>
       </c>
-      <c r="B93" s="18"/>
-      <c r="C93" s="18"/>
-      <c r="D93" s="18"/>
-      <c r="E93" s="18"/>
-      <c r="F93" s="18"/>
-      <c r="G93" s="18"/>
-      <c r="H93" s="18"/>
-      <c r="I93" s="18"/>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A94" s="17">
+      <c r="B93" s="17"/>
+      <c r="C93" s="17"/>
+      <c r="D93" s="17"/>
+      <c r="E93" s="17"/>
+      <c r="F93" s="17"/>
+      <c r="G93" s="17"/>
+      <c r="H93" s="17"/>
+      <c r="I93" s="17"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A94" s="5">
         <v>93</v>
       </c>
-      <c r="B94" s="18"/>
-      <c r="C94" s="18"/>
-      <c r="D94" s="18"/>
-      <c r="E94" s="18"/>
-      <c r="F94" s="18"/>
-      <c r="G94" s="18"/>
-      <c r="H94" s="18"/>
-      <c r="I94" s="18"/>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A95" s="17">
+      <c r="B94" s="17"/>
+      <c r="C94" s="17"/>
+      <c r="D94" s="17"/>
+      <c r="E94" s="17"/>
+      <c r="F94" s="17"/>
+      <c r="G94" s="17"/>
+      <c r="H94" s="17"/>
+      <c r="I94" s="17"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A95" s="5">
         <v>94</v>
       </c>
-      <c r="B95" s="18"/>
-      <c r="C95" s="18"/>
-      <c r="D95" s="18"/>
-      <c r="E95" s="18"/>
-      <c r="F95" s="18"/>
-      <c r="G95" s="18"/>
-      <c r="H95" s="18"/>
-      <c r="I95" s="18"/>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A96" s="17">
+      <c r="B95" s="17"/>
+      <c r="C95" s="17"/>
+      <c r="D95" s="17"/>
+      <c r="E95" s="17"/>
+      <c r="F95" s="17"/>
+      <c r="G95" s="17"/>
+      <c r="H95" s="17"/>
+      <c r="I95" s="17"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A96" s="5">
         <v>95</v>
       </c>
-      <c r="B96" s="18"/>
-      <c r="C96" s="18"/>
-      <c r="D96" s="18"/>
-      <c r="E96" s="18"/>
-      <c r="F96" s="18"/>
-      <c r="G96" s="18"/>
-      <c r="H96" s="18"/>
-      <c r="I96" s="18"/>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A97" s="17">
+      <c r="B96" s="17"/>
+      <c r="C96" s="17"/>
+      <c r="D96" s="17"/>
+      <c r="E96" s="17"/>
+      <c r="F96" s="17"/>
+      <c r="G96" s="17"/>
+      <c r="H96" s="17"/>
+      <c r="I96" s="17"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A97" s="5">
         <v>96</v>
       </c>
-      <c r="B97" s="18"/>
-      <c r="C97" s="18"/>
-      <c r="D97" s="18"/>
-      <c r="E97" s="18"/>
-      <c r="F97" s="18"/>
-      <c r="G97" s="18"/>
-      <c r="H97" s="18"/>
-      <c r="I97" s="18"/>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A98" s="17">
+      <c r="B97" s="17"/>
+      <c r="C97" s="17"/>
+      <c r="D97" s="17"/>
+      <c r="E97" s="17"/>
+      <c r="F97" s="17"/>
+      <c r="G97" s="17"/>
+      <c r="H97" s="17"/>
+      <c r="I97" s="17"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A98" s="5">
         <v>97</v>
       </c>
-      <c r="B98" s="18"/>
-      <c r="C98" s="18"/>
-      <c r="D98" s="18"/>
-      <c r="E98" s="18"/>
-      <c r="F98" s="18"/>
-      <c r="G98" s="18"/>
-      <c r="H98" s="18"/>
-      <c r="I98" s="18"/>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A99" s="17">
+      <c r="B98" s="17"/>
+      <c r="C98" s="17"/>
+      <c r="D98" s="17"/>
+      <c r="E98" s="17"/>
+      <c r="F98" s="17"/>
+      <c r="G98" s="17"/>
+      <c r="H98" s="17"/>
+      <c r="I98" s="17"/>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A99" s="5">
         <v>98</v>
       </c>
-      <c r="B99" s="18"/>
-      <c r="C99" s="18"/>
-      <c r="D99" s="18"/>
-      <c r="E99" s="18"/>
-      <c r="F99" s="18"/>
-      <c r="G99" s="18"/>
-      <c r="H99" s="18"/>
-      <c r="I99" s="18"/>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A100" s="17">
+      <c r="B99" s="17"/>
+      <c r="C99" s="17"/>
+      <c r="D99" s="17"/>
+      <c r="E99" s="17"/>
+      <c r="F99" s="17"/>
+      <c r="G99" s="17"/>
+      <c r="H99" s="17"/>
+      <c r="I99" s="17"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A100" s="5">
         <v>99</v>
       </c>
-      <c r="B100" s="18"/>
-      <c r="C100" s="18"/>
-      <c r="D100" s="18"/>
-      <c r="E100" s="18"/>
-      <c r="F100" s="18"/>
-      <c r="G100" s="18"/>
-      <c r="H100" s="18"/>
-      <c r="I100" s="18"/>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A101" s="17">
+      <c r="B100" s="17"/>
+      <c r="C100" s="17"/>
+      <c r="D100" s="17"/>
+      <c r="E100" s="17"/>
+      <c r="F100" s="17"/>
+      <c r="G100" s="17"/>
+      <c r="H100" s="17"/>
+      <c r="I100" s="17"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A101" s="5">
         <v>100</v>
       </c>
-      <c r="B101" s="18"/>
-      <c r="C101" s="18"/>
-      <c r="D101" s="18"/>
-      <c r="E101" s="18"/>
-      <c r="F101" s="18"/>
-      <c r="G101" s="18"/>
-      <c r="H101" s="18"/>
-      <c r="I101" s="18"/>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A102" s="17">
+      <c r="B101" s="17"/>
+      <c r="C101" s="17"/>
+      <c r="D101" s="17"/>
+      <c r="E101" s="17"/>
+      <c r="F101" s="17"/>
+      <c r="G101" s="17"/>
+      <c r="H101" s="17"/>
+      <c r="I101" s="17"/>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A102" s="5">
         <v>101</v>
       </c>
-      <c r="B102" s="18"/>
-      <c r="C102" s="18"/>
-      <c r="D102" s="18"/>
-      <c r="E102" s="18"/>
-      <c r="F102" s="18"/>
-      <c r="G102" s="18"/>
-      <c r="H102" s="18"/>
-      <c r="I102" s="18"/>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A103" s="17">
+      <c r="B102" s="17"/>
+      <c r="C102" s="17"/>
+      <c r="D102" s="17"/>
+      <c r="E102" s="17"/>
+      <c r="F102" s="17"/>
+      <c r="G102" s="17"/>
+      <c r="H102" s="17"/>
+      <c r="I102" s="17"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A103" s="5">
         <v>102</v>
       </c>
-      <c r="B103" s="18"/>
-      <c r="C103" s="18"/>
-      <c r="D103" s="18"/>
-      <c r="E103" s="18"/>
-      <c r="F103" s="18"/>
-      <c r="G103" s="18"/>
-      <c r="H103" s="18"/>
-      <c r="I103" s="18"/>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A104" s="17">
+      <c r="B103" s="17"/>
+      <c r="C103" s="17"/>
+      <c r="D103" s="17"/>
+      <c r="E103" s="17"/>
+      <c r="F103" s="17"/>
+      <c r="G103" s="17"/>
+      <c r="H103" s="17"/>
+      <c r="I103" s="17"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A104" s="5">
         <v>103</v>
       </c>
-      <c r="B104" s="18"/>
-      <c r="C104" s="18"/>
-      <c r="D104" s="18"/>
-      <c r="E104" s="18"/>
-      <c r="F104" s="18"/>
-      <c r="G104" s="18"/>
-      <c r="H104" s="18"/>
-      <c r="I104" s="18"/>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A105" s="17">
+      <c r="B104" s="17"/>
+      <c r="C104" s="17"/>
+      <c r="D104" s="17"/>
+      <c r="E104" s="17"/>
+      <c r="F104" s="17"/>
+      <c r="G104" s="17"/>
+      <c r="H104" s="17"/>
+      <c r="I104" s="17"/>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A105" s="5">
         <v>104</v>
       </c>
-      <c r="B105" s="18"/>
-      <c r="C105" s="18"/>
-      <c r="D105" s="18"/>
-      <c r="E105" s="18"/>
-      <c r="F105" s="18"/>
-      <c r="G105" s="18"/>
-      <c r="H105" s="18"/>
-      <c r="I105" s="18"/>
+      <c r="B105" s="17"/>
+      <c r="C105" s="17"/>
+      <c r="D105" s="17"/>
+      <c r="E105" s="17"/>
+      <c r="F105" s="17"/>
+      <c r="G105" s="17"/>
+      <c r="H105" s="17"/>
+      <c r="I105" s="17"/>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A106" s="5">
+        <v>105</v>
+      </c>
+      <c r="B106" s="17"/>
+      <c r="C106" s="17"/>
+      <c r="D106" s="17"/>
+      <c r="E106" s="17"/>
+      <c r="F106" s="17"/>
+      <c r="G106" s="17"/>
+      <c r="H106" s="17"/>
+      <c r="I106" s="17"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -3534,13 +3563,13 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1">
       <formula1>"Pass,Fail"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D31" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D32" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D32" r:id="rId1"/>
+    <hyperlink ref="D33" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
Added TestCases for Iteration 3
</commit_message>
<xml_diff>
--- a/testing/Team eXi Test Cases.xlsx
+++ b/testing/Team eXi Test Cases.xlsx
@@ -5,22 +5,23 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SCHOOL\y3s1\IS480 FYP\Thriving-Stones-Project\testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DEYU\Documents\YR3 Term1\Thriving-Stones-Project\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{486D4823-32EC-48F8-A571-0AA3DF8C2FE4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BF828B0B-EF2F-4FDC-A23E-400758C1A437}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="36" windowWidth="25752" windowHeight="11592" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 2" sheetId="1" r:id="rId1"/>
+    <sheet name="Iteration 3" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="228">
   <si>
     <t>S/N</t>
   </si>
@@ -191,9 +192,6 @@
   </si>
   <si>
     <t>The tutor should be removed from the database</t>
-  </si>
-  <si>
-    <t>Sign Ups</t>
   </si>
   <si>
     <t>Verify that when all the neccessary information are filled in, the admin user would be able to successfully create the Student record in the database</t>
@@ -718,16 +716,232 @@
   <si>
     <t>Student Deleted successfully and display message "Deleted Student record successfully"</t>
   </si>
+  <si>
+    <t>Student Creation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete Student </t>
+  </si>
+  <si>
+    <t>Create Tutor</t>
+  </si>
+  <si>
+    <t>Delete Tutor</t>
+  </si>
+  <si>
+    <t>Update Tutor</t>
+  </si>
+  <si>
+    <t>Create Tuition Grade</t>
+  </si>
+  <si>
+    <t>Failed to create grade</t>
+  </si>
+  <si>
+    <t>Validating the field before create grade</t>
+  </si>
+  <si>
+    <t>Input the information as specified into the corresponding fields and click Create Grade</t>
+  </si>
+  <si>
+    <t>Error Message Display "The grade created for this class can only be English"</t>
+  </si>
+  <si>
+    <t>Left Grade empty</t>
+  </si>
+  <si>
+    <t>Select class:  -LHRRS0ATm04Hiarglhj (English) 
+Output lists of students in that class (Jimmy, Jenny)
+Select Examination: CA1
+Select Subject: English
+Select Location: Center
+Grade: Empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select class:  -LHRRS0ATm04Hiarglhj (English) 
+Select Examination: CA1
+Select Subject: Chemistry
+Select Location: Center
+Grade: 88
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select class:  -LHRRS0ATm04Hiarglhj (English) 
+Select Examination: CA1
+Select Subject: English
+Select Location: Center
+Grade: 1000
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select class:  -LHRRS0ATm04Hiarglhj (English) 
+Select Examination: CA1
+Select Subject: English
+Select Location: Center
+Grade: 88
+</t>
+  </si>
+  <si>
+    <t>Validating duplicate data before create grade</t>
+  </si>
+  <si>
+    <t>The CA1 grade for English is being created before however input the Examination field as CA1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Failed to create grade with errror message, pls enter valid grade </t>
+  </si>
+  <si>
+    <t>Failed to create grade with errror message, pls select location, subject, examination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select class:  -LHRRS0ATm04Hiarglhj (English) 
+Select Examination: Select Examination
+Select Subject: Select Subject
+Select Location: Select Location
+Grade: 88
+</t>
+  </si>
+  <si>
+    <t>Failed to create grade with errror message, CA1 grade already exist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select class:  -LHRRS0ATm04Hiarglhj (English) 
+Select Examination: SA2
+Select Subject: English
+Select Location: Center
+Grade: 88
+</t>
+  </si>
+  <si>
+    <t>Grade created successfully</t>
+  </si>
+  <si>
+    <t>Update Grade</t>
+  </si>
+  <si>
+    <t>StudentID: -</t>
+  </si>
+  <si>
+    <t>Doesn't input anything at StudentID field</t>
+  </si>
+  <si>
+    <t>Display message to input studentID</t>
+  </si>
+  <si>
+    <t>Retrieve Grade</t>
+  </si>
+  <si>
+    <t>Input all the neccessary information with correct data</t>
+  </si>
+  <si>
+    <t>StudentID: G1234567L</t>
+  </si>
+  <si>
+    <t>Input the information as specified into the corresponding fields and click Retrieve</t>
+  </si>
+  <si>
+    <t>Display specific student's grades</t>
+  </si>
+  <si>
+    <t>Redirect to another page to add info</t>
+  </si>
+  <si>
+    <t>Validating the field before update grade</t>
+  </si>
+  <si>
+    <t>Subject: Select Subject</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The dropdown of subjets should only be the subjects that student is taking currently. For studentID G1234567L (Jimmy Lee) is enrolled in English and Add-Maths) </t>
+  </si>
+  <si>
+    <t>If the dropdown is not English and Add-Maths only then it is wrong else success</t>
+  </si>
+  <si>
+    <t>Validating the data before update grade</t>
+  </si>
+  <si>
+    <t>Subject: Select Subject
+Level: Select Assessment Type
+Grade: -</t>
+  </si>
+  <si>
+    <t>Input the information as specified into the corresponding fields and click Update</t>
+  </si>
+  <si>
+    <t>Display all error messages. 
+Pls select subject!
+Pls Select Assessment Type!
+Invalid Grade!</t>
+  </si>
+  <si>
+    <t>Subject: Select Subject
+Level: Select Level</t>
+  </si>
+  <si>
+    <t>Input the information as specified into the corresponding fields and click Save</t>
+  </si>
+  <si>
+    <t>Display all error messages. 
+Pls select subject! 
+Pls select level!</t>
+  </si>
+  <si>
+    <t>Create Schedule</t>
+  </si>
+  <si>
+    <t>Create schedule successfully</t>
+  </si>
+  <si>
+    <t>Able to save 2 classes with same date/time</t>
+  </si>
+  <si>
+    <t>Subject: English
+Level: P3
+Time: 8:30-10:00 20 Aug 1018</t>
+  </si>
+  <si>
+    <t>Subject: English
+Level: P4
+Time: 8:30-10:00 20 Aug 1018</t>
+  </si>
+  <si>
+    <t>Update Schedule</t>
+  </si>
+  <si>
+    <t>Able to update the</t>
+  </si>
+  <si>
+    <t>Click Edit Icon on specific time and change date time</t>
+  </si>
+  <si>
+    <t>Update schedule successfully</t>
+  </si>
+  <si>
+    <t>Subject: English
+Level: P4
+Time: 8:30-10:00 23 Aug 1018</t>
+  </si>
+  <si>
+    <t>Create Grade</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -895,13 +1109,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -913,28 +1127,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -946,11 +1160,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1283,24 +1546,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C61" sqref="C61"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1:I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="29.140625" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="29.109375" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="23.7109375" customWidth="1"/>
+    <col min="9" max="9" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1326,7 +1589,7 @@
         <v>6</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -1346,7 +1609,7 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1369,7 +1632,7 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="1:26" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1392,7 +1655,7 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:26" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1415,7 +1678,7 @@
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:26" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1438,7 +1701,7 @@
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:26" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1461,7 +1724,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:26" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1484,7 +1747,7 @@
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:26" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -1507,7 +1770,7 @@
       <c r="H8" s="16"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:26" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -1530,7 +1793,7 @@
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="1:26" ht="150" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1553,7 +1816,7 @@
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" spans="1:26" ht="150" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1576,7 +1839,7 @@
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
     </row>
-    <row r="12" spans="1:26" ht="150" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -1599,7 +1862,7 @@
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" spans="1:26" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1622,7 +1885,7 @@
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:26" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1645,7 +1908,7 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:26" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1668,7 +1931,7 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:26" ht="120" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1691,7 +1954,7 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1714,7 +1977,7 @@
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1728,7 +1991,7 @@
         <v>25</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>51</v>
@@ -1737,253 +2000,253 @@
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
     </row>
-    <row r="19" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>53</v>
-      </c>
       <c r="D19" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>90</v>
-      </c>
       <c r="H19" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>52</v>
+        <v>173</v>
       </c>
       <c r="C20" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E20" s="4" t="s">
+      <c r="G20" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F20" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="H20" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>52</v>
+        <v>173</v>
       </c>
       <c r="C21" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="G21" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="E21" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>93</v>
-      </c>
       <c r="H21" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>52</v>
+        <v>173</v>
       </c>
       <c r="C22" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="E22" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F22" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="G22" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F22" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="H22" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>52</v>
+        <v>173</v>
       </c>
       <c r="C23" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="E23" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F23" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="G23" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F23" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="H23" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>52</v>
+        <v>173</v>
       </c>
       <c r="C24" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>101</v>
-      </c>
       <c r="E24" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G24" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F24" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="H24" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>52</v>
+        <v>173</v>
       </c>
       <c r="C25" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="E25" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F25" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="G25" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F25" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="H25" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>25</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="D26" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E26" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="F26" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="E26" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>173</v>
-      </c>
       <c r="G26" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>26</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D27" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>12</v>
@@ -1992,1022 +2255,1022 @@
         <v>12</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>27</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E28" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>66</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>12</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D29" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F29" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="G29" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H29" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F29" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="I29" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>29</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E30" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H30" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F30" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="I30" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
         <v>30</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C31" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F31" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D31" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="E31" s="5" t="s">
+      <c r="G31" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H31" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F31" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="I31" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <v>31</v>
       </c>
       <c r="B32" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D32" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="E32" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D32" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="E32" s="4" t="s">
+      <c r="F32" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="F32" s="4" t="s">
-        <v>83</v>
-      </c>
       <c r="G32" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I32" s="4"/>
     </row>
-    <row r="33" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
         <v>32</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C33" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D33" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="E33" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F33" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E33" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>86</v>
-      </c>
       <c r="G33" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I33" s="4"/>
     </row>
-    <row r="34" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
         <v>33</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C34" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D34" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D34" s="4" t="s">
-        <v>88</v>
-      </c>
       <c r="E34" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I34" s="4"/>
     </row>
-    <row r="35" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A35" s="5">
         <v>34</v>
       </c>
       <c r="B35" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C35" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="D35" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="D35" s="11" t="s">
+      <c r="E35" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="E35" s="11" t="s">
+      <c r="F35" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="F35" s="11" t="s">
+      <c r="G35" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="G35" s="11" t="s">
-        <v>110</v>
-      </c>
       <c r="H35" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I35" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
         <v>35</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C36" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="E36" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="D36" s="11" t="s">
+      <c r="F36" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="E36" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="F36" s="11" t="s">
-        <v>114</v>
-      </c>
       <c r="G36" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H36" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I36" s="4"/>
     </row>
-    <row r="37" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
         <v>36</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C37" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E37" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="D37" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="E37" s="11" t="s">
-        <v>112</v>
-      </c>
       <c r="F37" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G37" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H37" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I37" s="4"/>
     </row>
-    <row r="38" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
         <v>37</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G38" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H38" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I38" s="4"/>
     </row>
-    <row r="39" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
         <v>38</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C39" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="E39" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="D39" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="E39" s="11" t="s">
-        <v>119</v>
-      </c>
       <c r="F39" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G39" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H39" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I39" s="4"/>
     </row>
-    <row r="40" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A40" s="5">
         <v>39</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G40" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H40" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I40" s="4"/>
     </row>
-    <row r="41" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A41" s="5">
         <v>40</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C41" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="D41" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="D41" s="11" t="s">
+      <c r="E41" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="E41" s="11" t="s">
-        <v>139</v>
-      </c>
       <c r="F41" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G41" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H41" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I41" s="4"/>
     </row>
-    <row r="42" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
         <v>41</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C42" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D42" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="D42" s="11" t="s">
+      <c r="E42" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="E42" s="11" t="s">
-        <v>124</v>
-      </c>
       <c r="F42" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G42" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H42" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I42" s="4"/>
     </row>
-    <row r="43" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A43" s="5">
         <v>42</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C43" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D43" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="D43" s="11" t="s">
+      <c r="E43" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="E43" s="11" t="s">
-        <v>128</v>
-      </c>
       <c r="F43" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G43" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H43" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I43" s="4"/>
     </row>
-    <row r="44" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A44" s="5">
         <v>43</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F44" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G44" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H44" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I44" s="4"/>
     </row>
-    <row r="45" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A45" s="5">
         <v>44</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F45" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G45" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H45" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I45" s="4"/>
     </row>
-    <row r="46" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A46" s="5">
         <v>45</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D46" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E46" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="E46" s="11" t="s">
-        <v>134</v>
-      </c>
       <c r="F46" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H46" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I46" s="4"/>
     </row>
-    <row r="47" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A47" s="5">
         <v>46</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D47" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="E47" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="E47" s="11" t="s">
-        <v>136</v>
-      </c>
       <c r="F47" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G47" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H47" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I47" s="4"/>
     </row>
-    <row r="48" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A48" s="5">
         <v>47</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G48" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H48" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I48" s="4"/>
     </row>
-    <row r="49" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A49" s="5">
         <v>48</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D49" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E49" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F49" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G49" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H49" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I49" s="16"/>
     </row>
-    <row r="50" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="5">
         <v>49</v>
       </c>
       <c r="B50" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="C50" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="C50" s="14" t="s">
+      <c r="D50" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="D50" s="14" t="s">
+      <c r="E50" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="E50" s="14" t="s">
+      <c r="F50" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="F50" s="14" t="s">
-        <v>148</v>
-      </c>
       <c r="G50" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H50" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I50" s="17"/>
     </row>
-    <row r="51" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" s="5">
         <v>50</v>
       </c>
       <c r="B51" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="C51" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="C51" s="14" t="s">
-        <v>145</v>
-      </c>
       <c r="D51" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="E51" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="E51" s="14" t="s">
-        <v>151</v>
-      </c>
       <c r="F51" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G51" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H51" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I51" s="17"/>
     </row>
-    <row r="52" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A52" s="5">
         <v>51</v>
       </c>
       <c r="B52" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="C52" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="C52" s="14" t="s">
-        <v>145</v>
-      </c>
       <c r="D52" s="14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E52" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F52" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G52" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H52" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I52" s="17"/>
     </row>
-    <row r="53" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A53" s="5">
         <v>52</v>
       </c>
       <c r="B53" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="C53" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="C53" s="11" t="s">
+      <c r="D53" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="E53" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="F53" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="D53" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="E53" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="F53" s="11" t="s">
-        <v>155</v>
-      </c>
       <c r="G53" s="11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H53" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I53" s="17"/>
     </row>
-    <row r="54" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A54" s="5">
         <v>53</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C54" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D54" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="E54" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="D54" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="E54" s="11" t="s">
-        <v>112</v>
-      </c>
       <c r="F54" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G54" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H54" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I54" s="17"/>
     </row>
-    <row r="55" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A55" s="5">
         <v>54</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C55" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D55" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="E55" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="D55" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="E55" s="11" t="s">
-        <v>112</v>
-      </c>
       <c r="F55" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G55" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H55" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I55" s="17"/>
     </row>
-    <row r="56" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A56" s="5">
         <v>55</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D56" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E56" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F56" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G56" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H56" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I56" s="17"/>
     </row>
-    <row r="57" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A57" s="5">
         <v>56</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C57" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="D57" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="E57" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="D57" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="E57" s="11" t="s">
-        <v>119</v>
-      </c>
       <c r="F57" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G57" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H57" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I57" s="17"/>
     </row>
-    <row r="58" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A58" s="5">
         <v>57</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F58" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G58" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H58" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I58" s="17"/>
     </row>
-    <row r="59" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A59" s="5">
         <v>58</v>
       </c>
       <c r="B59" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D59" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E59" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F59" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G59" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H59" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I59" s="17"/>
     </row>
-    <row r="60" spans="1:9" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="150.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="5">
         <v>59</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D60" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E60" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F60" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G60" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H60" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I60" s="17"/>
     </row>
-    <row r="61" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A61" s="5">
         <v>60</v>
       </c>
       <c r="B61" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E61" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F61" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G61" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H61" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I61" s="17"/>
     </row>
-    <row r="62" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A62" s="5">
         <v>61</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E62" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F62" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G62" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H62" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I62" s="17"/>
     </row>
-    <row r="63" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A63" s="5">
         <v>62</v>
       </c>
       <c r="B63" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D63" s="11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E63" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F63" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G63" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H63" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I63" s="17"/>
     </row>
-    <row r="64" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A64" s="5">
         <v>63</v>
       </c>
       <c r="B64" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D64" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E64" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F64" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G64" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H64" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I64" s="17"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="5">
         <v>64</v>
       </c>
@@ -3020,7 +3283,7 @@
       <c r="H65" s="11"/>
       <c r="I65" s="17"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="5">
         <v>65</v>
       </c>
@@ -3033,7 +3296,7 @@
       <c r="H66" s="13"/>
       <c r="I66" s="17"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="5">
         <v>66</v>
       </c>
@@ -3046,7 +3309,7 @@
       <c r="H67" s="17"/>
       <c r="I67" s="17"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="5">
         <v>67</v>
       </c>
@@ -3059,7 +3322,7 @@
       <c r="H68" s="17"/>
       <c r="I68" s="17"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="5">
         <v>68</v>
       </c>
@@ -3072,7 +3335,7 @@
       <c r="H69" s="17"/>
       <c r="I69" s="17"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="5">
         <v>69</v>
       </c>
@@ -3085,7 +3348,7 @@
       <c r="H70" s="17"/>
       <c r="I70" s="17"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="5">
         <v>70</v>
       </c>
@@ -3098,7 +3361,7 @@
       <c r="H71" s="17"/>
       <c r="I71" s="17"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="5">
         <v>71</v>
       </c>
@@ -3111,7 +3374,7 @@
       <c r="H72" s="17"/>
       <c r="I72" s="17"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="5">
         <v>72</v>
       </c>
@@ -3124,7 +3387,7 @@
       <c r="H73" s="17"/>
       <c r="I73" s="17"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="5">
         <v>73</v>
       </c>
@@ -3137,7 +3400,7 @@
       <c r="H74" s="17"/>
       <c r="I74" s="17"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="5">
         <v>74</v>
       </c>
@@ -3150,7 +3413,7 @@
       <c r="H75" s="17"/>
       <c r="I75" s="17"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="5">
         <v>75</v>
       </c>
@@ -3163,7 +3426,7 @@
       <c r="H76" s="17"/>
       <c r="I76" s="17"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="5">
         <v>76</v>
       </c>
@@ -3176,7 +3439,7 @@
       <c r="H77" s="17"/>
       <c r="I77" s="17"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="5">
         <v>77</v>
       </c>
@@ -3189,7 +3452,7 @@
       <c r="H78" s="17"/>
       <c r="I78" s="17"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="5">
         <v>78</v>
       </c>
@@ -3202,7 +3465,7 @@
       <c r="H79" s="17"/>
       <c r="I79" s="17"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="5">
         <v>79</v>
       </c>
@@ -3215,7 +3478,7 @@
       <c r="H80" s="17"/>
       <c r="I80" s="17"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="5">
         <v>80</v>
       </c>
@@ -3228,7 +3491,7 @@
       <c r="H81" s="17"/>
       <c r="I81" s="17"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" s="5">
         <v>81</v>
       </c>
@@ -3241,7 +3504,7 @@
       <c r="H82" s="17"/>
       <c r="I82" s="17"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="5">
         <v>82</v>
       </c>
@@ -3254,7 +3517,7 @@
       <c r="H83" s="17"/>
       <c r="I83" s="17"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="5">
         <v>83</v>
       </c>
@@ -3267,7 +3530,7 @@
       <c r="H84" s="17"/>
       <c r="I84" s="17"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="5">
         <v>84</v>
       </c>
@@ -3280,7 +3543,7 @@
       <c r="H85" s="17"/>
       <c r="I85" s="17"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="5">
         <v>85</v>
       </c>
@@ -3293,7 +3556,7 @@
       <c r="H86" s="17"/>
       <c r="I86" s="17"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="5">
         <v>86</v>
       </c>
@@ -3306,7 +3569,7 @@
       <c r="H87" s="17"/>
       <c r="I87" s="17"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="5">
         <v>87</v>
       </c>
@@ -3319,7 +3582,7 @@
       <c r="H88" s="17"/>
       <c r="I88" s="17"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="5">
         <v>88</v>
       </c>
@@ -3332,7 +3595,7 @@
       <c r="H89" s="17"/>
       <c r="I89" s="17"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" s="5">
         <v>89</v>
       </c>
@@ -3345,7 +3608,7 @@
       <c r="H90" s="17"/>
       <c r="I90" s="17"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" s="5">
         <v>90</v>
       </c>
@@ -3358,7 +3621,7 @@
       <c r="H91" s="17"/>
       <c r="I91" s="17"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" s="5">
         <v>91</v>
       </c>
@@ -3371,7 +3634,7 @@
       <c r="H92" s="17"/>
       <c r="I92" s="17"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" s="5">
         <v>92</v>
       </c>
@@ -3384,7 +3647,7 @@
       <c r="H93" s="17"/>
       <c r="I93" s="17"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" s="5">
         <v>93</v>
       </c>
@@ -3397,7 +3660,7 @@
       <c r="H94" s="17"/>
       <c r="I94" s="17"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" s="5">
         <v>94</v>
       </c>
@@ -3410,7 +3673,7 @@
       <c r="H95" s="17"/>
       <c r="I95" s="17"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" s="5">
         <v>95</v>
       </c>
@@ -3423,7 +3686,7 @@
       <c r="H96" s="17"/>
       <c r="I96" s="17"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" s="5">
         <v>96</v>
       </c>
@@ -3436,7 +3699,7 @@
       <c r="H97" s="17"/>
       <c r="I97" s="17"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" s="5">
         <v>97</v>
       </c>
@@ -3449,7 +3712,7 @@
       <c r="H98" s="17"/>
       <c r="I98" s="17"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" s="5">
         <v>98</v>
       </c>
@@ -3462,7 +3725,7 @@
       <c r="H99" s="17"/>
       <c r="I99" s="17"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" s="5">
         <v>99</v>
       </c>
@@ -3475,7 +3738,7 @@
       <c r="H100" s="17"/>
       <c r="I100" s="17"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" s="5">
         <v>100</v>
       </c>
@@ -3488,7 +3751,7 @@
       <c r="H101" s="17"/>
       <c r="I101" s="17"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" s="5">
         <v>101</v>
       </c>
@@ -3501,7 +3764,7 @@
       <c r="H102" s="17"/>
       <c r="I102" s="17"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" s="5">
         <v>102</v>
       </c>
@@ -3514,7 +3777,7 @@
       <c r="H103" s="17"/>
       <c r="I103" s="17"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" s="5">
         <v>103</v>
       </c>
@@ -3527,7 +3790,7 @@
       <c r="H104" s="17"/>
       <c r="I104" s="17"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" s="5">
         <v>104</v>
       </c>
@@ -3540,7 +3803,7 @@
       <c r="H105" s="17"/>
       <c r="I105" s="17"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" s="5">
         <v>105</v>
       </c>
@@ -3554,12 +3817,12 @@
       <c r="I106" s="17"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3575,4 +3838,2045 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5155472-66AF-4323-ACD5-D08CB3B87B8B}">
+  <dimension ref="A1:I98"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B63" sqref="B63"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7" customWidth="1"/>
+    <col min="2" max="2" width="16.21875" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" customWidth="1"/>
+    <col min="4" max="4" width="35.77734375" customWidth="1"/>
+    <col min="5" max="5" width="27.77734375" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
+    <col min="7" max="7" width="17.88671875" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" customWidth="1"/>
+    <col min="9" max="9" width="19.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="15"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="15"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="15"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="15"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="15"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+    </row>
+    <row r="10" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+    </row>
+    <row r="13" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="5">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="5">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+    </row>
+    <row r="18" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="5">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+    </row>
+    <row r="19" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="5">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+    </row>
+    <row r="20" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="5">
+        <v>19</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+    </row>
+    <row r="21" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="5">
+        <v>20</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+    </row>
+    <row r="22" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A22" s="5">
+        <v>21</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+    </row>
+    <row r="23" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A23" s="5">
+        <v>22</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+    </row>
+    <row r="24" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="5">
+        <v>23</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+    </row>
+    <row r="25" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A25" s="5">
+        <v>24</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+    </row>
+    <row r="26" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A26" s="5">
+        <v>25</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="G26" s="5"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+    </row>
+    <row r="27" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="5">
+        <v>26</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+    </row>
+    <row r="28" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="5">
+        <v>27</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="4"/>
+    </row>
+    <row r="29" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="5">
+        <v>28</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="4"/>
+    </row>
+    <row r="30" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="5">
+        <v>29</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="4"/>
+    </row>
+    <row r="31" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="5">
+        <v>30</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="4"/>
+    </row>
+    <row r="32" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="5">
+        <v>31</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="4"/>
+    </row>
+    <row r="33" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="5">
+        <v>32</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="4"/>
+    </row>
+    <row r="34" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="5">
+        <v>33</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="4"/>
+    </row>
+    <row r="35" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="5">
+        <v>34</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="4"/>
+    </row>
+    <row r="36" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="5">
+        <v>35</v>
+      </c>
+      <c r="B36" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="4"/>
+    </row>
+    <row r="37" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="5">
+        <v>36</v>
+      </c>
+      <c r="B37" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="F37" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="4"/>
+    </row>
+    <row r="38" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="5">
+        <v>37</v>
+      </c>
+      <c r="B38" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="4"/>
+    </row>
+    <row r="39" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="5">
+        <v>38</v>
+      </c>
+      <c r="B39" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="F39" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="4"/>
+    </row>
+    <row r="40" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="5">
+        <v>39</v>
+      </c>
+      <c r="B40" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="4"/>
+    </row>
+    <row r="41" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="5">
+        <v>40</v>
+      </c>
+      <c r="B41" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="D41" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="F41" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="16"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" s="5">
+        <v>41</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="E42" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="F42" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="17"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" s="5">
+        <v>42</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="E43" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="F43" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="17"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" s="5">
+        <v>43</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="E44" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="F44" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="G44" s="14"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="17"/>
+    </row>
+    <row r="45" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="5">
+        <v>44</v>
+      </c>
+      <c r="B45" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="E45" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="F45" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="G45" s="11"/>
+      <c r="H45" s="14"/>
+      <c r="I45" s="17"/>
+    </row>
+    <row r="46" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="5">
+        <v>45</v>
+      </c>
+      <c r="B46" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="F46" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="17"/>
+    </row>
+    <row r="47" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A47" s="5">
+        <v>46</v>
+      </c>
+      <c r="B47" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D47" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="F47" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="17"/>
+    </row>
+    <row r="48" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A48" s="5">
+        <v>47</v>
+      </c>
+      <c r="B48" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="D48" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="E48" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F48" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="17"/>
+    </row>
+    <row r="49" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A49" s="5">
+        <v>48</v>
+      </c>
+      <c r="B49" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="D49" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="E49" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="F49" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="17"/>
+    </row>
+    <row r="50" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A50" s="5">
+        <v>49</v>
+      </c>
+      <c r="B50" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D50" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="E50" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="F50" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="17"/>
+    </row>
+    <row r="51" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A51" s="5">
+        <v>50</v>
+      </c>
+      <c r="B51" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D51" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="E51" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="F51" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="17"/>
+    </row>
+    <row r="52" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A52" s="5">
+        <v>51</v>
+      </c>
+      <c r="B52" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D52" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="E52" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="F52" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="G52" s="11"/>
+      <c r="H52" s="11"/>
+      <c r="I52" s="17"/>
+    </row>
+    <row r="53" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A53" s="5">
+        <v>52</v>
+      </c>
+      <c r="B53" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D53" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="E53" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="F53" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="G53" s="11"/>
+      <c r="H53" s="11"/>
+      <c r="I53" s="17"/>
+    </row>
+    <row r="54" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A54" s="5">
+        <v>53</v>
+      </c>
+      <c r="B54" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="C54" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D54" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="E54" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="F54" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="G54" s="11"/>
+      <c r="H54" s="11"/>
+      <c r="I54" s="17"/>
+    </row>
+    <row r="55" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A55" s="5">
+        <v>54</v>
+      </c>
+      <c r="B55" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D55" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="E55" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="F55" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="G55" s="11"/>
+      <c r="H55" s="11"/>
+      <c r="I55" s="17"/>
+    </row>
+    <row r="56" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A56" s="5">
+        <v>55</v>
+      </c>
+      <c r="B56" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D56" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="E56" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="F56" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="G56" s="11"/>
+      <c r="H56" s="11"/>
+      <c r="I56" s="17"/>
+    </row>
+    <row r="57" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A57" s="5">
+        <v>56</v>
+      </c>
+      <c r="B57" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="C57" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="D57" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="E57" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="F57" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="G57" s="11"/>
+      <c r="H57" s="11"/>
+      <c r="I57" s="17"/>
+    </row>
+    <row r="58" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A58" s="5">
+        <v>57</v>
+      </c>
+      <c r="B58" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="C58" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="D58" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="E58" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="F58" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="G58" s="11"/>
+      <c r="H58" s="13"/>
+      <c r="I58" s="17"/>
+    </row>
+    <row r="59" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A59" s="5">
+        <v>58</v>
+      </c>
+      <c r="B59" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="C59" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="D59" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="E59" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="F59" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="G59" s="17"/>
+      <c r="H59" s="17"/>
+      <c r="I59" s="17"/>
+    </row>
+    <row r="60" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A60" s="5">
+        <v>59</v>
+      </c>
+      <c r="B60" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="C60" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="D60" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="E60" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="F60" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="G60" s="17"/>
+      <c r="H60" s="17"/>
+      <c r="I60" s="17"/>
+    </row>
+    <row r="61" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A61" s="5">
+        <v>60</v>
+      </c>
+      <c r="B61" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="C61" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="D61" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="E61" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="F61" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="G61" s="17"/>
+      <c r="H61" s="17"/>
+      <c r="I61" s="17"/>
+    </row>
+    <row r="62" spans="1:9" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="5">
+        <v>61</v>
+      </c>
+      <c r="B62" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="C62" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="D62" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="E62" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="F62" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="G62" s="17"/>
+      <c r="H62" s="17"/>
+      <c r="I62" s="17"/>
+    </row>
+    <row r="63" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A63" s="5">
+        <v>62</v>
+      </c>
+      <c r="B63" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="C63" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="D63" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="E63" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="F63" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="G63" s="17"/>
+      <c r="H63" s="17"/>
+      <c r="I63" s="17"/>
+    </row>
+    <row r="64" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A64" s="5">
+        <v>63</v>
+      </c>
+      <c r="B64" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="C64" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="D64" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="E64" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="F64" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="G64" s="17"/>
+      <c r="H64" s="17"/>
+      <c r="I64" s="17"/>
+    </row>
+    <row r="65" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A65" s="5">
+        <v>64</v>
+      </c>
+      <c r="B65" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="C65" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="D65" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="E65" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="F65" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="G65" s="17"/>
+      <c r="H65" s="17"/>
+      <c r="I65" s="17"/>
+    </row>
+    <row r="66" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A66" s="5">
+        <v>65</v>
+      </c>
+      <c r="B66" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="C66" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="D66" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="E66" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="F66" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="G66" s="17"/>
+      <c r="H66" s="17"/>
+      <c r="I66" s="17"/>
+    </row>
+    <row r="67" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A67" s="5">
+        <v>66</v>
+      </c>
+      <c r="B67" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="C67" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="D67" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="E67" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="F67" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="G67" s="17"/>
+      <c r="H67" s="17"/>
+      <c r="I67" s="17"/>
+    </row>
+    <row r="68" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A68" s="5">
+        <v>67</v>
+      </c>
+      <c r="B68" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="C68" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="D68" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="E68" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="F68" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="G68" s="17"/>
+      <c r="H68" s="17"/>
+      <c r="I68" s="17"/>
+    </row>
+    <row r="69" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A69" s="5">
+        <v>68</v>
+      </c>
+      <c r="B69" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="C69" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="D69" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="E69" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="F69" s="17" t="s">
+        <v>216</v>
+      </c>
+      <c r="G69" s="17"/>
+      <c r="H69" s="17"/>
+      <c r="I69" s="17"/>
+    </row>
+    <row r="70" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A70" s="5">
+        <v>69</v>
+      </c>
+      <c r="B70" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="C70" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="D70" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="E70" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="F70" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="G70" s="17"/>
+      <c r="H70" s="17"/>
+      <c r="I70" s="17"/>
+    </row>
+    <row r="71" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A71" s="5">
+        <v>70</v>
+      </c>
+      <c r="B71" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="C71" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="D71" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="E71" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="F71" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="G71" s="17"/>
+      <c r="H71" s="17"/>
+      <c r="I71" s="17"/>
+    </row>
+    <row r="72" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A72" s="5">
+        <v>71</v>
+      </c>
+      <c r="B72" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="C72" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="D72" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="F72" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="G72" s="17"/>
+      <c r="H72" s="17"/>
+      <c r="I72" s="17"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A73" s="5">
+        <v>72</v>
+      </c>
+      <c r="B73" s="17"/>
+      <c r="C73" s="17"/>
+      <c r="D73" s="17"/>
+      <c r="E73" s="17"/>
+      <c r="F73" s="17"/>
+      <c r="G73" s="17"/>
+      <c r="H73" s="17"/>
+      <c r="I73" s="17"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A74" s="5">
+        <v>73</v>
+      </c>
+      <c r="B74" s="17"/>
+      <c r="C74" s="17"/>
+      <c r="D74" s="17"/>
+      <c r="E74" s="17"/>
+      <c r="F74" s="17"/>
+      <c r="G74" s="17"/>
+      <c r="H74" s="17"/>
+      <c r="I74" s="17"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A75" s="5">
+        <v>74</v>
+      </c>
+      <c r="B75" s="17"/>
+      <c r="C75" s="17"/>
+      <c r="D75" s="17"/>
+      <c r="E75" s="17"/>
+      <c r="F75" s="17"/>
+      <c r="G75" s="17"/>
+      <c r="H75" s="17"/>
+      <c r="I75" s="17"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A76" s="5">
+        <v>75</v>
+      </c>
+      <c r="B76" s="17"/>
+      <c r="C76" s="17"/>
+      <c r="D76" s="17"/>
+      <c r="E76" s="17"/>
+      <c r="F76" s="17"/>
+      <c r="G76" s="17"/>
+      <c r="H76" s="17"/>
+      <c r="I76" s="17"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A77" s="5">
+        <v>76</v>
+      </c>
+      <c r="B77" s="17"/>
+      <c r="C77" s="17"/>
+      <c r="D77" s="17"/>
+      <c r="E77" s="17"/>
+      <c r="F77" s="17"/>
+      <c r="G77" s="17"/>
+      <c r="H77" s="17"/>
+      <c r="I77" s="17"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A78" s="5">
+        <v>77</v>
+      </c>
+      <c r="B78" s="17"/>
+      <c r="C78" s="17"/>
+      <c r="D78" s="17"/>
+      <c r="E78" s="17"/>
+      <c r="F78" s="17"/>
+      <c r="G78" s="17"/>
+      <c r="H78" s="17"/>
+      <c r="I78" s="17"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A79" s="5">
+        <v>78</v>
+      </c>
+      <c r="B79" s="17"/>
+      <c r="C79" s="17"/>
+      <c r="D79" s="17"/>
+      <c r="E79" s="17"/>
+      <c r="F79" s="17"/>
+      <c r="G79" s="17"/>
+      <c r="H79" s="17"/>
+      <c r="I79" s="17"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A80" s="5">
+        <v>79</v>
+      </c>
+      <c r="B80" s="17"/>
+      <c r="C80" s="17"/>
+      <c r="D80" s="17"/>
+      <c r="E80" s="17"/>
+      <c r="F80" s="17"/>
+      <c r="G80" s="17"/>
+      <c r="H80" s="17"/>
+      <c r="I80" s="17"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A81" s="5">
+        <v>80</v>
+      </c>
+      <c r="B81" s="17"/>
+      <c r="C81" s="17"/>
+      <c r="D81" s="17"/>
+      <c r="E81" s="17"/>
+      <c r="F81" s="17"/>
+      <c r="G81" s="17"/>
+      <c r="H81" s="17"/>
+      <c r="I81" s="17"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A82" s="5">
+        <v>81</v>
+      </c>
+      <c r="B82" s="17"/>
+      <c r="C82" s="17"/>
+      <c r="D82" s="17"/>
+      <c r="E82" s="17"/>
+      <c r="F82" s="17"/>
+      <c r="G82" s="17"/>
+      <c r="H82" s="17"/>
+      <c r="I82" s="17"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A83" s="5">
+        <v>82</v>
+      </c>
+      <c r="B83" s="17"/>
+      <c r="C83" s="17"/>
+      <c r="D83" s="17"/>
+      <c r="E83" s="17"/>
+      <c r="F83" s="17"/>
+      <c r="G83" s="17"/>
+      <c r="H83" s="17"/>
+      <c r="I83" s="17"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A84" s="5">
+        <v>83</v>
+      </c>
+      <c r="B84" s="17"/>
+      <c r="C84" s="17"/>
+      <c r="D84" s="17"/>
+      <c r="E84" s="17"/>
+      <c r="F84" s="17"/>
+      <c r="G84" s="17"/>
+      <c r="H84" s="17"/>
+      <c r="I84" s="17"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A85" s="5">
+        <v>84</v>
+      </c>
+      <c r="B85" s="17"/>
+      <c r="C85" s="17"/>
+      <c r="D85" s="17"/>
+      <c r="E85" s="17"/>
+      <c r="F85" s="17"/>
+      <c r="G85" s="17"/>
+      <c r="H85" s="17"/>
+      <c r="I85" s="17"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A86" s="5">
+        <v>85</v>
+      </c>
+      <c r="B86" s="17"/>
+      <c r="C86" s="17"/>
+      <c r="D86" s="17"/>
+      <c r="E86" s="17"/>
+      <c r="F86" s="17"/>
+      <c r="G86" s="17"/>
+      <c r="H86" s="17"/>
+      <c r="I86" s="17"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A87" s="5">
+        <v>86</v>
+      </c>
+      <c r="B87" s="17"/>
+      <c r="C87" s="17"/>
+      <c r="D87" s="17"/>
+      <c r="E87" s="17"/>
+      <c r="F87" s="17"/>
+      <c r="G87" s="17"/>
+      <c r="H87" s="17"/>
+      <c r="I87" s="17"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A88" s="5">
+        <v>87</v>
+      </c>
+      <c r="B88" s="17"/>
+      <c r="C88" s="17"/>
+      <c r="D88" s="17"/>
+      <c r="E88" s="17"/>
+      <c r="F88" s="17"/>
+      <c r="G88" s="17"/>
+      <c r="H88" s="17"/>
+      <c r="I88" s="17"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A89" s="5">
+        <v>88</v>
+      </c>
+      <c r="B89" s="17"/>
+      <c r="C89" s="17"/>
+      <c r="D89" s="17"/>
+      <c r="E89" s="17"/>
+      <c r="F89" s="17"/>
+      <c r="G89" s="17"/>
+      <c r="H89" s="17"/>
+      <c r="I89" s="17"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A90" s="5">
+        <v>89</v>
+      </c>
+      <c r="B90" s="17"/>
+      <c r="C90" s="17"/>
+      <c r="D90" s="17"/>
+      <c r="E90" s="17"/>
+      <c r="F90" s="17"/>
+      <c r="G90" s="17"/>
+      <c r="H90" s="17"/>
+      <c r="I90" s="17"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A91" s="5">
+        <v>90</v>
+      </c>
+      <c r="B91" s="17"/>
+      <c r="C91" s="17"/>
+      <c r="D91" s="17"/>
+      <c r="E91" s="17"/>
+      <c r="F91" s="17"/>
+      <c r="G91" s="17"/>
+      <c r="H91" s="17"/>
+      <c r="I91" s="17"/>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A92" s="5">
+        <v>91</v>
+      </c>
+      <c r="B92" s="17"/>
+      <c r="C92" s="17"/>
+      <c r="D92" s="17"/>
+      <c r="E92" s="17"/>
+      <c r="F92" s="17"/>
+      <c r="G92" s="17"/>
+      <c r="H92" s="17"/>
+      <c r="I92" s="17"/>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A93" s="5">
+        <v>92</v>
+      </c>
+      <c r="B93" s="17"/>
+      <c r="C93" s="17"/>
+      <c r="D93" s="17"/>
+      <c r="E93" s="17"/>
+      <c r="F93" s="17"/>
+      <c r="G93" s="17"/>
+      <c r="H93" s="17"/>
+      <c r="I93" s="17"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A94" s="5">
+        <v>93</v>
+      </c>
+      <c r="B94" s="17"/>
+      <c r="C94" s="17"/>
+      <c r="D94" s="17"/>
+      <c r="E94" s="17"/>
+      <c r="F94" s="17"/>
+      <c r="G94" s="17"/>
+      <c r="H94" s="17"/>
+      <c r="I94" s="17"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A95" s="5">
+        <v>94</v>
+      </c>
+      <c r="B95" s="17"/>
+      <c r="C95" s="17"/>
+      <c r="D95" s="17"/>
+      <c r="E95" s="17"/>
+      <c r="F95" s="17"/>
+      <c r="G95" s="17"/>
+      <c r="H95" s="17"/>
+      <c r="I95" s="17"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A96" s="5">
+        <v>95</v>
+      </c>
+      <c r="B96" s="17"/>
+      <c r="C96" s="17"/>
+      <c r="D96" s="17"/>
+      <c r="E96" s="17"/>
+      <c r="F96" s="17"/>
+      <c r="G96" s="17"/>
+      <c r="H96" s="17"/>
+      <c r="I96" s="17"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A97" s="5">
+        <v>96</v>
+      </c>
+      <c r="B97" s="17"/>
+      <c r="C97" s="17"/>
+      <c r="D97" s="17"/>
+      <c r="E97" s="17"/>
+      <c r="F97" s="17"/>
+      <c r="G97" s="17"/>
+      <c r="H97" s="17"/>
+      <c r="I97" s="17"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A98" s="5">
+        <v>97</v>
+      </c>
+      <c r="B98" s="17"/>
+      <c r="C98" s="17"/>
+      <c r="D98" s="17"/>
+      <c r="E98" s="17"/>
+      <c r="F98" s="17"/>
+      <c r="G98" s="17"/>
+      <c r="H98" s="17"/>
+      <c r="I98" s="17"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1" xr:uid="{6F6142C4-D9FC-4FFF-ABCD-0B9CD32F1EFD}">
+      <formula1>"Pass,Fail"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
testing for update schedule functionality
</commit_message>
<xml_diff>
--- a/testing/Team eXi Test Cases.xlsx
+++ b/testing/Team eXi Test Cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DEYU\Documents\YR3 Term1\Thriving-Stones-Project\testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HuiXin\Documents\FYP\Thriving-Stones-Project\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BF828B0B-EF2F-4FDC-A23E-400758C1A437}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B37B021D-402E-4FD3-A61D-89F43547F352}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="36" windowWidth="25752" windowHeight="11592" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="40" windowWidth="25750" windowHeight="11590" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 2" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="249">
   <si>
     <t>S/N</t>
   </si>
@@ -909,21 +909,112 @@
     <t>Update Schedule</t>
   </si>
   <si>
-    <t>Able to update the</t>
-  </si>
-  <si>
-    <t>Click Edit Icon on specific time and change date time</t>
-  </si>
-  <si>
     <t>Update schedule successfully</t>
   </si>
   <si>
+    <t>Create Grade</t>
+  </si>
+  <si>
+    <t>Able to update schedule with all the correct input fields</t>
+  </si>
+  <si>
+    <t>Unable to update schedule with unselected subject field</t>
+  </si>
+  <si>
+    <t>Failure to update schedule with error message "Please select Subject" displayed</t>
+  </si>
+  <si>
+    <t>Unable to update schedule with unselected level field</t>
+  </si>
+  <si>
+    <t>Failure to update schedule with error message "Please select Level" displayed</t>
+  </si>
+  <si>
     <t>Subject: English
-Level: P4
-Time: 8:30-10:00 23 Aug 1018</t>
-  </si>
-  <si>
-    <t>Create Grade</t>
+Level: P1
+Day: Mon
+Start Time: 12
+End Time: 2
+Tutor Assigned: Irene</t>
+  </si>
+  <si>
+    <t>Subject: 
+Level: P1
+Day: Mon
+Start Time: 12
+End Time: 2
+Tutor Assigned: Irene</t>
+  </si>
+  <si>
+    <t>Subject: English
+Level: 
+Day: Mon
+Start Time: 12
+End Time: 2
+Tutor Assigned: Irene</t>
+  </si>
+  <si>
+    <t>Unable to update schedule with unselected day field</t>
+  </si>
+  <si>
+    <t>Subject: English
+Level: P1
+Day:
+Start Time: 12
+End Time: 2
+Tutor Assigned: Irene</t>
+  </si>
+  <si>
+    <t>Unable to update schedule with unselected start time field</t>
+  </si>
+  <si>
+    <t>Subject: English
+Level: P1
+Day: Mon
+Start Time: 
+End Time: 2
+Tutor Assigned: Irene</t>
+  </si>
+  <si>
+    <t>Unable to update schedule with unselected end time field</t>
+  </si>
+  <si>
+    <t>Subject: English
+Level: P1
+Day: Mon
+Start Time: 12 
+End Time: 
+Tutor Assigned: Irene</t>
+  </si>
+  <si>
+    <t>Select the corresponding fields into the form and click update schedule</t>
+  </si>
+  <si>
+    <t>Failure to update schedule with error message "Please select day" displayed</t>
+  </si>
+  <si>
+    <t>Failure to update schedule with error message "Please select start time" displayed</t>
+  </si>
+  <si>
+    <t>Failure to update schedule with error message "Please select end time" displayed</t>
+  </si>
+  <si>
+    <t>Schedule updated successfully</t>
+  </si>
+  <si>
+    <t>Error message "Please select subject displayed"</t>
+  </si>
+  <si>
+    <t>Error message "Please select level displayed"</t>
+  </si>
+  <si>
+    <t>Error message "Please select day displayed"</t>
+  </si>
+  <si>
+    <t>Error message "Please select start time displayed"</t>
+  </si>
+  <si>
+    <t>Error message "Please select end time displayed"</t>
   </si>
 </sst>
 </file>
@@ -1173,27 +1264,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1547,20 +1618,20 @@
   <dimension ref="A1:Z106"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1:I1"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="26.6640625" customWidth="1"/>
+    <col min="2" max="2" width="26.6328125" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="29.109375" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="29.08984375" customWidth="1"/>
+    <col min="5" max="5" width="19.54296875" customWidth="1"/>
+    <col min="6" max="6" width="16.36328125" customWidth="1"/>
+    <col min="7" max="7" width="13.36328125" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="23.6640625" customWidth="1"/>
+    <col min="9" max="9" width="23.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -1609,7 +1680,7 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1632,7 +1703,7 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1655,7 +1726,7 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1678,7 +1749,7 @@
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1701,7 +1772,7 @@
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1724,7 +1795,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1747,7 +1818,7 @@
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -1770,7 +1841,7 @@
       <c r="H8" s="16"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -1793,7 +1864,7 @@
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="1:26" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1816,7 +1887,7 @@
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" spans="1:26" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1839,7 +1910,7 @@
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
     </row>
-    <row r="12" spans="1:26" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -1862,7 +1933,7 @@
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" ht="58" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1885,7 +1956,7 @@
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" ht="58" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1908,7 +1979,7 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" ht="58" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1931,7 +2002,7 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:26" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1954,7 +2025,7 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1977,7 +2048,7 @@
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -2000,7 +2071,7 @@
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
     </row>
-    <row r="19" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -2029,7 +2100,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -2058,7 +2129,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -2087,7 +2158,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -2116,7 +2187,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -2145,7 +2216,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -2174,7 +2245,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -2203,7 +2274,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -2232,7 +2303,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -2261,7 +2332,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -2290,7 +2361,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -2319,7 +2390,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -2348,7 +2419,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -2377,7 +2448,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -2404,7 +2475,7 @@
       </c>
       <c r="I32" s="4"/>
     </row>
-    <row r="33" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -2431,7 +2502,7 @@
       </c>
       <c r="I33" s="4"/>
     </row>
-    <row r="34" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -2458,7 +2529,7 @@
       </c>
       <c r="I34" s="4"/>
     </row>
-    <row r="35" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -2487,7 +2558,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -2514,7 +2585,7 @@
       </c>
       <c r="I36" s="4"/>
     </row>
-    <row r="37" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -2541,7 +2612,7 @@
       </c>
       <c r="I37" s="4"/>
     </row>
-    <row r="38" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -2568,7 +2639,7 @@
       </c>
       <c r="I38" s="4"/>
     </row>
-    <row r="39" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -2595,7 +2666,7 @@
       </c>
       <c r="I39" s="4"/>
     </row>
-    <row r="40" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -2622,7 +2693,7 @@
       </c>
       <c r="I40" s="4"/>
     </row>
-    <row r="41" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -2649,7 +2720,7 @@
       </c>
       <c r="I41" s="4"/>
     </row>
-    <row r="42" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -2676,7 +2747,7 @@
       </c>
       <c r="I42" s="4"/>
     </row>
-    <row r="43" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -2703,7 +2774,7 @@
       </c>
       <c r="I43" s="4"/>
     </row>
-    <row r="44" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -2730,7 +2801,7 @@
       </c>
       <c r="I44" s="4"/>
     </row>
-    <row r="45" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -2757,7 +2828,7 @@
       </c>
       <c r="I45" s="4"/>
     </row>
-    <row r="46" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -2784,7 +2855,7 @@
       </c>
       <c r="I46" s="4"/>
     </row>
-    <row r="47" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -2811,7 +2882,7 @@
       </c>
       <c r="I47" s="4"/>
     </row>
-    <row r="48" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -2838,7 +2909,7 @@
       </c>
       <c r="I48" s="4"/>
     </row>
-    <row r="49" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -2865,7 +2936,7 @@
       </c>
       <c r="I49" s="16"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -2892,7 +2963,7 @@
       </c>
       <c r="I50" s="17"/>
     </row>
-    <row r="51" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -2919,7 +2990,7 @@
       </c>
       <c r="I51" s="17"/>
     </row>
-    <row r="52" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -2946,7 +3017,7 @@
       </c>
       <c r="I52" s="17"/>
     </row>
-    <row r="53" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -2973,7 +3044,7 @@
       </c>
       <c r="I53" s="17"/>
     </row>
-    <row r="54" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -3000,7 +3071,7 @@
       </c>
       <c r="I54" s="17"/>
     </row>
-    <row r="55" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -3027,7 +3098,7 @@
       </c>
       <c r="I55" s="17"/>
     </row>
-    <row r="56" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A56" s="5">
         <v>55</v>
       </c>
@@ -3054,7 +3125,7 @@
       </c>
       <c r="I56" s="17"/>
     </row>
-    <row r="57" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A57" s="5">
         <v>56</v>
       </c>
@@ -3081,7 +3152,7 @@
       </c>
       <c r="I57" s="17"/>
     </row>
-    <row r="58" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A58" s="5">
         <v>57</v>
       </c>
@@ -3108,7 +3179,7 @@
       </c>
       <c r="I58" s="17"/>
     </row>
-    <row r="59" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
         <v>58</v>
       </c>
@@ -3135,7 +3206,7 @@
       </c>
       <c r="I59" s="17"/>
     </row>
-    <row r="60" spans="1:9" ht="150.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" ht="150.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="5">
         <v>59</v>
       </c>
@@ -3162,7 +3233,7 @@
       </c>
       <c r="I60" s="17"/>
     </row>
-    <row r="61" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A61" s="5">
         <v>60</v>
       </c>
@@ -3189,7 +3260,7 @@
       </c>
       <c r="I61" s="17"/>
     </row>
-    <row r="62" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A62" s="5">
         <v>61</v>
       </c>
@@ -3216,7 +3287,7 @@
       </c>
       <c r="I62" s="17"/>
     </row>
-    <row r="63" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A63" s="5">
         <v>62</v>
       </c>
@@ -3243,7 +3314,7 @@
       </c>
       <c r="I63" s="17"/>
     </row>
-    <row r="64" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A64" s="5">
         <v>63</v>
       </c>
@@ -3270,7 +3341,7 @@
       </c>
       <c r="I64" s="17"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" s="5">
         <v>64</v>
       </c>
@@ -3283,7 +3354,7 @@
       <c r="H65" s="11"/>
       <c r="I65" s="17"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" s="5">
         <v>65</v>
       </c>
@@ -3296,7 +3367,7 @@
       <c r="H66" s="13"/>
       <c r="I66" s="17"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" s="5">
         <v>66</v>
       </c>
@@ -3309,7 +3380,7 @@
       <c r="H67" s="17"/>
       <c r="I67" s="17"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" s="5">
         <v>67</v>
       </c>
@@ -3322,7 +3393,7 @@
       <c r="H68" s="17"/>
       <c r="I68" s="17"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" s="5">
         <v>68</v>
       </c>
@@ -3335,7 +3406,7 @@
       <c r="H69" s="17"/>
       <c r="I69" s="17"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" s="5">
         <v>69</v>
       </c>
@@ -3348,7 +3419,7 @@
       <c r="H70" s="17"/>
       <c r="I70" s="17"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" s="5">
         <v>70</v>
       </c>
@@ -3361,7 +3432,7 @@
       <c r="H71" s="17"/>
       <c r="I71" s="17"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" s="5">
         <v>71</v>
       </c>
@@ -3374,7 +3445,7 @@
       <c r="H72" s="17"/>
       <c r="I72" s="17"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" s="5">
         <v>72</v>
       </c>
@@ -3387,7 +3458,7 @@
       <c r="H73" s="17"/>
       <c r="I73" s="17"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" s="5">
         <v>73</v>
       </c>
@@ -3400,7 +3471,7 @@
       <c r="H74" s="17"/>
       <c r="I74" s="17"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" s="5">
         <v>74</v>
       </c>
@@ -3413,7 +3484,7 @@
       <c r="H75" s="17"/>
       <c r="I75" s="17"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" s="5">
         <v>75</v>
       </c>
@@ -3426,7 +3497,7 @@
       <c r="H76" s="17"/>
       <c r="I76" s="17"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" s="5">
         <v>76</v>
       </c>
@@ -3439,7 +3510,7 @@
       <c r="H77" s="17"/>
       <c r="I77" s="17"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" s="5">
         <v>77</v>
       </c>
@@ -3452,7 +3523,7 @@
       <c r="H78" s="17"/>
       <c r="I78" s="17"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" s="5">
         <v>78</v>
       </c>
@@ -3465,7 +3536,7 @@
       <c r="H79" s="17"/>
       <c r="I79" s="17"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" s="5">
         <v>79</v>
       </c>
@@ -3478,7 +3549,7 @@
       <c r="H80" s="17"/>
       <c r="I80" s="17"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" s="5">
         <v>80</v>
       </c>
@@ -3491,7 +3562,7 @@
       <c r="H81" s="17"/>
       <c r="I81" s="17"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" s="5">
         <v>81</v>
       </c>
@@ -3504,7 +3575,7 @@
       <c r="H82" s="17"/>
       <c r="I82" s="17"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" s="5">
         <v>82</v>
       </c>
@@ -3517,7 +3588,7 @@
       <c r="H83" s="17"/>
       <c r="I83" s="17"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84" s="5">
         <v>83</v>
       </c>
@@ -3530,7 +3601,7 @@
       <c r="H84" s="17"/>
       <c r="I84" s="17"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" s="5">
         <v>84</v>
       </c>
@@ -3543,7 +3614,7 @@
       <c r="H85" s="17"/>
       <c r="I85" s="17"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" s="5">
         <v>85</v>
       </c>
@@ -3556,7 +3627,7 @@
       <c r="H86" s="17"/>
       <c r="I86" s="17"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" s="5">
         <v>86</v>
       </c>
@@ -3569,7 +3640,7 @@
       <c r="H87" s="17"/>
       <c r="I87" s="17"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" s="5">
         <v>87</v>
       </c>
@@ -3582,7 +3653,7 @@
       <c r="H88" s="17"/>
       <c r="I88" s="17"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" s="5">
         <v>88</v>
       </c>
@@ -3595,7 +3666,7 @@
       <c r="H89" s="17"/>
       <c r="I89" s="17"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" s="5">
         <v>89</v>
       </c>
@@ -3608,7 +3679,7 @@
       <c r="H90" s="17"/>
       <c r="I90" s="17"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" s="5">
         <v>90</v>
       </c>
@@ -3621,7 +3692,7 @@
       <c r="H91" s="17"/>
       <c r="I91" s="17"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" s="5">
         <v>91</v>
       </c>
@@ -3634,7 +3705,7 @@
       <c r="H92" s="17"/>
       <c r="I92" s="17"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" s="5">
         <v>92</v>
       </c>
@@ -3647,7 +3718,7 @@
       <c r="H93" s="17"/>
       <c r="I93" s="17"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" s="5">
         <v>93</v>
       </c>
@@ -3660,7 +3731,7 @@
       <c r="H94" s="17"/>
       <c r="I94" s="17"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" s="5">
         <v>94</v>
       </c>
@@ -3673,7 +3744,7 @@
       <c r="H95" s="17"/>
       <c r="I95" s="17"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" s="5">
         <v>95</v>
       </c>
@@ -3686,7 +3757,7 @@
       <c r="H96" s="17"/>
       <c r="I96" s="17"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97" s="5">
         <v>96</v>
       </c>
@@ -3699,7 +3770,7 @@
       <c r="H97" s="17"/>
       <c r="I97" s="17"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" s="5">
         <v>97</v>
       </c>
@@ -3712,7 +3783,7 @@
       <c r="H98" s="17"/>
       <c r="I98" s="17"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99" s="5">
         <v>98</v>
       </c>
@@ -3725,7 +3796,7 @@
       <c r="H99" s="17"/>
       <c r="I99" s="17"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A100" s="5">
         <v>99</v>
       </c>
@@ -3738,7 +3809,7 @@
       <c r="H100" s="17"/>
       <c r="I100" s="17"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A101" s="5">
         <v>100</v>
       </c>
@@ -3751,7 +3822,7 @@
       <c r="H101" s="17"/>
       <c r="I101" s="17"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A102" s="5">
         <v>101</v>
       </c>
@@ -3764,7 +3835,7 @@
       <c r="H102" s="17"/>
       <c r="I102" s="17"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A103" s="5">
         <v>102</v>
       </c>
@@ -3777,7 +3848,7 @@
       <c r="H103" s="17"/>
       <c r="I103" s="17"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A104" s="5">
         <v>103</v>
       </c>
@@ -3790,7 +3861,7 @@
       <c r="H104" s="17"/>
       <c r="I104" s="17"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A105" s="5">
         <v>104</v>
       </c>
@@ -3803,7 +3874,7 @@
       <c r="H105" s="17"/>
       <c r="I105" s="17"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A106" s="5">
         <v>105</v>
       </c>
@@ -3819,10 +3890,10 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3845,24 +3916,24 @@
   <dimension ref="A1:I98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B63" sqref="B63"/>
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H72" sqref="H72:H77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="2" width="16.21875" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" customWidth="1"/>
-    <col min="4" max="4" width="35.77734375" customWidth="1"/>
-    <col min="5" max="5" width="27.77734375" customWidth="1"/>
+    <col min="2" max="2" width="16.1796875" customWidth="1"/>
+    <col min="3" max="3" width="27.6328125" customWidth="1"/>
+    <col min="4" max="4" width="35.81640625" customWidth="1"/>
+    <col min="5" max="5" width="27.81640625" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
-    <col min="7" max="7" width="17.88671875" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" customWidth="1"/>
-    <col min="9" max="9" width="19.77734375" customWidth="1"/>
+    <col min="7" max="7" width="17.90625" customWidth="1"/>
+    <col min="8" max="8" width="10.36328125" customWidth="1"/>
+    <col min="9" max="9" width="19.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3891,7 +3962,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -3914,7 +3985,7 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -3937,7 +4008,7 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -3960,7 +4031,7 @@
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -3983,7 +4054,7 @@
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -4006,7 +4077,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -4029,7 +4100,7 @@
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -4052,7 +4123,7 @@
       <c r="H8" s="16"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -4075,7 +4146,7 @@
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -4098,7 +4169,7 @@
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -4121,7 +4192,7 @@
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
     </row>
-    <row r="12" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -4144,7 +4215,7 @@
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -4167,7 +4238,7 @@
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -4190,7 +4261,7 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -4213,7 +4284,7 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -4236,7 +4307,7 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -4259,7 +4330,7 @@
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -4282,7 +4353,7 @@
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
     </row>
-    <row r="19" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -4305,7 +4376,7 @@
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
     </row>
-    <row r="20" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -4328,7 +4399,7 @@
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
     </row>
-    <row r="21" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -4351,7 +4422,7 @@
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
     </row>
-    <row r="22" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -4374,7 +4445,7 @@
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
     </row>
-    <row r="23" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -4397,7 +4468,7 @@
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
     </row>
-    <row r="24" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -4420,7 +4491,7 @@
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
     </row>
-    <row r="25" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -4443,7 +4514,7 @@
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
     </row>
-    <row r="26" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -4466,7 +4537,7 @@
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
     </row>
-    <row r="27" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -4489,7 +4560,7 @@
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
     </row>
-    <row r="28" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -4512,7 +4583,7 @@
       <c r="H28" s="11"/>
       <c r="I28" s="4"/>
     </row>
-    <row r="29" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -4535,7 +4606,7 @@
       <c r="H29" s="11"/>
       <c r="I29" s="4"/>
     </row>
-    <row r="30" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -4558,7 +4629,7 @@
       <c r="H30" s="11"/>
       <c r="I30" s="4"/>
     </row>
-    <row r="31" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -4581,7 +4652,7 @@
       <c r="H31" s="11"/>
       <c r="I31" s="4"/>
     </row>
-    <row r="32" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -4604,7 +4675,7 @@
       <c r="H32" s="11"/>
       <c r="I32" s="4"/>
     </row>
-    <row r="33" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -4627,7 +4698,7 @@
       <c r="H33" s="11"/>
       <c r="I33" s="4"/>
     </row>
-    <row r="34" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -4650,7 +4721,7 @@
       <c r="H34" s="11"/>
       <c r="I34" s="4"/>
     </row>
-    <row r="35" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -4673,7 +4744,7 @@
       <c r="H35" s="11"/>
       <c r="I35" s="4"/>
     </row>
-    <row r="36" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -4696,7 +4767,7 @@
       <c r="H36" s="11"/>
       <c r="I36" s="4"/>
     </row>
-    <row r="37" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -4719,7 +4790,7 @@
       <c r="H37" s="11"/>
       <c r="I37" s="4"/>
     </row>
-    <row r="38" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -4742,7 +4813,7 @@
       <c r="H38" s="11"/>
       <c r="I38" s="4"/>
     </row>
-    <row r="39" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -4765,7 +4836,7 @@
       <c r="H39" s="11"/>
       <c r="I39" s="4"/>
     </row>
-    <row r="40" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -4788,7 +4859,7 @@
       <c r="H40" s="11"/>
       <c r="I40" s="4"/>
     </row>
-    <row r="41" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -4811,7 +4882,7 @@
       <c r="H41" s="13"/>
       <c r="I41" s="16"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -4834,7 +4905,7 @@
       <c r="H42" s="14"/>
       <c r="I42" s="17"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -4857,7 +4928,7 @@
       <c r="H43" s="14"/>
       <c r="I43" s="17"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -4880,7 +4951,7 @@
       <c r="H44" s="14"/>
       <c r="I44" s="17"/>
     </row>
-    <row r="45" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -4903,7 +4974,7 @@
       <c r="H45" s="14"/>
       <c r="I45" s="17"/>
     </row>
-    <row r="46" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -4926,7 +4997,7 @@
       <c r="H46" s="11"/>
       <c r="I46" s="17"/>
     </row>
-    <row r="47" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -4949,7 +5020,7 @@
       <c r="H47" s="11"/>
       <c r="I47" s="17"/>
     </row>
-    <row r="48" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -4972,7 +5043,7 @@
       <c r="H48" s="11"/>
       <c r="I48" s="17"/>
     </row>
-    <row r="49" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -4995,7 +5066,7 @@
       <c r="H49" s="11"/>
       <c r="I49" s="17"/>
     </row>
-    <row r="50" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -5018,7 +5089,7 @@
       <c r="H50" s="11"/>
       <c r="I50" s="17"/>
     </row>
-    <row r="51" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -5041,7 +5112,7 @@
       <c r="H51" s="11"/>
       <c r="I51" s="17"/>
     </row>
-    <row r="52" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -5064,7 +5135,7 @@
       <c r="H52" s="11"/>
       <c r="I52" s="17"/>
     </row>
-    <row r="53" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -5087,7 +5158,7 @@
       <c r="H53" s="11"/>
       <c r="I53" s="17"/>
     </row>
-    <row r="54" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -5110,7 +5181,7 @@
       <c r="H54" s="11"/>
       <c r="I54" s="17"/>
     </row>
-    <row r="55" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -5133,7 +5204,7 @@
       <c r="H55" s="11"/>
       <c r="I55" s="17"/>
     </row>
-    <row r="56" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A56" s="5">
         <v>55</v>
       </c>
@@ -5156,7 +5227,7 @@
       <c r="H56" s="11"/>
       <c r="I56" s="17"/>
     </row>
-    <row r="57" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A57" s="5">
         <v>56</v>
       </c>
@@ -5179,12 +5250,12 @@
       <c r="H57" s="11"/>
       <c r="I57" s="17"/>
     </row>
-    <row r="58" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A58" s="5">
         <v>57</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C58" s="20" t="s">
         <v>180</v>
@@ -5202,12 +5273,12 @@
       <c r="H58" s="13"/>
       <c r="I58" s="17"/>
     </row>
-    <row r="59" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
         <v>58</v>
       </c>
       <c r="B59" s="17" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C59" s="20" t="s">
         <v>180</v>
@@ -5225,12 +5296,12 @@
       <c r="H59" s="17"/>
       <c r="I59" s="17"/>
     </row>
-    <row r="60" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A60" s="5">
         <v>59</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C60" s="20" t="s">
         <v>180</v>
@@ -5248,12 +5319,12 @@
       <c r="H60" s="17"/>
       <c r="I60" s="17"/>
     </row>
-    <row r="61" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A61" s="5">
         <v>60</v>
       </c>
       <c r="B61" s="17" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C61" s="20" t="s">
         <v>188</v>
@@ -5271,12 +5342,12 @@
       <c r="H61" s="17"/>
       <c r="I61" s="17"/>
     </row>
-    <row r="62" spans="1:9" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" ht="99.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="5">
         <v>61</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C62" s="17" t="s">
         <v>201</v>
@@ -5294,7 +5365,7 @@
       <c r="H62" s="17"/>
       <c r="I62" s="17"/>
     </row>
-    <row r="63" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A63" s="5">
         <v>62</v>
       </c>
@@ -5317,7 +5388,7 @@
       <c r="H63" s="17"/>
       <c r="I63" s="17"/>
     </row>
-    <row r="64" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A64" s="5">
         <v>63</v>
       </c>
@@ -5340,7 +5411,7 @@
       <c r="H64" s="17"/>
       <c r="I64" s="17"/>
     </row>
-    <row r="65" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A65" s="5">
         <v>64</v>
       </c>
@@ -5363,7 +5434,7 @@
       <c r="H65" s="17"/>
       <c r="I65" s="17"/>
     </row>
-    <row r="66" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A66" s="5">
         <v>65</v>
       </c>
@@ -5386,7 +5457,7 @@
       <c r="H66" s="17"/>
       <c r="I66" s="17"/>
     </row>
-    <row r="67" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A67" s="5">
         <v>66</v>
       </c>
@@ -5409,7 +5480,7 @@
       <c r="H67" s="17"/>
       <c r="I67" s="17"/>
     </row>
-    <row r="68" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A68" s="5">
         <v>67</v>
       </c>
@@ -5432,7 +5503,7 @@
       <c r="H68" s="17"/>
       <c r="I68" s="17"/>
     </row>
-    <row r="69" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A69" s="5">
         <v>68</v>
       </c>
@@ -5455,7 +5526,7 @@
       <c r="H69" s="17"/>
       <c r="I69" s="17"/>
     </row>
-    <row r="70" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A70" s="5">
         <v>69</v>
       </c>
@@ -5478,7 +5549,7 @@
       <c r="H70" s="17"/>
       <c r="I70" s="17"/>
     </row>
-    <row r="71" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A71" s="5">
         <v>70</v>
       </c>
@@ -5501,7 +5572,7 @@
       <c r="H71" s="17"/>
       <c r="I71" s="17"/>
     </row>
-    <row r="72" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A72" s="5">
         <v>71</v>
       </c>
@@ -5509,100 +5580,174 @@
         <v>222</v>
       </c>
       <c r="C72" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D72" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="F72" s="17" t="s">
         <v>223</v>
       </c>
-      <c r="D72" s="17" t="s">
-        <v>226</v>
-      </c>
-      <c r="E72" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="F72" s="17" t="s">
-        <v>225</v>
-      </c>
-      <c r="G72" s="17"/>
-      <c r="H72" s="17"/>
+      <c r="G72" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="H72" s="17" t="s">
+        <v>61</v>
+      </c>
       <c r="I72" s="17"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A73" s="5">
         <v>72</v>
       </c>
-      <c r="B73" s="17"/>
-      <c r="C73" s="17"/>
-      <c r="D73" s="17"/>
-      <c r="E73" s="17"/>
-      <c r="F73" s="17"/>
-      <c r="G73" s="17"/>
-      <c r="H73" s="17"/>
+      <c r="B73" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="C73" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="D73" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="F73" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="G73" s="17" t="s">
+        <v>244</v>
+      </c>
+      <c r="H73" s="17" t="s">
+        <v>61</v>
+      </c>
       <c r="I73" s="17"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A74" s="5">
         <v>73</v>
       </c>
-      <c r="B74" s="17"/>
-      <c r="C74" s="17"/>
-      <c r="D74" s="17"/>
-      <c r="E74" s="17"/>
-      <c r="F74" s="17"/>
-      <c r="G74" s="17"/>
-      <c r="H74" s="17"/>
+      <c r="B74" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="C74" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="D74" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="F74" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="G74" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="H74" s="17" t="s">
+        <v>61</v>
+      </c>
       <c r="I74" s="17"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A75" s="5">
         <v>74</v>
       </c>
-      <c r="B75" s="17"/>
-      <c r="C75" s="17"/>
-      <c r="D75" s="17"/>
-      <c r="E75" s="17"/>
-      <c r="F75" s="17"/>
-      <c r="G75" s="17"/>
-      <c r="H75" s="17"/>
+      <c r="B75" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="C75" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="D75" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="F75" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="G75" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="H75" s="17" t="s">
+        <v>61</v>
+      </c>
       <c r="I75" s="17"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A76" s="5">
         <v>75</v>
       </c>
-      <c r="B76" s="17"/>
-      <c r="C76" s="17"/>
-      <c r="D76" s="17"/>
-      <c r="E76" s="17"/>
-      <c r="F76" s="17"/>
-      <c r="G76" s="17"/>
-      <c r="H76" s="17"/>
+      <c r="B76" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="C76" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="D76" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="F76" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="G76" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="H76" s="17" t="s">
+        <v>61</v>
+      </c>
       <c r="I76" s="17"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A77" s="5">
         <v>76</v>
       </c>
-      <c r="B77" s="17"/>
-      <c r="C77" s="17"/>
-      <c r="D77" s="17"/>
-      <c r="E77" s="17"/>
-      <c r="F77" s="17"/>
-      <c r="G77" s="17"/>
-      <c r="H77" s="17"/>
+      <c r="B77" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="C77" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="D77" s="17" t="s">
+        <v>238</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="F77" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="G77" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="H77" s="17" t="s">
+        <v>61</v>
+      </c>
       <c r="I77" s="17"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" s="5">
         <v>77</v>
       </c>
       <c r="B78" s="17"/>
       <c r="C78" s="17"/>
       <c r="D78" s="17"/>
-      <c r="E78" s="17"/>
+      <c r="E78" s="5"/>
       <c r="F78" s="17"/>
       <c r="G78" s="17"/>
       <c r="H78" s="17"/>
       <c r="I78" s="17"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" s="5">
         <v>78</v>
       </c>
@@ -5615,7 +5760,7 @@
       <c r="H79" s="17"/>
       <c r="I79" s="17"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" s="5">
         <v>79</v>
       </c>
@@ -5628,7 +5773,7 @@
       <c r="H80" s="17"/>
       <c r="I80" s="17"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" s="5">
         <v>80</v>
       </c>
@@ -5641,7 +5786,7 @@
       <c r="H81" s="17"/>
       <c r="I81" s="17"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" s="5">
         <v>81</v>
       </c>
@@ -5654,7 +5799,7 @@
       <c r="H82" s="17"/>
       <c r="I82" s="17"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" s="5">
         <v>82</v>
       </c>
@@ -5667,7 +5812,7 @@
       <c r="H83" s="17"/>
       <c r="I83" s="17"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84" s="5">
         <v>83</v>
       </c>
@@ -5680,7 +5825,7 @@
       <c r="H84" s="17"/>
       <c r="I84" s="17"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" s="5">
         <v>84</v>
       </c>
@@ -5693,7 +5838,7 @@
       <c r="H85" s="17"/>
       <c r="I85" s="17"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" s="5">
         <v>85</v>
       </c>
@@ -5706,7 +5851,7 @@
       <c r="H86" s="17"/>
       <c r="I86" s="17"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" s="5">
         <v>86</v>
       </c>
@@ -5719,7 +5864,7 @@
       <c r="H87" s="17"/>
       <c r="I87" s="17"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" s="5">
         <v>87</v>
       </c>
@@ -5732,7 +5877,7 @@
       <c r="H88" s="17"/>
       <c r="I88" s="17"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" s="5">
         <v>88</v>
       </c>
@@ -5745,7 +5890,7 @@
       <c r="H89" s="17"/>
       <c r="I89" s="17"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" s="5">
         <v>89</v>
       </c>
@@ -5758,7 +5903,7 @@
       <c r="H90" s="17"/>
       <c r="I90" s="17"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" s="5">
         <v>90</v>
       </c>
@@ -5771,7 +5916,7 @@
       <c r="H91" s="17"/>
       <c r="I91" s="17"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" s="5">
         <v>91</v>
       </c>
@@ -5784,7 +5929,7 @@
       <c r="H92" s="17"/>
       <c r="I92" s="17"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" s="5">
         <v>92</v>
       </c>
@@ -5797,7 +5942,7 @@
       <c r="H93" s="17"/>
       <c r="I93" s="17"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" s="5">
         <v>93</v>
       </c>
@@ -5810,7 +5955,7 @@
       <c r="H94" s="17"/>
       <c r="I94" s="17"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" s="5">
         <v>94</v>
       </c>
@@ -5823,7 +5968,7 @@
       <c r="H95" s="17"/>
       <c r="I95" s="17"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" s="5">
         <v>95</v>
       </c>
@@ -5836,7 +5981,7 @@
       <c r="H96" s="17"/>
       <c r="I96" s="17"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97" s="5">
         <v>96</v>
       </c>
@@ -5849,7 +5994,7 @@
       <c r="H97" s="17"/>
       <c r="I97" s="17"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" s="5">
         <v>97</v>
       </c>
@@ -5864,10 +6009,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"pass"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
testing for reset password
</commit_message>
<xml_diff>
--- a/testing/Team eXi Test Cases.xlsx
+++ b/testing/Team eXi Test Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HuiXin\Documents\FYP\Thriving-Stones-Project\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B37B021D-402E-4FD3-A61D-89F43547F352}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F80950B-C86E-4D9F-9542-771309DD8708}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="40" windowWidth="25750" windowHeight="11590" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="260">
   <si>
     <t>S/N</t>
   </si>
@@ -1015,6 +1015,39 @@
   </si>
   <si>
     <t>Error message "Please select end time displayed"</t>
+  </si>
+  <si>
+    <t>Reset Password</t>
+  </si>
+  <si>
+    <t>Users who provided the valid email would be able to receive a reset password email</t>
+  </si>
+  <si>
+    <t>Email: irene.ng.1997@steppingstones.com.sg</t>
+  </si>
+  <si>
+    <t>Enter the email into the email field</t>
+  </si>
+  <si>
+    <t>Email Sent Successfully</t>
+  </si>
+  <si>
+    <t>Error Message displayed</t>
+  </si>
+  <si>
+    <t>Users who left the email empty would not be able to receive a reset password email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email: </t>
+  </si>
+  <si>
+    <t>Error Message "Please enter a valid email" to be displayed</t>
+  </si>
+  <si>
+    <t>Users who entered an invalid email would not be able to receive a reset password email</t>
+  </si>
+  <si>
+    <t>Email: irene.ng@steppingstones.com.sg</t>
   </si>
 </sst>
 </file>
@@ -3913,11 +3946,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5155472-66AF-4323-ACD5-D08CB3B87B8B}">
-  <dimension ref="A1:I98"/>
+  <dimension ref="A1:CV96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H72" sqref="H72:H77"/>
+      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3933,7 +3966,7 @@
     <col min="9" max="9" width="19.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:100" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3962,30 +3995,309 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:100" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="5">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5">
+        <v>3</v>
+      </c>
+      <c r="D2" s="5">
+        <v>4</v>
+      </c>
+      <c r="E2" s="5">
+        <v>5</v>
+      </c>
+      <c r="F2" s="5">
+        <v>6</v>
+      </c>
+      <c r="G2" s="5">
+        <v>7</v>
+      </c>
+      <c r="H2" s="5">
         <v>8</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="I2" s="5">
         <v>9</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="J2" s="5">
         <v>10</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="K2" s="5">
         <v>11</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="L2" s="5">
         <v>12</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-    </row>
-    <row r="3" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="M2" s="5">
+        <v>13</v>
+      </c>
+      <c r="N2" s="5">
+        <v>14</v>
+      </c>
+      <c r="O2" s="5">
+        <v>15</v>
+      </c>
+      <c r="P2" s="5">
+        <v>16</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>17</v>
+      </c>
+      <c r="R2" s="5">
+        <v>18</v>
+      </c>
+      <c r="S2" s="5">
+        <v>19</v>
+      </c>
+      <c r="T2" s="5">
+        <v>20</v>
+      </c>
+      <c r="U2" s="5">
+        <v>21</v>
+      </c>
+      <c r="V2" s="5">
+        <v>22</v>
+      </c>
+      <c r="W2" s="5">
+        <v>23</v>
+      </c>
+      <c r="X2" s="5">
+        <v>24</v>
+      </c>
+      <c r="Y2" s="5">
+        <v>25</v>
+      </c>
+      <c r="Z2" s="5">
+        <v>26</v>
+      </c>
+      <c r="AA2" s="5">
+        <v>27</v>
+      </c>
+      <c r="AB2" s="5">
+        <v>28</v>
+      </c>
+      <c r="AC2" s="5">
+        <v>29</v>
+      </c>
+      <c r="AD2" s="5">
+        <v>30</v>
+      </c>
+      <c r="AE2" s="5">
+        <v>31</v>
+      </c>
+      <c r="AF2" s="5">
+        <v>32</v>
+      </c>
+      <c r="AG2" s="5">
+        <v>33</v>
+      </c>
+      <c r="AH2" s="5">
+        <v>34</v>
+      </c>
+      <c r="AI2" s="5">
+        <v>35</v>
+      </c>
+      <c r="AJ2" s="5">
+        <v>36</v>
+      </c>
+      <c r="AK2" s="5">
+        <v>37</v>
+      </c>
+      <c r="AL2" s="5">
+        <v>38</v>
+      </c>
+      <c r="AM2" s="5">
+        <v>39</v>
+      </c>
+      <c r="AN2" s="5">
+        <v>40</v>
+      </c>
+      <c r="AO2" s="5">
+        <v>41</v>
+      </c>
+      <c r="AP2" s="5">
+        <v>42</v>
+      </c>
+      <c r="AQ2" s="5">
+        <v>43</v>
+      </c>
+      <c r="AR2" s="5">
+        <v>44</v>
+      </c>
+      <c r="AS2" s="5">
+        <v>45</v>
+      </c>
+      <c r="AT2" s="5">
+        <v>46</v>
+      </c>
+      <c r="AU2" s="5">
+        <v>47</v>
+      </c>
+      <c r="AV2" s="5">
+        <v>48</v>
+      </c>
+      <c r="AW2" s="5">
+        <v>49</v>
+      </c>
+      <c r="AX2" s="5">
+        <v>50</v>
+      </c>
+      <c r="AY2" s="5">
+        <v>51</v>
+      </c>
+      <c r="AZ2" s="5">
+        <v>52</v>
+      </c>
+      <c r="BA2" s="5">
+        <v>53</v>
+      </c>
+      <c r="BB2" s="5">
+        <v>54</v>
+      </c>
+      <c r="BC2" s="5">
+        <v>55</v>
+      </c>
+      <c r="BD2" s="5">
+        <v>56</v>
+      </c>
+      <c r="BE2" s="5">
+        <v>57</v>
+      </c>
+      <c r="BF2" s="5">
+        <v>58</v>
+      </c>
+      <c r="BG2" s="5">
+        <v>59</v>
+      </c>
+      <c r="BH2" s="5">
+        <v>60</v>
+      </c>
+      <c r="BI2" s="5">
+        <v>61</v>
+      </c>
+      <c r="BJ2" s="5">
+        <v>62</v>
+      </c>
+      <c r="BK2" s="5">
+        <v>63</v>
+      </c>
+      <c r="BL2" s="5">
+        <v>64</v>
+      </c>
+      <c r="BM2" s="5">
+        <v>65</v>
+      </c>
+      <c r="BN2" s="5">
+        <v>66</v>
+      </c>
+      <c r="BO2" s="5">
+        <v>67</v>
+      </c>
+      <c r="BP2" s="5">
+        <v>68</v>
+      </c>
+      <c r="BQ2" s="5">
+        <v>69</v>
+      </c>
+      <c r="BR2" s="5">
+        <v>70</v>
+      </c>
+      <c r="BS2" s="5">
+        <v>71</v>
+      </c>
+      <c r="BT2" s="5">
+        <v>72</v>
+      </c>
+      <c r="BU2" s="5">
+        <v>73</v>
+      </c>
+      <c r="BV2" s="5">
+        <v>74</v>
+      </c>
+      <c r="BW2" s="5">
+        <v>75</v>
+      </c>
+      <c r="BX2" s="5">
+        <v>76</v>
+      </c>
+      <c r="BY2" s="5">
+        <v>77</v>
+      </c>
+      <c r="BZ2" s="5">
+        <v>78</v>
+      </c>
+      <c r="CA2" s="5">
+        <v>79</v>
+      </c>
+      <c r="CB2" s="5">
+        <v>80</v>
+      </c>
+      <c r="CC2" s="5">
+        <v>81</v>
+      </c>
+      <c r="CD2" s="5">
+        <v>82</v>
+      </c>
+      <c r="CE2" s="5">
+        <v>83</v>
+      </c>
+      <c r="CF2" s="5">
+        <v>84</v>
+      </c>
+      <c r="CG2" s="5">
+        <v>85</v>
+      </c>
+      <c r="CH2" s="5">
+        <v>86</v>
+      </c>
+      <c r="CI2" s="5">
+        <v>87</v>
+      </c>
+      <c r="CJ2" s="5">
+        <v>88</v>
+      </c>
+      <c r="CK2" s="5">
+        <v>89</v>
+      </c>
+      <c r="CL2" s="5">
+        <v>90</v>
+      </c>
+      <c r="CM2" s="5">
+        <v>91</v>
+      </c>
+      <c r="CN2" s="5">
+        <v>92</v>
+      </c>
+      <c r="CO2" s="5">
+        <v>93</v>
+      </c>
+      <c r="CP2" s="5">
+        <v>94</v>
+      </c>
+      <c r="CQ2" s="5">
+        <v>95</v>
+      </c>
+      <c r="CR2" s="5">
+        <v>96</v>
+      </c>
+      <c r="CS2" s="5">
+        <v>97</v>
+      </c>
+      <c r="CT2" s="5">
+        <v>98</v>
+      </c>
+      <c r="CU2" s="5">
+        <v>99</v>
+      </c>
+      <c r="CV2" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:100" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -4008,7 +4320,7 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:100" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -4031,7 +4343,7 @@
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:100" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -4054,7 +4366,7 @@
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:100" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -4077,7 +4389,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:100" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -4100,7 +4412,7 @@
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:100" ht="58" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -4123,7 +4435,7 @@
       <c r="H8" s="16"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:100" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -4146,7 +4458,7 @@
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:100" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -4169,7 +4481,7 @@
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:100" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -4192,7 +4504,7 @@
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
     </row>
-    <row r="12" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:100" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -4215,139 +4527,139 @@
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:100" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>35</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:100" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:100" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:100" ht="87" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>42</v>
+        <v>173</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>48</v>
+        <v>88</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>42</v>
+        <v>173</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>25</v>
+        <v>90</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
@@ -4355,68 +4667,68 @@
     </row>
     <row r="19" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>173</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>54</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
     </row>
-    <row r="20" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>173</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>56</v>
+        <v>93</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>54</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>57</v>
+        <v>95</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
     </row>
-    <row r="21" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>173</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>58</v>
+        <v>96</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>54</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
@@ -4424,22 +4736,22 @@
     </row>
     <row r="22" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>173</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>54</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
@@ -4447,134 +4759,134 @@
     </row>
     <row r="23" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>173</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>54</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
     </row>
-    <row r="24" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
-        <v>23</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="G24" s="4"/>
+        <v>25</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="G24" s="5"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
     </row>
-    <row r="25" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
-        <v>24</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-    </row>
-    <row r="26" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+    </row>
+    <row r="26" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
-        <v>25</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="G26" s="5"/>
-      <c r="H26" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
       <c r="I26" s="4"/>
     </row>
     <row r="27" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B27" s="18" t="s">
         <v>175</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
+      <c r="I27" s="4"/>
     </row>
     <row r="28" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B28" s="18" t="s">
         <v>175</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="F28" s="11" t="s">
         <v>113</v>
@@ -4585,19 +4897,19 @@
     </row>
     <row r="29" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B29" s="18" t="s">
         <v>175</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="F29" s="11" t="s">
         <v>113</v>
@@ -4606,21 +4918,21 @@
       <c r="H29" s="11"/>
       <c r="I29" s="4"/>
     </row>
-    <row r="30" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B30" s="18" t="s">
         <v>175</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="F30" s="11" t="s">
         <v>113</v>
@@ -4631,19 +4943,19 @@
     </row>
     <row r="31" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B31" s="18" t="s">
         <v>175</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>117</v>
+        <v>136</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>118</v>
+        <v>138</v>
       </c>
       <c r="F31" s="11" t="s">
         <v>113</v>
@@ -4652,9 +4964,9 @@
       <c r="H31" s="11"/>
       <c r="I31" s="4"/>
     </row>
-    <row r="32" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B32" s="18" t="s">
         <v>175</v>
@@ -4663,10 +4975,10 @@
         <v>121</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F32" s="11" t="s">
         <v>113</v>
@@ -4677,19 +4989,19 @@
     </row>
     <row r="33" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B33" s="18" t="s">
         <v>175</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="F33" s="11" t="s">
         <v>113</v>
@@ -4700,19 +5012,19 @@
     </row>
     <row r="34" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B34" s="18" t="s">
         <v>175</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="F34" s="11" t="s">
         <v>113</v>
@@ -4723,7 +5035,7 @@
     </row>
     <row r="35" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B35" s="18" t="s">
         <v>175</v>
@@ -4732,10 +5044,10 @@
         <v>125</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="F35" s="11" t="s">
         <v>113</v>
@@ -4744,9 +5056,9 @@
       <c r="H35" s="11"/>
       <c r="I35" s="4"/>
     </row>
-    <row r="36" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B36" s="18" t="s">
         <v>175</v>
@@ -4755,10 +5067,10 @@
         <v>125</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F36" s="11" t="s">
         <v>113</v>
@@ -4769,7 +5081,7 @@
     </row>
     <row r="37" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B37" s="18" t="s">
         <v>175</v>
@@ -4778,10 +5090,10 @@
         <v>125</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="F37" s="11" t="s">
         <v>113</v>
@@ -4790,9 +5102,9 @@
       <c r="H37" s="11"/>
       <c r="I37" s="4"/>
     </row>
-    <row r="38" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B38" s="18" t="s">
         <v>175</v>
@@ -4801,10 +5113,10 @@
         <v>125</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="F38" s="11" t="s">
         <v>113</v>
@@ -4815,180 +5127,180 @@
     </row>
     <row r="39" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B39" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C39" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="D39" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="E39" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="F39" s="11" t="s">
+      <c r="D39" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="F39" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="4"/>
-    </row>
-    <row r="40" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="16"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
-        <v>39</v>
-      </c>
-      <c r="B40" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="E40" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="F40" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
-      <c r="I40" s="4"/>
-    </row>
-    <row r="41" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+      <c r="B40" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="E40" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="F40" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="17"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
-        <v>40</v>
-      </c>
-      <c r="B41" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="C41" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="D41" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="E41" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="F41" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
-      <c r="I41" s="16"/>
+        <v>42</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="E41" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="F41" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="17"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
-        <v>41</v>
-      </c>
-      <c r="B42" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42" s="14" t="s">
         <v>176</v>
       </c>
       <c r="C42" s="14" t="s">
         <v>144</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="E42" s="14" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="F42" s="14" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G42" s="14"/>
       <c r="H42" s="14"/>
       <c r="I42" s="17"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
-        <v>42</v>
-      </c>
-      <c r="B43" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="C43" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="D43" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="E43" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="F43" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="G43" s="14"/>
+        <v>44</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="F43" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="G43" s="11"/>
       <c r="H43" s="14"/>
       <c r="I43" s="17"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A44" s="5">
-        <v>43</v>
-      </c>
-      <c r="B44" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="C44" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="D44" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="E44" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="F44" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
+        <v>45</v>
+      </c>
+      <c r="B44" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="F44" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
       <c r="I44" s="17"/>
     </row>
     <row r="45" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A45" s="5">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B45" s="17" t="s">
         <v>177</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>153</v>
+        <v>110</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="F45" s="11" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G45" s="11"/>
-      <c r="H45" s="14"/>
+      <c r="H45" s="11"/>
       <c r="I45" s="17"/>
     </row>
     <row r="46" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A46" s="5">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B46" s="17" t="s">
         <v>177</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="F46" s="11" t="s">
         <v>155</v>
@@ -4999,19 +5311,19 @@
     </row>
     <row r="47" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A47" s="5">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B47" s="17" t="s">
         <v>177</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="F47" s="11" t="s">
         <v>155</v>
@@ -5020,21 +5332,21 @@
       <c r="H47" s="11"/>
       <c r="I47" s="17"/>
     </row>
-    <row r="48" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A48" s="5">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B48" s="17" t="s">
         <v>177</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="F48" s="11" t="s">
         <v>155</v>
@@ -5045,19 +5357,19 @@
     </row>
     <row r="49" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A49" s="5">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B49" s="17" t="s">
         <v>177</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="F49" s="11" t="s">
         <v>155</v>
@@ -5066,21 +5378,21 @@
       <c r="H49" s="11"/>
       <c r="I49" s="17"/>
     </row>
-    <row r="50" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A50" s="5">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B50" s="17" t="s">
         <v>177</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F50" s="11" t="s">
         <v>155</v>
@@ -5091,19 +5403,19 @@
     </row>
     <row r="51" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A51" s="5">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B51" s="17" t="s">
         <v>177</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E51" s="11" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="F51" s="11" t="s">
         <v>155</v>
@@ -5114,7 +5426,7 @@
     </row>
     <row r="52" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A52" s="5">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B52" s="17" t="s">
         <v>177</v>
@@ -5123,10 +5435,10 @@
         <v>125</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="F52" s="11" t="s">
         <v>155</v>
@@ -5135,9 +5447,9 @@
       <c r="H52" s="11"/>
       <c r="I52" s="17"/>
     </row>
-    <row r="53" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A53" s="5">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B53" s="17" t="s">
         <v>177</v>
@@ -5146,10 +5458,10 @@
         <v>125</v>
       </c>
       <c r="D53" s="11" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E53" s="11" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F53" s="11" t="s">
         <v>155</v>
@@ -5160,7 +5472,7 @@
     </row>
     <row r="54" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A54" s="5">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B54" s="17" t="s">
         <v>177</v>
@@ -5169,10 +5481,10 @@
         <v>125</v>
       </c>
       <c r="D54" s="11" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="F54" s="11" t="s">
         <v>155</v>
@@ -5181,78 +5493,78 @@
       <c r="H54" s="11"/>
       <c r="I54" s="17"/>
     </row>
-    <row r="55" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A55" s="5">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="C55" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="C55" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="D55" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="E55" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="F55" s="11" t="s">
-        <v>155</v>
+      <c r="D55" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="E55" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="F55" s="18" t="s">
+        <v>179</v>
       </c>
       <c r="G55" s="11"/>
       <c r="H55" s="11"/>
       <c r="I55" s="17"/>
     </row>
-    <row r="56" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A56" s="5">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="C56" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="D56" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="E56" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="F56" s="11" t="s">
-        <v>155</v>
+        <v>224</v>
+      </c>
+      <c r="C56" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="D56" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="E56" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="F56" s="18" t="s">
+        <v>182</v>
       </c>
       <c r="G56" s="11"/>
-      <c r="H56" s="11"/>
+      <c r="H56" s="13"/>
       <c r="I56" s="17"/>
     </row>
-    <row r="57" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A57" s="5">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="C57" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="D57" s="18" t="s">
-        <v>184</v>
-      </c>
-      <c r="E57" s="18" t="s">
-        <v>183</v>
+        <v>224</v>
+      </c>
+      <c r="C57" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="D57" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="E57" s="20" t="s">
+        <v>181</v>
       </c>
       <c r="F57" s="18" t="s">
-        <v>179</v>
-      </c>
-      <c r="G57" s="11"/>
-      <c r="H57" s="11"/>
+        <v>190</v>
+      </c>
+      <c r="G57" s="17"/>
+      <c r="H57" s="17"/>
       <c r="I57" s="17"/>
     </row>
     <row r="58" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A58" s="5">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B58" s="17" t="s">
         <v>224</v>
@@ -5261,105 +5573,105 @@
         <v>180</v>
       </c>
       <c r="D58" s="20" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="E58" s="20" t="s">
         <v>181</v>
       </c>
       <c r="F58" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="G58" s="11"/>
-      <c r="H58" s="13"/>
+        <v>191</v>
+      </c>
+      <c r="G58" s="17"/>
+      <c r="H58" s="17"/>
       <c r="I58" s="17"/>
     </row>
     <row r="59" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B59" s="17" t="s">
         <v>224</v>
       </c>
       <c r="C59" s="20" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="D59" s="20" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E59" s="20" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="F59" s="18" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="G59" s="17"/>
       <c r="H59" s="17"/>
       <c r="I59" s="17"/>
     </row>
-    <row r="60" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" ht="99.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="5">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B60" s="17" t="s">
         <v>224</v>
       </c>
-      <c r="C60" s="20" t="s">
-        <v>180</v>
+      <c r="C60" s="17" t="s">
+        <v>201</v>
       </c>
       <c r="D60" s="20" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="E60" s="20" t="s">
         <v>181</v>
       </c>
-      <c r="F60" s="18" t="s">
-        <v>191</v>
+      <c r="F60" s="17" t="s">
+        <v>195</v>
       </c>
       <c r="G60" s="17"/>
       <c r="H60" s="17"/>
       <c r="I60" s="17"/>
     </row>
-    <row r="61" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A61" s="5">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B61" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="C61" s="20" t="s">
-        <v>188</v>
-      </c>
-      <c r="D61" s="20" t="s">
-        <v>187</v>
-      </c>
-      <c r="E61" s="20" t="s">
-        <v>189</v>
-      </c>
-      <c r="F61" s="18" t="s">
-        <v>193</v>
+        <v>200</v>
+      </c>
+      <c r="C61" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="D61" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="E61" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="F61" s="17" t="s">
+        <v>199</v>
       </c>
       <c r="G61" s="17"/>
       <c r="H61" s="17"/>
       <c r="I61" s="17"/>
     </row>
-    <row r="62" spans="1:9" ht="99.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A62" s="5">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>224</v>
+        <v>200</v>
       </c>
       <c r="C62" s="17" t="s">
         <v>201</v>
       </c>
-      <c r="D62" s="20" t="s">
-        <v>194</v>
+      <c r="D62" s="17" t="s">
+        <v>202</v>
       </c>
       <c r="E62" s="20" t="s">
-        <v>181</v>
+        <v>203</v>
       </c>
       <c r="F62" s="17" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="G62" s="17"/>
       <c r="H62" s="17"/>
@@ -5367,10 +5679,10 @@
     </row>
     <row r="63" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A63" s="5">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B63" s="17" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C63" s="17" t="s">
         <v>125</v>
@@ -5390,10 +5702,10 @@
     </row>
     <row r="64" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A64" s="5">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B64" s="17" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C64" s="17" t="s">
         <v>201</v>
@@ -5402,102 +5714,102 @@
         <v>202</v>
       </c>
       <c r="E64" s="20" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="F64" s="17" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="G64" s="17"/>
       <c r="H64" s="17"/>
       <c r="I64" s="17"/>
     </row>
-    <row r="65" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A65" s="5">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B65" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="C65" s="17" t="s">
-        <v>125</v>
+      <c r="C65" s="20" t="s">
+        <v>210</v>
       </c>
       <c r="D65" s="17" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
       <c r="E65" s="17" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="F65" s="17" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="G65" s="17"/>
       <c r="H65" s="17"/>
       <c r="I65" s="17"/>
     </row>
-    <row r="66" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A66" s="5">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B66" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="C66" s="17" t="s">
-        <v>201</v>
+      <c r="C66" s="20" t="s">
+        <v>206</v>
       </c>
       <c r="D66" s="17" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="E66" s="20" t="s">
         <v>212</v>
       </c>
       <c r="F66" s="17" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="G66" s="17"/>
       <c r="H66" s="17"/>
       <c r="I66" s="17"/>
     </row>
-    <row r="67" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A67" s="5">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B67" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="C67" s="20" t="s">
-        <v>210</v>
+        <v>217</v>
+      </c>
+      <c r="C67" s="17" t="s">
+        <v>125</v>
       </c>
       <c r="D67" s="17" t="s">
-        <v>207</v>
-      </c>
-      <c r="E67" s="17" t="s">
-        <v>208</v>
+        <v>214</v>
+      </c>
+      <c r="E67" s="20" t="s">
+        <v>215</v>
       </c>
       <c r="F67" s="17" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="G67" s="17"/>
       <c r="H67" s="17"/>
       <c r="I67" s="17"/>
     </row>
-    <row r="68" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A68" s="5">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B68" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="C68" s="20" t="s">
-        <v>206</v>
+        <v>217</v>
+      </c>
+      <c r="C68" s="17" t="s">
+        <v>201</v>
       </c>
       <c r="D68" s="17" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="E68" s="20" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="F68" s="17" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="G68" s="17"/>
       <c r="H68" s="17"/>
@@ -5505,94 +5817,102 @@
     </row>
     <row r="69" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A69" s="5">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B69" s="17" t="s">
         <v>217</v>
       </c>
       <c r="C69" s="17" t="s">
-        <v>125</v>
+        <v>219</v>
       </c>
       <c r="D69" s="17" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="E69" s="20" t="s">
         <v>215</v>
       </c>
       <c r="F69" s="17" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="G69" s="17"/>
       <c r="H69" s="17"/>
       <c r="I69" s="17"/>
     </row>
-    <row r="70" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A70" s="5">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B70" s="17" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="C70" s="17" t="s">
-        <v>201</v>
+        <v>225</v>
       </c>
       <c r="D70" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="E70" s="20" t="s">
-        <v>215</v>
+        <v>230</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>239</v>
       </c>
       <c r="F70" s="17" t="s">
-        <v>218</v>
-      </c>
-      <c r="G70" s="17"/>
-      <c r="H70" s="17"/>
+        <v>223</v>
+      </c>
+      <c r="G70" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="H70" s="17" t="s">
+        <v>61</v>
+      </c>
       <c r="I70" s="17"/>
     </row>
-    <row r="71" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A71" s="5">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B71" s="17" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="C71" s="17" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="D71" s="17" t="s">
-        <v>221</v>
-      </c>
-      <c r="E71" s="20" t="s">
-        <v>215</v>
+        <v>231</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>239</v>
       </c>
       <c r="F71" s="17" t="s">
-        <v>218</v>
-      </c>
-      <c r="G71" s="17"/>
-      <c r="H71" s="17"/>
+        <v>227</v>
+      </c>
+      <c r="G71" s="17" t="s">
+        <v>244</v>
+      </c>
+      <c r="H71" s="17" t="s">
+        <v>61</v>
+      </c>
       <c r="I71" s="17"/>
     </row>
     <row r="72" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A72" s="5">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B72" s="17" t="s">
         <v>222</v>
       </c>
       <c r="C72" s="17" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="D72" s="17" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="E72" s="5" t="s">
         <v>239</v>
       </c>
       <c r="F72" s="17" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="G72" s="17" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="H72" s="17" t="s">
         <v>61</v>
@@ -5601,25 +5921,25 @@
     </row>
     <row r="73" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A73" s="5">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B73" s="17" t="s">
         <v>222</v>
       </c>
       <c r="C73" s="17" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="D73" s="17" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="E73" s="5" t="s">
         <v>239</v>
       </c>
       <c r="F73" s="17" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="G73" s="17" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="H73" s="17" t="s">
         <v>61</v>
@@ -5628,25 +5948,25 @@
     </row>
     <row r="74" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A74" s="5">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B74" s="17" t="s">
         <v>222</v>
       </c>
       <c r="C74" s="17" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="D74" s="17" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="E74" s="5" t="s">
         <v>239</v>
       </c>
       <c r="F74" s="17" t="s">
-        <v>229</v>
+        <v>241</v>
       </c>
       <c r="G74" s="17" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="H74" s="17" t="s">
         <v>61</v>
@@ -5655,101 +5975,117 @@
     </row>
     <row r="75" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A75" s="5">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B75" s="17" t="s">
         <v>222</v>
       </c>
       <c r="C75" s="17" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="D75" s="17" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="E75" s="5" t="s">
         <v>239</v>
       </c>
       <c r="F75" s="17" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="G75" s="17" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="H75" s="17" t="s">
         <v>61</v>
       </c>
       <c r="I75" s="17"/>
     </row>
-    <row r="76" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A76" s="5">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B76" s="17" t="s">
-        <v>222</v>
+        <v>249</v>
       </c>
       <c r="C76" s="17" t="s">
-        <v>235</v>
+        <v>250</v>
       </c>
       <c r="D76" s="17" t="s">
-        <v>236</v>
+        <v>251</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>239</v>
+        <v>252</v>
       </c>
       <c r="F76" s="17" t="s">
-        <v>241</v>
+        <v>253</v>
       </c>
       <c r="G76" s="17" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="H76" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="I76" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="I76" s="17"/>
-    </row>
-    <row r="77" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    </row>
+    <row r="77" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A77" s="5">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B77" s="17" t="s">
-        <v>222</v>
+        <v>249</v>
       </c>
       <c r="C77" s="17" t="s">
-        <v>237</v>
+        <v>255</v>
       </c>
       <c r="D77" s="17" t="s">
-        <v>238</v>
+        <v>256</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>239</v>
+        <v>252</v>
       </c>
       <c r="F77" s="17" t="s">
-        <v>242</v>
+        <v>257</v>
       </c>
       <c r="G77" s="17" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="H77" s="17" t="s">
         <v>61</v>
       </c>
       <c r="I77" s="17"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A78" s="5">
-        <v>77</v>
-      </c>
-      <c r="B78" s="17"/>
-      <c r="C78" s="17"/>
-      <c r="D78" s="17"/>
-      <c r="E78" s="5"/>
-      <c r="F78" s="17"/>
-      <c r="G78" s="17"/>
-      <c r="H78" s="17"/>
+        <v>79</v>
+      </c>
+      <c r="B78" s="17" t="s">
+        <v>249</v>
+      </c>
+      <c r="C78" s="17" t="s">
+        <v>258</v>
+      </c>
+      <c r="D78" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="F78" s="17" t="s">
+        <v>257</v>
+      </c>
+      <c r="G78" s="17" t="s">
+        <v>254</v>
+      </c>
+      <c r="H78" s="17" t="s">
+        <v>61</v>
+      </c>
       <c r="I78" s="17"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" s="5">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B79" s="17"/>
       <c r="C79" s="17"/>
@@ -5762,7 +6098,7 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" s="5">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B80" s="17"/>
       <c r="C80" s="17"/>
@@ -5775,7 +6111,7 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" s="5">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B81" s="17"/>
       <c r="C81" s="17"/>
@@ -5788,7 +6124,7 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" s="5">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B82" s="17"/>
       <c r="C82" s="17"/>
@@ -5801,7 +6137,7 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" s="5">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B83" s="17"/>
       <c r="C83" s="17"/>
@@ -5814,7 +6150,7 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84" s="5">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B84" s="17"/>
       <c r="C84" s="17"/>
@@ -5827,7 +6163,7 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" s="5">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B85" s="17"/>
       <c r="C85" s="17"/>
@@ -5840,7 +6176,7 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" s="5">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B86" s="17"/>
       <c r="C86" s="17"/>
@@ -5853,7 +6189,7 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" s="5">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B87" s="17"/>
       <c r="C87" s="17"/>
@@ -5866,7 +6202,7 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" s="5">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B88" s="17"/>
       <c r="C88" s="17"/>
@@ -5879,7 +6215,7 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" s="5">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B89" s="17"/>
       <c r="C89" s="17"/>
@@ -5892,7 +6228,7 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" s="5">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B90" s="17"/>
       <c r="C90" s="17"/>
@@ -5905,7 +6241,7 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" s="5">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B91" s="17"/>
       <c r="C91" s="17"/>
@@ -5918,7 +6254,7 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" s="5">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B92" s="17"/>
       <c r="C92" s="17"/>
@@ -5931,7 +6267,7 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" s="5">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B93" s="17"/>
       <c r="C93" s="17"/>
@@ -5944,7 +6280,7 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" s="5">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B94" s="17"/>
       <c r="C94" s="17"/>
@@ -5957,7 +6293,7 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" s="5">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B95" s="17"/>
       <c r="C95" s="17"/>
@@ -5970,7 +6306,7 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" s="5">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B96" s="17"/>
       <c r="C96" s="17"/>
@@ -5980,32 +6316,6 @@
       <c r="G96" s="17"/>
       <c r="H96" s="17"/>
       <c r="I96" s="17"/>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A97" s="5">
-        <v>96</v>
-      </c>
-      <c r="B97" s="17"/>
-      <c r="C97" s="17"/>
-      <c r="D97" s="17"/>
-      <c r="E97" s="17"/>
-      <c r="F97" s="17"/>
-      <c r="G97" s="17"/>
-      <c r="H97" s="17"/>
-      <c r="I97" s="17"/>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A98" s="5">
-        <v>97</v>
-      </c>
-      <c r="B98" s="17"/>
-      <c r="C98" s="17"/>
-      <c r="D98" s="17"/>
-      <c r="E98" s="17"/>
-      <c r="F98" s="17"/>
-      <c r="G98" s="17"/>
-      <c r="H98" s="17"/>
-      <c r="I98" s="17"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1">

</xml_diff>

<commit_message>
Touch up on grades creation, update test case
</commit_message>
<xml_diff>
--- a/testing/Team eXi Test Cases.xlsx
+++ b/testing/Team eXi Test Cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HuiXin\Documents\FYP\Thriving-Stones-Project\testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SCHOOL\y3s1\IS480 FYP\Thriving-Stones-Project\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F80950B-C86E-4D9F-9542-771309DD8708}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{371FD9C2-2119-46B4-A1DD-A58644AE9C39}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="40" windowWidth="25750" windowHeight="11590" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="25755" windowHeight="11595" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 2" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="262">
   <si>
     <t>S/N</t>
   </si>
@@ -744,9 +744,6 @@
     <t>Input the information as specified into the corresponding fields and click Create Grade</t>
   </si>
   <si>
-    <t>Error Message Display "The grade created for this class can only be English"</t>
-  </si>
-  <si>
     <t>Left Grade empty</t>
   </si>
   <si>
@@ -760,14 +757,6 @@
   <si>
     <t xml:space="preserve">Select class:  -LHRRS0ATm04Hiarglhj (English) 
 Select Examination: CA1
-Select Subject: Chemistry
-Select Location: Center
-Grade: 88
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Select class:  -LHRRS0ATm04Hiarglhj (English) 
-Select Examination: CA1
 Select Subject: English
 Select Location: Center
 Grade: 1000
@@ -788,9 +777,6 @@
     <t>The CA1 grade for English is being created before however input the Examination field as CA1</t>
   </si>
   <si>
-    <t xml:space="preserve">Failed to create grade with errror message, pls enter valid grade </t>
-  </si>
-  <si>
     <t>Failed to create grade with errror message, pls select location, subject, examination</t>
   </si>
   <si>
@@ -802,9 +788,6 @@
 </t>
   </si>
   <si>
-    <t>Failed to create grade with errror message, CA1 grade already exist</t>
-  </si>
-  <si>
     <t xml:space="preserve">Select class:  -LHRRS0ATm04Hiarglhj (English) 
 Select Examination: SA2
 Select Subject: English
@@ -1049,12 +1032,30 @@
   <si>
     <t>Email: irene.ng@steppingstones.com.sg</t>
   </si>
+  <si>
+    <t>Parse exception</t>
+  </si>
+  <si>
+    <t>Deleting tutor</t>
+  </si>
+  <si>
+    <t>Click remove</t>
+  </si>
+  <si>
+    <t>Clicking on "yes, remove"</t>
+  </si>
+  <si>
+    <t>Failed to create grade with error message,"Invalid grade"</t>
+  </si>
+  <si>
+    <t>Failed to create grade with errror message, grade already exist</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1105,6 +1106,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1230,10 +1237,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1287,15 +1295,40 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{0B9887A6-7CC9-441C-B771-FC27E966D64E}"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
@@ -1655,19 +1688,19 @@
       <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.6328125" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="29.08984375" customWidth="1"/>
-    <col min="5" max="5" width="19.54296875" customWidth="1"/>
-    <col min="6" max="6" width="16.36328125" customWidth="1"/>
-    <col min="7" max="7" width="13.36328125" customWidth="1"/>
+    <col min="4" max="4" width="29.140625" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="23.6328125" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1713,7 +1746,7 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1736,7 +1769,7 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="1:26" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1759,7 +1792,7 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:26" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1782,7 +1815,7 @@
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:26" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1805,7 +1838,7 @@
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:26" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1828,7 +1861,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:26" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:26" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1851,7 +1884,7 @@
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:26" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:26" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -1874,7 +1907,7 @@
       <c r="H8" s="16"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:26" ht="58" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:26" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -1897,7 +1930,7 @@
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="1:26" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:26" ht="150" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1920,7 +1953,7 @@
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" spans="1:26" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:26" ht="150" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1943,7 +1976,7 @@
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
     </row>
-    <row r="12" spans="1:26" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:26" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -1966,7 +1999,7 @@
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" spans="1:26" ht="58" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:26" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1989,7 +2022,7 @@
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:26" ht="58" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:26" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -2012,7 +2045,7 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:26" ht="58" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:26" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -2035,7 +2068,7 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:26" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:26" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -2058,7 +2091,7 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -2081,7 +2114,7 @@
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" spans="1:9" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -2104,7 +2137,7 @@
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
     </row>
-    <row r="19" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -2133,7 +2166,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -2162,7 +2195,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -2191,7 +2224,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -2220,7 +2253,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -2249,7 +2282,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -2278,7 +2311,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -2307,7 +2340,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -2336,7 +2369,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -2365,7 +2398,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -2394,7 +2427,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -2423,7 +2456,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -2452,7 +2485,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -2481,7 +2514,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -2508,7 +2541,7 @@
       </c>
       <c r="I32" s="4"/>
     </row>
-    <row r="33" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -2535,7 +2568,7 @@
       </c>
       <c r="I33" s="4"/>
     </row>
-    <row r="34" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -2562,7 +2595,7 @@
       </c>
       <c r="I34" s="4"/>
     </row>
-    <row r="35" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -2591,7 +2624,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -2618,7 +2651,7 @@
       </c>
       <c r="I36" s="4"/>
     </row>
-    <row r="37" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -2645,7 +2678,7 @@
       </c>
       <c r="I37" s="4"/>
     </row>
-    <row r="38" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -2672,7 +2705,7 @@
       </c>
       <c r="I38" s="4"/>
     </row>
-    <row r="39" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -2699,7 +2732,7 @@
       </c>
       <c r="I39" s="4"/>
     </row>
-    <row r="40" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -2726,7 +2759,7 @@
       </c>
       <c r="I40" s="4"/>
     </row>
-    <row r="41" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -2753,7 +2786,7 @@
       </c>
       <c r="I41" s="4"/>
     </row>
-    <row r="42" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -2780,7 +2813,7 @@
       </c>
       <c r="I42" s="4"/>
     </row>
-    <row r="43" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -2807,7 +2840,7 @@
       </c>
       <c r="I43" s="4"/>
     </row>
-    <row r="44" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -2834,7 +2867,7 @@
       </c>
       <c r="I44" s="4"/>
     </row>
-    <row r="45" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -2861,7 +2894,7 @@
       </c>
       <c r="I45" s="4"/>
     </row>
-    <row r="46" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -2888,7 +2921,7 @@
       </c>
       <c r="I46" s="4"/>
     </row>
-    <row r="47" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -2915,7 +2948,7 @@
       </c>
       <c r="I47" s="4"/>
     </row>
-    <row r="48" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -2942,7 +2975,7 @@
       </c>
       <c r="I48" s="4"/>
     </row>
-    <row r="49" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -2969,7 +3002,7 @@
       </c>
       <c r="I49" s="16"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -2996,7 +3029,7 @@
       </c>
       <c r="I50" s="17"/>
     </row>
-    <row r="51" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -3023,7 +3056,7 @@
       </c>
       <c r="I51" s="17"/>
     </row>
-    <row r="52" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -3050,7 +3083,7 @@
       </c>
       <c r="I52" s="17"/>
     </row>
-    <row r="53" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -3077,7 +3110,7 @@
       </c>
       <c r="I53" s="17"/>
     </row>
-    <row r="54" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -3104,7 +3137,7 @@
       </c>
       <c r="I54" s="17"/>
     </row>
-    <row r="55" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -3131,7 +3164,7 @@
       </c>
       <c r="I55" s="17"/>
     </row>
-    <row r="56" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>55</v>
       </c>
@@ -3158,7 +3191,7 @@
       </c>
       <c r="I56" s="17"/>
     </row>
-    <row r="57" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>56</v>
       </c>
@@ -3185,7 +3218,7 @@
       </c>
       <c r="I57" s="17"/>
     </row>
-    <row r="58" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>57</v>
       </c>
@@ -3212,7 +3245,7 @@
       </c>
       <c r="I58" s="17"/>
     </row>
-    <row r="59" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>58</v>
       </c>
@@ -3239,7 +3272,7 @@
       </c>
       <c r="I59" s="17"/>
     </row>
-    <row r="60" spans="1:9" ht="150.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>59</v>
       </c>
@@ -3266,7 +3299,7 @@
       </c>
       <c r="I60" s="17"/>
     </row>
-    <row r="61" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <v>60</v>
       </c>
@@ -3293,7 +3326,7 @@
       </c>
       <c r="I61" s="17"/>
     </row>
-    <row r="62" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <v>61</v>
       </c>
@@ -3320,7 +3353,7 @@
       </c>
       <c r="I62" s="17"/>
     </row>
-    <row r="63" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
         <v>62</v>
       </c>
@@ -3347,7 +3380,7 @@
       </c>
       <c r="I63" s="17"/>
     </row>
-    <row r="64" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
         <v>63</v>
       </c>
@@ -3374,7 +3407,7 @@
       </c>
       <c r="I64" s="17"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
         <v>64</v>
       </c>
@@ -3387,7 +3420,7 @@
       <c r="H65" s="11"/>
       <c r="I65" s="17"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
         <v>65</v>
       </c>
@@ -3400,7 +3433,7 @@
       <c r="H66" s="13"/>
       <c r="I66" s="17"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
         <v>66</v>
       </c>
@@ -3413,7 +3446,7 @@
       <c r="H67" s="17"/>
       <c r="I67" s="17"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
         <v>67</v>
       </c>
@@ -3426,7 +3459,7 @@
       <c r="H68" s="17"/>
       <c r="I68" s="17"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
         <v>68</v>
       </c>
@@ -3439,7 +3472,7 @@
       <c r="H69" s="17"/>
       <c r="I69" s="17"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <v>69</v>
       </c>
@@ -3452,7 +3485,7 @@
       <c r="H70" s="17"/>
       <c r="I70" s="17"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
         <v>70</v>
       </c>
@@ -3465,7 +3498,7 @@
       <c r="H71" s="17"/>
       <c r="I71" s="17"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
         <v>71</v>
       </c>
@@ -3478,7 +3511,7 @@
       <c r="H72" s="17"/>
       <c r="I72" s="17"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
         <v>72</v>
       </c>
@@ -3491,7 +3524,7 @@
       <c r="H73" s="17"/>
       <c r="I73" s="17"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
         <v>73</v>
       </c>
@@ -3504,7 +3537,7 @@
       <c r="H74" s="17"/>
       <c r="I74" s="17"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="5">
         <v>74</v>
       </c>
@@ -3517,7 +3550,7 @@
       <c r="H75" s="17"/>
       <c r="I75" s="17"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="5">
         <v>75</v>
       </c>
@@ -3530,7 +3563,7 @@
       <c r="H76" s="17"/>
       <c r="I76" s="17"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="5">
         <v>76</v>
       </c>
@@ -3543,7 +3576,7 @@
       <c r="H77" s="17"/>
       <c r="I77" s="17"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
         <v>77</v>
       </c>
@@ -3556,7 +3589,7 @@
       <c r="H78" s="17"/>
       <c r="I78" s="17"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="5">
         <v>78</v>
       </c>
@@ -3569,7 +3602,7 @@
       <c r="H79" s="17"/>
       <c r="I79" s="17"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="5">
         <v>79</v>
       </c>
@@ -3582,7 +3615,7 @@
       <c r="H80" s="17"/>
       <c r="I80" s="17"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="5">
         <v>80</v>
       </c>
@@ -3595,7 +3628,7 @@
       <c r="H81" s="17"/>
       <c r="I81" s="17"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="5">
         <v>81</v>
       </c>
@@ -3608,7 +3641,7 @@
       <c r="H82" s="17"/>
       <c r="I82" s="17"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="5">
         <v>82</v>
       </c>
@@ -3621,7 +3654,7 @@
       <c r="H83" s="17"/>
       <c r="I83" s="17"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="5">
         <v>83</v>
       </c>
@@ -3634,7 +3667,7 @@
       <c r="H84" s="17"/>
       <c r="I84" s="17"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="5">
         <v>84</v>
       </c>
@@ -3647,7 +3680,7 @@
       <c r="H85" s="17"/>
       <c r="I85" s="17"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="5">
         <v>85</v>
       </c>
@@ -3660,7 +3693,7 @@
       <c r="H86" s="17"/>
       <c r="I86" s="17"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="5">
         <v>86</v>
       </c>
@@ -3673,7 +3706,7 @@
       <c r="H87" s="17"/>
       <c r="I87" s="17"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="5">
         <v>87</v>
       </c>
@@ -3686,7 +3719,7 @@
       <c r="H88" s="17"/>
       <c r="I88" s="17"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="5">
         <v>88</v>
       </c>
@@ -3699,7 +3732,7 @@
       <c r="H89" s="17"/>
       <c r="I89" s="17"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="5">
         <v>89</v>
       </c>
@@ -3712,7 +3745,7 @@
       <c r="H90" s="17"/>
       <c r="I90" s="17"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="5">
         <v>90</v>
       </c>
@@ -3725,7 +3758,7 @@
       <c r="H91" s="17"/>
       <c r="I91" s="17"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="5">
         <v>91</v>
       </c>
@@ -3738,7 +3771,7 @@
       <c r="H92" s="17"/>
       <c r="I92" s="17"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="5">
         <v>92</v>
       </c>
@@ -3751,7 +3784,7 @@
       <c r="H93" s="17"/>
       <c r="I93" s="17"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="5">
         <v>93</v>
       </c>
@@ -3764,7 +3797,7 @@
       <c r="H94" s="17"/>
       <c r="I94" s="17"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="5">
         <v>94</v>
       </c>
@@ -3777,7 +3810,7 @@
       <c r="H95" s="17"/>
       <c r="I95" s="17"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="5">
         <v>95</v>
       </c>
@@ -3790,7 +3823,7 @@
       <c r="H96" s="17"/>
       <c r="I96" s="17"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="5">
         <v>96</v>
       </c>
@@ -3803,7 +3836,7 @@
       <c r="H97" s="17"/>
       <c r="I97" s="17"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="5">
         <v>97</v>
       </c>
@@ -3816,7 +3849,7 @@
       <c r="H98" s="17"/>
       <c r="I98" s="17"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="5">
         <v>98</v>
       </c>
@@ -3829,7 +3862,7 @@
       <c r="H99" s="17"/>
       <c r="I99" s="17"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="5">
         <v>99</v>
       </c>
@@ -3842,7 +3875,7 @@
       <c r="H100" s="17"/>
       <c r="I100" s="17"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="5">
         <v>100</v>
       </c>
@@ -3855,7 +3888,7 @@
       <c r="H101" s="17"/>
       <c r="I101" s="17"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="5">
         <v>101</v>
       </c>
@@ -3868,7 +3901,7 @@
       <c r="H102" s="17"/>
       <c r="I102" s="17"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="5">
         <v>102</v>
       </c>
@@ -3881,7 +3914,7 @@
       <c r="H103" s="17"/>
       <c r="I103" s="17"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="5">
         <v>103</v>
       </c>
@@ -3894,7 +3927,7 @@
       <c r="H104" s="17"/>
       <c r="I104" s="17"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="5">
         <v>104</v>
       </c>
@@ -3907,7 +3940,7 @@
       <c r="H105" s="17"/>
       <c r="I105" s="17"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="5">
         <v>105</v>
       </c>
@@ -3946,27 +3979,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5155472-66AF-4323-ACD5-D08CB3B87B8B}">
-  <dimension ref="A1:CV96"/>
+  <dimension ref="A1:CV95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D79" sqref="D79"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="2" width="16.1796875" customWidth="1"/>
-    <col min="3" max="3" width="27.6328125" customWidth="1"/>
-    <col min="4" max="4" width="35.81640625" customWidth="1"/>
-    <col min="5" max="5" width="27.81640625" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="35.85546875" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
-    <col min="7" max="7" width="17.90625" customWidth="1"/>
-    <col min="8" max="8" width="10.36328125" customWidth="1"/>
-    <col min="9" max="9" width="19.81640625" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:100" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:100" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3995,7 +4028,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:100" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -4297,7 +4330,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:100" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:100" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -4320,7 +4353,7 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:100" ht="58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:100" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -4343,7 +4376,7 @@
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:100" ht="58" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:100" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -4366,7 +4399,7 @@
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:100" ht="58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:100" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -4389,7 +4422,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:100" ht="58" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:100" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -4412,7 +4445,7 @@
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:100" ht="58" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:100" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -4435,7 +4468,7 @@
       <c r="H8" s="16"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:100" ht="58" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:100" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -4458,7 +4491,7 @@
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="1:100" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:100" ht="120" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -4481,7 +4514,7 @@
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" spans="1:100" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:100" ht="120" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -4504,7 +4537,7 @@
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
     </row>
-    <row r="12" spans="1:100" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:100" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -4527,7 +4560,7 @@
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" spans="1:100" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:100" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>14</v>
       </c>
@@ -4550,7 +4583,7 @@
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:100" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:100" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>15</v>
       </c>
@@ -4573,7 +4606,7 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:100" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:100" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>16</v>
       </c>
@@ -4596,7 +4629,7 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:100" ht="87" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:100" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>17</v>
       </c>
@@ -4619,7 +4652,7 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>18</v>
       </c>
@@ -4642,7 +4675,7 @@
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>19</v>
       </c>
@@ -4665,7 +4698,7 @@
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
     </row>
-    <row r="19" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>20</v>
       </c>
@@ -4688,7 +4721,7 @@
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
     </row>
-    <row r="20" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>21</v>
       </c>
@@ -4711,7 +4744,7 @@
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
     </row>
-    <row r="21" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>22</v>
       </c>
@@ -4734,7 +4767,7 @@
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
     </row>
-    <row r="22" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>23</v>
       </c>
@@ -4757,7 +4790,7 @@
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
     </row>
-    <row r="23" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>24</v>
       </c>
@@ -4780,7 +4813,7 @@
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
     </row>
-    <row r="24" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>25</v>
       </c>
@@ -4803,826 +4836,962 @@
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
     </row>
-    <row r="25" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>26</v>
       </c>
       <c r="B25" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D25" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="E25" s="11" t="s">
+      <c r="E25" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="F25" s="11" t="s">
+      <c r="F25" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-    </row>
-    <row r="26" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+      <c r="G25" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="H25" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="I25" s="18"/>
+    </row>
+    <row r="26" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>27</v>
       </c>
       <c r="B26" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="D26" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="E26" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="F26" s="11" t="s">
+      <c r="F26" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
+      <c r="G26" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="H26" s="18" t="s">
+        <v>61</v>
+      </c>
       <c r="I26" s="4"/>
     </row>
-    <row r="27" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>28</v>
       </c>
       <c r="B27" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D27" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="E27" s="11" t="s">
+      <c r="E27" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="F27" s="11" t="s">
+      <c r="F27" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
+      <c r="G27" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="H27" s="18" t="s">
+        <v>61</v>
+      </c>
       <c r="I27" s="4"/>
     </row>
-    <row r="28" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>29</v>
       </c>
       <c r="B28" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="D28" s="11" t="s">
+      <c r="D28" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="E28" s="11" t="s">
+      <c r="E28" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="F28" s="11" t="s">
+      <c r="F28" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
+      <c r="G28" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="H28" s="18" t="s">
+        <v>61</v>
+      </c>
       <c r="I28" s="4"/>
     </row>
-    <row r="29" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>30</v>
       </c>
       <c r="B29" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="D29" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="E29" s="11" t="s">
+      <c r="E29" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="F29" s="11" t="s">
+      <c r="F29" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
+      <c r="G29" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="H29" s="18" t="s">
+        <v>61</v>
+      </c>
       <c r="I29" s="4"/>
     </row>
-    <row r="30" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>31</v>
       </c>
       <c r="B30" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="D30" s="11" t="s">
+      <c r="D30" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="E30" s="11" t="s">
+      <c r="E30" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="F30" s="11" t="s">
+      <c r="F30" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
+      <c r="G30" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="H30" s="18" t="s">
+        <v>61</v>
+      </c>
       <c r="I30" s="4"/>
     </row>
-    <row r="31" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>32</v>
       </c>
       <c r="B31" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="D31" s="11" t="s">
+      <c r="D31" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="E31" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="F31" s="11" t="s">
+      <c r="F31" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
+      <c r="G31" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="H31" s="18" t="s">
+        <v>61</v>
+      </c>
       <c r="I31" s="4"/>
     </row>
-    <row r="32" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>33</v>
       </c>
       <c r="B32" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="D32" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="E32" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="F32" s="11" t="s">
+      <c r="F32" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
+      <c r="G32" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="H32" s="18" t="s">
+        <v>61</v>
+      </c>
       <c r="I32" s="4"/>
     </row>
-    <row r="33" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>34</v>
       </c>
       <c r="B33" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="D33" s="11" t="s">
+      <c r="D33" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="E33" s="11" t="s">
+      <c r="E33" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="F33" s="11" t="s">
+      <c r="F33" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
+      <c r="G33" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="H33" s="18" t="s">
+        <v>61</v>
+      </c>
       <c r="I33" s="4"/>
     </row>
-    <row r="34" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>35</v>
       </c>
       <c r="B34" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="D34" s="11" t="s">
+      <c r="D34" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="E34" s="11" t="s">
+      <c r="E34" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="F34" s="11" t="s">
+      <c r="F34" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
+      <c r="G34" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="H34" s="18" t="s">
+        <v>61</v>
+      </c>
       <c r="I34" s="4"/>
     </row>
-    <row r="35" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>36</v>
       </c>
       <c r="B35" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="D35" s="11" t="s">
+      <c r="D35" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="E35" s="11" t="s">
+      <c r="E35" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="F35" s="11" t="s">
+      <c r="F35" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
+      <c r="G35" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="H35" s="18" t="s">
+        <v>61</v>
+      </c>
       <c r="I35" s="4"/>
     </row>
-    <row r="36" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>37</v>
       </c>
       <c r="B36" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="D36" s="11" t="s">
+      <c r="D36" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="E36" s="11" t="s">
+      <c r="E36" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="F36" s="11" t="s">
+      <c r="F36" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
+      <c r="G36" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="H36" s="18" t="s">
+        <v>61</v>
+      </c>
       <c r="I36" s="4"/>
     </row>
-    <row r="37" spans="1:9" ht="116" x14ac:dyDescent="0.35">
-      <c r="A37" s="5">
+    <row r="37" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="A37" s="19">
         <v>38</v>
       </c>
-      <c r="B37" s="18" t="s">
+      <c r="B37" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C37" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="D37" s="11" t="s">
+      <c r="D37" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="E37" s="11" t="s">
+      <c r="E37" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="F37" s="11" t="s">
+      <c r="F37" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="4"/>
-    </row>
-    <row r="38" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+      <c r="G37" s="21" t="s">
+        <v>256</v>
+      </c>
+      <c r="H37" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="I37" s="22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>39</v>
       </c>
       <c r="B38" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C38" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="D38" s="11" t="s">
+      <c r="D38" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="E38" s="11" t="s">
+      <c r="E38" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="F38" s="11" t="s">
+      <c r="F38" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
+      <c r="G38" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="H38" s="18" t="s">
+        <v>61</v>
+      </c>
       <c r="I38" s="4"/>
     </row>
-    <row r="39" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>40</v>
       </c>
       <c r="B39" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C39" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="D39" s="13" t="s">
+      <c r="D39" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="E39" s="13" t="s">
+      <c r="E39" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="F39" s="13" t="s">
+      <c r="F39" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="G39" s="13"/>
-      <c r="H39" s="13"/>
+      <c r="G39" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="H39" s="23" t="s">
+        <v>61</v>
+      </c>
       <c r="I39" s="16"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>41</v>
       </c>
-      <c r="B40" s="19" t="s">
+      <c r="B40" s="24" t="s">
         <v>176</v>
       </c>
-      <c r="C40" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="D40" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="E40" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="F40" s="14" t="s">
+      <c r="C40" s="24" t="s">
+        <v>257</v>
+      </c>
+      <c r="D40" s="24" t="s">
+        <v>258</v>
+      </c>
+      <c r="E40" s="24" t="s">
+        <v>259</v>
+      </c>
+      <c r="F40" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
+      <c r="G40" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="H40" s="24" t="s">
+        <v>61</v>
+      </c>
       <c r="I40" s="17"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>42</v>
       </c>
-      <c r="B41" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="C41" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="D41" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="E41" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="F41" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
+      <c r="B41" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="D41" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="E41" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="F41" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="G41" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="H41" s="24" t="s">
+        <v>61</v>
+      </c>
       <c r="I41" s="17"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>43</v>
       </c>
-      <c r="B42" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="C42" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="D42" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="E42" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="F42" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
+      <c r="B42" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="D42" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="E42" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="F42" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="G42" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="H42" s="18" t="s">
+        <v>61</v>
+      </c>
       <c r="I42" s="17"/>
     </row>
-    <row r="43" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>44</v>
       </c>
       <c r="B43" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="C43" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="D43" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="E43" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="F43" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="G43" s="11"/>
-      <c r="H43" s="14"/>
+      <c r="C43" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="D43" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="E43" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="F43" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="G43" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="H43" s="18" t="s">
+        <v>61</v>
+      </c>
       <c r="I43" s="17"/>
     </row>
-    <row r="44" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>45</v>
       </c>
       <c r="B44" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="C44" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="D44" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="E44" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="F44" s="11" t="s">
+      <c r="C44" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="D44" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="E44" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="F44" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11"/>
+      <c r="G44" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="H44" s="18" t="s">
+        <v>61</v>
+      </c>
       <c r="I44" s="17"/>
     </row>
-    <row r="45" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>46</v>
       </c>
       <c r="B45" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="C45" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="D45" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="E45" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="F45" s="11" t="s">
+      <c r="C45" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="D45" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="E45" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="F45" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
+      <c r="G45" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="H45" s="18" t="s">
+        <v>61</v>
+      </c>
       <c r="I45" s="17"/>
     </row>
-    <row r="46" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>47</v>
       </c>
       <c r="B46" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="C46" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="D46" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="E46" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="F46" s="11" t="s">
+      <c r="C46" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="D46" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="E46" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="F46" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="G46" s="11"/>
-      <c r="H46" s="11"/>
+      <c r="G46" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="H46" s="18" t="s">
+        <v>61</v>
+      </c>
       <c r="I46" s="17"/>
     </row>
-    <row r="47" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>48</v>
       </c>
       <c r="B47" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="C47" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="D47" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="E47" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="F47" s="11" t="s">
+      <c r="C47" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="D47" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="E47" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="F47" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
+      <c r="G47" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="H47" s="18" t="s">
+        <v>61</v>
+      </c>
       <c r="I47" s="17"/>
     </row>
-    <row r="48" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>49</v>
       </c>
       <c r="B48" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="C48" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="D48" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="E48" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="F48" s="11" t="s">
+      <c r="C48" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="D48" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="E48" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="F48" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="G48" s="11"/>
-      <c r="H48" s="11"/>
+      <c r="G48" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="H48" s="18" t="s">
+        <v>61</v>
+      </c>
       <c r="I48" s="17"/>
     </row>
-    <row r="49" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>50</v>
       </c>
       <c r="B49" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="C49" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="D49" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="E49" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="F49" s="11" t="s">
+      <c r="C49" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="D49" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="E49" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="F49" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="G49" s="11"/>
-      <c r="H49" s="11"/>
+      <c r="G49" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="H49" s="18" t="s">
+        <v>61</v>
+      </c>
       <c r="I49" s="17"/>
     </row>
-    <row r="50" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>51</v>
       </c>
       <c r="B50" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="C50" s="11" t="s">
+      <c r="C50" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="D50" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="E50" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="F50" s="11" t="s">
+      <c r="D50" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="E50" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="F50" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="G50" s="11"/>
-      <c r="H50" s="11"/>
+      <c r="G50" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="H50" s="18" t="s">
+        <v>61</v>
+      </c>
       <c r="I50" s="17"/>
     </row>
-    <row r="51" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>52</v>
       </c>
       <c r="B51" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="C51" s="11" t="s">
+      <c r="C51" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="D51" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="E51" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="F51" s="11" t="s">
+      <c r="D51" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="E51" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="F51" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="G51" s="11"/>
-      <c r="H51" s="11"/>
+      <c r="G51" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="H51" s="18" t="s">
+        <v>61</v>
+      </c>
       <c r="I51" s="17"/>
     </row>
-    <row r="52" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>53</v>
       </c>
-      <c r="B52" s="17" t="s">
+      <c r="B52" s="22" t="s">
         <v>177</v>
       </c>
-      <c r="C52" s="11" t="s">
+      <c r="C52" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="D52" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="E52" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="F52" s="11" t="s">
+      <c r="D52" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="E52" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="F52" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="G52" s="11"/>
-      <c r="H52" s="11"/>
-      <c r="I52" s="17"/>
-    </row>
-    <row r="53" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="G52" s="21" t="s">
+        <v>256</v>
+      </c>
+      <c r="H52" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="I52" s="22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>54</v>
       </c>
       <c r="B53" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="C53" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="C53" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="D53" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="E53" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="F53" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="G53" s="11"/>
-      <c r="H53" s="11"/>
+      <c r="D53" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="E53" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="F53" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="G53" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="H53" s="18" t="s">
+        <v>61</v>
+      </c>
       <c r="I53" s="17"/>
     </row>
-    <row r="54" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>55</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="C54" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="D54" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="E54" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="F54" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="G54" s="11"/>
-      <c r="H54" s="11"/>
+        <v>220</v>
+      </c>
+      <c r="C54" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="D54" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="E54" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="F54" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="G54" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="H54" s="26" t="s">
+        <v>61</v>
+      </c>
       <c r="I54" s="17"/>
     </row>
-    <row r="55" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>56</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="C55" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="D55" s="18" t="s">
-        <v>184</v>
-      </c>
-      <c r="E55" s="18" t="s">
-        <v>183</v>
+        <v>220</v>
+      </c>
+      <c r="C55" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="D55" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="E55" s="23" t="s">
+        <v>181</v>
       </c>
       <c r="F55" s="18" t="s">
-        <v>179</v>
-      </c>
-      <c r="G55" s="11"/>
-      <c r="H55" s="11"/>
+        <v>188</v>
+      </c>
+      <c r="G55" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="H55" s="26" t="s">
+        <v>61</v>
+      </c>
       <c r="I55" s="17"/>
     </row>
-    <row r="56" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>57</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="C56" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="D56" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="C56" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="D56" s="23" t="s">
         <v>185</v>
       </c>
-      <c r="E56" s="20" t="s">
-        <v>181</v>
+      <c r="E56" s="23" t="s">
+        <v>187</v>
       </c>
       <c r="F56" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="G56" s="11"/>
-      <c r="H56" s="13"/>
+        <v>261</v>
+      </c>
+      <c r="G56" s="18" t="s">
+        <v>261</v>
+      </c>
+      <c r="H56" s="26" t="s">
+        <v>61</v>
+      </c>
       <c r="I56" s="17"/>
     </row>
-    <row r="57" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>58</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="C57" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="D57" s="20" t="s">
-        <v>186</v>
-      </c>
-      <c r="E57" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="C57" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="D57" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="E57" s="23" t="s">
         <v>181</v>
       </c>
-      <c r="F57" s="18" t="s">
-        <v>190</v>
-      </c>
-      <c r="G57" s="17"/>
-      <c r="H57" s="17"/>
+      <c r="F57" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="G57" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="H57" s="26" t="s">
+        <v>61</v>
+      </c>
       <c r="I57" s="17"/>
     </row>
-    <row r="58" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>59</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="C58" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="D58" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="E58" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="F58" s="18" t="s">
-        <v>191</v>
+        <v>196</v>
+      </c>
+      <c r="C58" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="D58" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="E58" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="F58" s="17" t="s">
+        <v>195</v>
       </c>
       <c r="G58" s="17"/>
       <c r="H58" s="17"/>
       <c r="I58" s="17"/>
     </row>
-    <row r="59" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" ht="99.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>60</v>
       </c>
       <c r="B59" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="C59" s="20" t="s">
-        <v>188</v>
-      </c>
-      <c r="D59" s="20" t="s">
-        <v>187</v>
-      </c>
-      <c r="E59" s="20" t="s">
-        <v>189</v>
-      </c>
-      <c r="F59" s="18" t="s">
-        <v>193</v>
+        <v>196</v>
+      </c>
+      <c r="C59" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="D59" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="E59" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="F59" s="17" t="s">
+        <v>200</v>
       </c>
       <c r="G59" s="17"/>
       <c r="H59" s="17"/>
       <c r="I59" s="17"/>
     </row>
-    <row r="60" spans="1:9" ht="99.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>61</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>224</v>
+        <v>192</v>
       </c>
       <c r="C60" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="D60" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="D60" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="E60" s="17" t="s">
         <v>194</v>
-      </c>
-      <c r="E60" s="20" t="s">
-        <v>181</v>
       </c>
       <c r="F60" s="17" t="s">
         <v>195</v>
@@ -5631,459 +5800,429 @@
       <c r="H60" s="17"/>
       <c r="I60" s="17"/>
     </row>
-    <row r="61" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <v>62</v>
       </c>
       <c r="B61" s="17" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="C61" s="17" t="s">
-        <v>125</v>
+        <v>197</v>
       </c>
       <c r="D61" s="17" t="s">
-        <v>197</v>
-      </c>
-      <c r="E61" s="17" t="s">
         <v>198</v>
       </c>
+      <c r="E61" s="23" t="s">
+        <v>208</v>
+      </c>
       <c r="F61" s="17" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="G61" s="17"/>
       <c r="H61" s="17"/>
       <c r="I61" s="17"/>
     </row>
-    <row r="62" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <v>63</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>200</v>
-      </c>
-      <c r="C62" s="17" t="s">
-        <v>201</v>
+        <v>192</v>
+      </c>
+      <c r="C62" s="23" t="s">
+        <v>206</v>
       </c>
       <c r="D62" s="17" t="s">
-        <v>202</v>
-      </c>
-      <c r="E62" s="20" t="s">
         <v>203</v>
       </c>
+      <c r="E62" s="17" t="s">
+        <v>204</v>
+      </c>
       <c r="F62" s="17" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="G62" s="17"/>
       <c r="H62" s="17"/>
       <c r="I62" s="17"/>
     </row>
-    <row r="63" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
         <v>64</v>
       </c>
       <c r="B63" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="C63" s="17" t="s">
-        <v>125</v>
+        <v>192</v>
+      </c>
+      <c r="C63" s="23" t="s">
+        <v>202</v>
       </c>
       <c r="D63" s="17" t="s">
-        <v>197</v>
-      </c>
-      <c r="E63" s="17" t="s">
-        <v>198</v>
+        <v>207</v>
+      </c>
+      <c r="E63" s="23" t="s">
+        <v>208</v>
       </c>
       <c r="F63" s="17" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="G63" s="17"/>
       <c r="H63" s="17"/>
       <c r="I63" s="17"/>
     </row>
-    <row r="64" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
         <v>65</v>
       </c>
       <c r="B64" s="17" t="s">
-        <v>196</v>
+        <v>213</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>201</v>
+        <v>125</v>
       </c>
       <c r="D64" s="17" t="s">
-        <v>202</v>
-      </c>
-      <c r="E64" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="E64" s="23" t="s">
+        <v>211</v>
+      </c>
+      <c r="F64" s="17" t="s">
         <v>212</v>
-      </c>
-      <c r="F64" s="17" t="s">
-        <v>205</v>
       </c>
       <c r="G64" s="17"/>
       <c r="H64" s="17"/>
       <c r="I64" s="17"/>
     </row>
-    <row r="65" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
         <v>66</v>
       </c>
       <c r="B65" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="C65" s="20" t="s">
-        <v>210</v>
+        <v>213</v>
+      </c>
+      <c r="C65" s="17" t="s">
+        <v>197</v>
       </c>
       <c r="D65" s="17" t="s">
-        <v>207</v>
-      </c>
-      <c r="E65" s="17" t="s">
-        <v>208</v>
+        <v>216</v>
+      </c>
+      <c r="E65" s="23" t="s">
+        <v>211</v>
       </c>
       <c r="F65" s="17" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="G65" s="17"/>
       <c r="H65" s="17"/>
       <c r="I65" s="17"/>
     </row>
-    <row r="66" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
         <v>67</v>
       </c>
       <c r="B66" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="C66" s="20" t="s">
-        <v>206</v>
+        <v>213</v>
+      </c>
+      <c r="C66" s="17" t="s">
+        <v>215</v>
       </c>
       <c r="D66" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="E66" s="23" t="s">
         <v>211</v>
       </c>
-      <c r="E66" s="20" t="s">
-        <v>212</v>
-      </c>
       <c r="F66" s="17" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="G66" s="17"/>
       <c r="H66" s="17"/>
       <c r="I66" s="17"/>
     </row>
-    <row r="67" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
         <v>68</v>
       </c>
       <c r="B67" s="17" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C67" s="17" t="s">
-        <v>125</v>
+        <v>221</v>
       </c>
       <c r="D67" s="17" t="s">
-        <v>214</v>
-      </c>
-      <c r="E67" s="20" t="s">
-        <v>215</v>
+        <v>226</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>235</v>
       </c>
       <c r="F67" s="17" t="s">
-        <v>216</v>
-      </c>
-      <c r="G67" s="17"/>
-      <c r="H67" s="17"/>
+        <v>219</v>
+      </c>
+      <c r="G67" s="17" t="s">
+        <v>239</v>
+      </c>
+      <c r="H67" s="17" t="s">
+        <v>61</v>
+      </c>
       <c r="I67" s="17"/>
     </row>
-    <row r="68" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
         <v>69</v>
       </c>
       <c r="B68" s="17" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C68" s="17" t="s">
-        <v>201</v>
+        <v>222</v>
       </c>
       <c r="D68" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="E68" s="20" t="s">
-        <v>215</v>
+        <v>227</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>235</v>
       </c>
       <c r="F68" s="17" t="s">
-        <v>218</v>
-      </c>
-      <c r="G68" s="17"/>
-      <c r="H68" s="17"/>
+        <v>223</v>
+      </c>
+      <c r="G68" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="H68" s="17" t="s">
+        <v>61</v>
+      </c>
       <c r="I68" s="17"/>
     </row>
-    <row r="69" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
         <v>70</v>
       </c>
       <c r="B69" s="17" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C69" s="17" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="D69" s="17" t="s">
-        <v>221</v>
-      </c>
-      <c r="E69" s="20" t="s">
-        <v>215</v>
+        <v>228</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>235</v>
       </c>
       <c r="F69" s="17" t="s">
-        <v>218</v>
-      </c>
-      <c r="G69" s="17"/>
-      <c r="H69" s="17"/>
+        <v>225</v>
+      </c>
+      <c r="G69" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="H69" s="17" t="s">
+        <v>61</v>
+      </c>
       <c r="I69" s="17"/>
     </row>
-    <row r="70" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <v>71</v>
       </c>
       <c r="B70" s="17" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C70" s="17" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="D70" s="17" t="s">
         <v>230</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F70" s="17" t="s">
-        <v>223</v>
+        <v>236</v>
       </c>
       <c r="G70" s="17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H70" s="17" t="s">
         <v>61</v>
       </c>
       <c r="I70" s="17"/>
     </row>
-    <row r="71" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
         <v>72</v>
       </c>
       <c r="B71" s="17" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C71" s="17" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="D71" s="17" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F71" s="17" t="s">
-        <v>227</v>
+        <v>237</v>
       </c>
       <c r="G71" s="17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H71" s="17" t="s">
         <v>61</v>
       </c>
       <c r="I71" s="17"/>
     </row>
-    <row r="72" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
         <v>73</v>
       </c>
       <c r="B72" s="17" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C72" s="17" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="D72" s="17" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F72" s="17" t="s">
-        <v>229</v>
+        <v>238</v>
       </c>
       <c r="G72" s="17" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H72" s="17" t="s">
         <v>61</v>
       </c>
       <c r="I72" s="17"/>
     </row>
-    <row r="73" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
         <v>74</v>
       </c>
-      <c r="B73" s="17" t="s">
-        <v>222</v>
-      </c>
-      <c r="C73" s="17" t="s">
-        <v>233</v>
-      </c>
-      <c r="D73" s="17" t="s">
-        <v>234</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="F73" s="17" t="s">
-        <v>240</v>
-      </c>
-      <c r="G73" s="17" t="s">
+      <c r="B73" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="C73" s="27" t="s">
         <v>246</v>
       </c>
-      <c r="H73" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="I73" s="17"/>
-    </row>
-    <row r="74" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+      <c r="D73" s="27" t="s">
+        <v>247</v>
+      </c>
+      <c r="E73" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="F73" s="27" t="s">
+        <v>249</v>
+      </c>
+      <c r="G73" s="27" t="s">
+        <v>250</v>
+      </c>
+      <c r="H73" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="I73" s="27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
         <v>75</v>
       </c>
-      <c r="B74" s="17" t="s">
-        <v>222</v>
-      </c>
-      <c r="C74" s="17" t="s">
-        <v>235</v>
-      </c>
-      <c r="D74" s="17" t="s">
-        <v>236</v>
-      </c>
-      <c r="E74" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="F74" s="17" t="s">
-        <v>241</v>
-      </c>
-      <c r="G74" s="17" t="s">
-        <v>247</v>
-      </c>
-      <c r="H74" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="I74" s="17"/>
-    </row>
-    <row r="75" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+      <c r="B74" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="C74" s="27" t="s">
+        <v>251</v>
+      </c>
+      <c r="D74" s="27" t="s">
+        <v>252</v>
+      </c>
+      <c r="E74" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="F74" s="27" t="s">
+        <v>253</v>
+      </c>
+      <c r="G74" s="27" t="s">
+        <v>250</v>
+      </c>
+      <c r="H74" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="I74" s="27"/>
+    </row>
+    <row r="75" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A75" s="5">
         <v>76</v>
       </c>
-      <c r="B75" s="17" t="s">
-        <v>222</v>
-      </c>
-      <c r="C75" s="17" t="s">
-        <v>237</v>
-      </c>
-      <c r="D75" s="17" t="s">
-        <v>238</v>
-      </c>
-      <c r="E75" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="F75" s="17" t="s">
-        <v>242</v>
-      </c>
-      <c r="G75" s="17" t="s">
+      <c r="B75" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="C75" s="27" t="s">
+        <v>254</v>
+      </c>
+      <c r="D75" s="27" t="s">
+        <v>255</v>
+      </c>
+      <c r="E75" s="28" t="s">
         <v>248</v>
       </c>
-      <c r="H75" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="I75" s="17"/>
-    </row>
-    <row r="76" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="F75" s="27" t="s">
+        <v>253</v>
+      </c>
+      <c r="G75" s="27" t="s">
+        <v>250</v>
+      </c>
+      <c r="H75" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="I75" s="27"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="5">
         <v>77</v>
       </c>
-      <c r="B76" s="17" t="s">
-        <v>249</v>
-      </c>
-      <c r="C76" s="17" t="s">
-        <v>250</v>
-      </c>
-      <c r="D76" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="E76" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="F76" s="17" t="s">
-        <v>253</v>
-      </c>
-      <c r="G76" s="17" t="s">
-        <v>254</v>
-      </c>
-      <c r="H76" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="I76" s="17" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="B76" s="17"/>
+      <c r="C76" s="17"/>
+      <c r="D76" s="17"/>
+      <c r="E76" s="17"/>
+      <c r="F76" s="17"/>
+      <c r="G76" s="17"/>
+      <c r="H76" s="17"/>
+      <c r="I76" s="17"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="5">
         <v>78</v>
       </c>
-      <c r="B77" s="17" t="s">
-        <v>249</v>
-      </c>
-      <c r="C77" s="17" t="s">
-        <v>255</v>
-      </c>
-      <c r="D77" s="17" t="s">
-        <v>256</v>
-      </c>
-      <c r="E77" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="F77" s="17" t="s">
-        <v>257</v>
-      </c>
-      <c r="G77" s="17" t="s">
-        <v>254</v>
-      </c>
-      <c r="H77" s="17" t="s">
-        <v>61</v>
-      </c>
+      <c r="B77" s="17"/>
+      <c r="C77" s="17"/>
+      <c r="D77" s="17"/>
+      <c r="E77" s="17"/>
+      <c r="F77" s="17"/>
+      <c r="G77" s="17"/>
+      <c r="H77" s="17"/>
       <c r="I77" s="17"/>
     </row>
-    <row r="78" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
         <v>79</v>
       </c>
-      <c r="B78" s="17" t="s">
-        <v>249</v>
-      </c>
-      <c r="C78" s="17" t="s">
-        <v>258</v>
-      </c>
-      <c r="D78" s="17" t="s">
-        <v>259</v>
-      </c>
-      <c r="E78" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="F78" s="17" t="s">
-        <v>257</v>
-      </c>
-      <c r="G78" s="17" t="s">
-        <v>254</v>
-      </c>
-      <c r="H78" s="17" t="s">
-        <v>61</v>
-      </c>
+      <c r="B78" s="17"/>
+      <c r="C78" s="17"/>
+      <c r="D78" s="17"/>
+      <c r="E78" s="17"/>
+      <c r="F78" s="17"/>
+      <c r="G78" s="17"/>
+      <c r="H78" s="17"/>
       <c r="I78" s="17"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="5">
         <v>80</v>
       </c>
@@ -6096,7 +6235,7 @@
       <c r="H79" s="17"/>
       <c r="I79" s="17"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="5">
         <v>81</v>
       </c>
@@ -6109,7 +6248,7 @@
       <c r="H80" s="17"/>
       <c r="I80" s="17"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="5">
         <v>82</v>
       </c>
@@ -6122,7 +6261,7 @@
       <c r="H81" s="17"/>
       <c r="I81" s="17"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="5">
         <v>83</v>
       </c>
@@ -6135,7 +6274,7 @@
       <c r="H82" s="17"/>
       <c r="I82" s="17"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="5">
         <v>84</v>
       </c>
@@ -6148,7 +6287,7 @@
       <c r="H83" s="17"/>
       <c r="I83" s="17"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="5">
         <v>85</v>
       </c>
@@ -6161,7 +6300,7 @@
       <c r="H84" s="17"/>
       <c r="I84" s="17"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="5">
         <v>86</v>
       </c>
@@ -6174,7 +6313,7 @@
       <c r="H85" s="17"/>
       <c r="I85" s="17"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="5">
         <v>87</v>
       </c>
@@ -6187,7 +6326,7 @@
       <c r="H86" s="17"/>
       <c r="I86" s="17"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="5">
         <v>88</v>
       </c>
@@ -6200,7 +6339,7 @@
       <c r="H87" s="17"/>
       <c r="I87" s="17"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="5">
         <v>89</v>
       </c>
@@ -6213,7 +6352,7 @@
       <c r="H88" s="17"/>
       <c r="I88" s="17"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="5">
         <v>90</v>
       </c>
@@ -6226,7 +6365,7 @@
       <c r="H89" s="17"/>
       <c r="I89" s="17"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="5">
         <v>91</v>
       </c>
@@ -6239,7 +6378,7 @@
       <c r="H90" s="17"/>
       <c r="I90" s="17"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="5">
         <v>92</v>
       </c>
@@ -6252,7 +6391,7 @@
       <c r="H91" s="17"/>
       <c r="I91" s="17"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="5">
         <v>93</v>
       </c>
@@ -6265,7 +6404,7 @@
       <c r="H92" s="17"/>
       <c r="I92" s="17"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="5">
         <v>94</v>
       </c>
@@ -6278,7 +6417,7 @@
       <c r="H93" s="17"/>
       <c r="I93" s="17"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="5">
         <v>95</v>
       </c>
@@ -6291,7 +6430,7 @@
       <c r="H94" s="17"/>
       <c r="I94" s="17"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="5">
         <v>96</v>
       </c>
@@ -6303,19 +6442,6 @@
       <c r="G95" s="17"/>
       <c r="H95" s="17"/>
       <c r="I95" s="17"/>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A96" s="5">
-        <v>97</v>
-      </c>
-      <c r="B96" s="17"/>
-      <c r="C96" s="17"/>
-      <c r="D96" s="17"/>
-      <c r="E96" s="17"/>
-      <c r="F96" s="17"/>
-      <c r="G96" s="17"/>
-      <c r="H96" s="17"/>
-      <c r="I96" s="17"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1">

</xml_diff>